<commit_message>
Split 2 WT and 2 KO.
</commit_message>
<xml_diff>
--- a/scripts/file_params.xlsx
+++ b/scripts/file_params.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jai/Documents/Computing/DataScience/Columbia/rwalk/input/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jai/Documents/Computing/DataScience/Columbia/rwalk/scripts/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="11">
   <si>
     <t>filename</t>
   </si>
@@ -42,6 +42,24 @@
   </si>
   <si>
     <t>180920_10mg-kgAMPH_2.csv</t>
+  </si>
+  <si>
+    <t>190205_a-synKO_AMPH1.csv</t>
+  </si>
+  <si>
+    <t>amph</t>
+  </si>
+  <si>
+    <t>genotype</t>
+  </si>
+  <si>
+    <t>wt</t>
+  </si>
+  <si>
+    <t>ko</t>
+  </si>
+  <si>
+    <t>190205_a-synKO_AMPH2.csv</t>
   </si>
 </sst>
 </file>
@@ -356,10 +374,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C31"/>
+  <dimension ref="A1:E61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+    <sheetView tabSelected="1" topLeftCell="A44" workbookViewId="0">
+      <selection activeCell="C59" sqref="C59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -367,7 +385,7 @@
     <col min="1" max="1" width="28.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -377,8 +395,14 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -388,8 +412,14 @@
       <c r="C2">
         <v>105</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -399,8 +429,14 @@
       <c r="C3">
         <v>1303</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -410,8 +446,14 @@
       <c r="C4">
         <v>2503</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -421,8 +463,14 @@
       <c r="C5">
         <v>3706</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -432,8 +480,14 @@
       <c r="C6">
         <v>4901</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>3</v>
       </c>
@@ -444,8 +498,14 @@
         <f t="shared" ref="C7:C16" si="0">C6+1200</f>
         <v>6101</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>3</v>
       </c>
@@ -456,8 +516,14 @@
         <f t="shared" si="0"/>
         <v>7301</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D8" t="s">
+        <v>8</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>3</v>
       </c>
@@ -468,8 +534,14 @@
         <f t="shared" si="0"/>
         <v>8501</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D9" t="s">
+        <v>8</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>3</v>
       </c>
@@ -480,8 +552,14 @@
         <f t="shared" si="0"/>
         <v>9701</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D10" t="s">
+        <v>8</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>3</v>
       </c>
@@ -492,8 +570,14 @@
         <f t="shared" si="0"/>
         <v>10901</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D11" t="s">
+        <v>8</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>3</v>
       </c>
@@ -504,8 +588,14 @@
         <f t="shared" si="0"/>
         <v>12101</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D12" t="s">
+        <v>8</v>
+      </c>
+      <c r="E12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>3</v>
       </c>
@@ -516,8 +606,14 @@
         <f t="shared" si="0"/>
         <v>13301</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D13" t="s">
+        <v>8</v>
+      </c>
+      <c r="E13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>3</v>
       </c>
@@ -528,8 +624,14 @@
         <f t="shared" si="0"/>
         <v>14501</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D14" t="s">
+        <v>8</v>
+      </c>
+      <c r="E14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>3</v>
       </c>
@@ -539,8 +641,14 @@
       <c r="C15">
         <v>15699</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D15" t="s">
+        <v>8</v>
+      </c>
+      <c r="E15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>3</v>
       </c>
@@ -551,8 +659,14 @@
         <f t="shared" si="0"/>
         <v>16899</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D16" t="s">
+        <v>8</v>
+      </c>
+      <c r="E16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>4</v>
       </c>
@@ -562,8 +676,14 @@
       <c r="C17">
         <v>103</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D17" t="s">
+        <v>8</v>
+      </c>
+      <c r="E17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" t="str">
         <f>A17</f>
         <v>180920_10mg-kgAMPH_2.csv</v>
@@ -576,22 +696,34 @@
         <f>C17+1200</f>
         <v>1303</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D18" t="s">
+        <v>8</v>
+      </c>
+      <c r="E18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" t="str">
-        <f t="shared" ref="A19:A36" si="1">A18</f>
+        <f t="shared" ref="A19:A31" si="1">A18</f>
         <v>180920_10mg-kgAMPH_2.csv</v>
       </c>
       <c r="B19">
-        <f t="shared" ref="B19:B36" si="2">B18+1</f>
+        <f t="shared" ref="B19:B31" si="2">B18+1</f>
         <v>3</v>
       </c>
       <c r="C19">
-        <f t="shared" ref="C19:C36" si="3">C18+1200</f>
+        <f t="shared" ref="C19:C30" si="3">C18+1200</f>
         <v>2503</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D19" t="s">
+        <v>8</v>
+      </c>
+      <c r="E19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" t="str">
         <f t="shared" si="1"/>
         <v>180920_10mg-kgAMPH_2.csv</v>
@@ -603,8 +735,14 @@
       <c r="C20">
         <v>3705</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D20" t="s">
+        <v>8</v>
+      </c>
+      <c r="E20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" t="str">
         <f t="shared" si="1"/>
         <v>180920_10mg-kgAMPH_2.csv</v>
@@ -616,8 +754,14 @@
       <c r="C21">
         <v>4904</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D21" t="s">
+        <v>8</v>
+      </c>
+      <c r="E21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" t="str">
         <f t="shared" si="1"/>
         <v>180920_10mg-kgAMPH_2.csv</v>
@@ -630,8 +774,14 @@
         <f t="shared" si="3"/>
         <v>6104</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D22" t="s">
+        <v>8</v>
+      </c>
+      <c r="E22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" t="str">
         <f t="shared" si="1"/>
         <v>180920_10mg-kgAMPH_2.csv</v>
@@ -643,8 +793,14 @@
       <c r="C23">
         <v>7302</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D23" t="s">
+        <v>8</v>
+      </c>
+      <c r="E23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" t="str">
         <f t="shared" si="1"/>
         <v>180920_10mg-kgAMPH_2.csv</v>
@@ -656,8 +812,14 @@
       <c r="C24">
         <v>8500</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D24" t="s">
+        <v>8</v>
+      </c>
+      <c r="E24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" t="str">
         <f t="shared" si="1"/>
         <v>180920_10mg-kgAMPH_2.csv</v>
@@ -670,8 +832,14 @@
         <f t="shared" si="3"/>
         <v>9700</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D25" t="s">
+        <v>8</v>
+      </c>
+      <c r="E25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" t="str">
         <f t="shared" si="1"/>
         <v>180920_10mg-kgAMPH_2.csv</v>
@@ -683,8 +851,14 @@
       <c r="C26">
         <v>10904</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D26" t="s">
+        <v>8</v>
+      </c>
+      <c r="E26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" t="str">
         <f t="shared" si="1"/>
         <v>180920_10mg-kgAMPH_2.csv</v>
@@ -696,8 +870,14 @@
       <c r="C27">
         <v>12100</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D27" t="s">
+        <v>8</v>
+      </c>
+      <c r="E27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" t="str">
         <f t="shared" si="1"/>
         <v>180920_10mg-kgAMPH_2.csv</v>
@@ -709,8 +889,14 @@
       <c r="C28">
         <v>13299</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D28" t="s">
+        <v>8</v>
+      </c>
+      <c r="E28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" t="str">
         <f t="shared" si="1"/>
         <v>180920_10mg-kgAMPH_2.csv</v>
@@ -723,8 +909,14 @@
         <f t="shared" si="3"/>
         <v>14499</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D29" t="s">
+        <v>8</v>
+      </c>
+      <c r="E29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" t="str">
         <f t="shared" si="1"/>
         <v>180920_10mg-kgAMPH_2.csv</v>
@@ -737,8 +929,14 @@
         <f t="shared" si="3"/>
         <v>15699</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D30" t="s">
+        <v>8</v>
+      </c>
+      <c r="E30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" t="str">
         <f t="shared" si="1"/>
         <v>180920_10mg-kgAMPH_2.csv</v>
@@ -749,6 +947,631 @@
       </c>
       <c r="C31">
         <v>16895</v>
+      </c>
+      <c r="D31" t="s">
+        <v>8</v>
+      </c>
+      <c r="E31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>5</v>
+      </c>
+      <c r="B32">
+        <v>1</v>
+      </c>
+      <c r="C32">
+        <v>100</v>
+      </c>
+      <c r="D32" t="s">
+        <v>9</v>
+      </c>
+      <c r="E32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A33" t="str">
+        <f>A32</f>
+        <v>190205_a-synKO_AMPH1.csv</v>
+      </c>
+      <c r="B33">
+        <f>B32+1</f>
+        <v>2</v>
+      </c>
+      <c r="C33">
+        <f>C32+1200</f>
+        <v>1300</v>
+      </c>
+      <c r="D33" t="str">
+        <f>D32</f>
+        <v>ko</v>
+      </c>
+      <c r="E33">
+        <f>E32</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A34" t="str">
+        <f t="shared" ref="A34:A46" si="4">A33</f>
+        <v>190205_a-synKO_AMPH1.csv</v>
+      </c>
+      <c r="B34">
+        <f t="shared" ref="B34:B46" si="5">B33+1</f>
+        <v>3</v>
+      </c>
+      <c r="C34">
+        <v>2501</v>
+      </c>
+      <c r="D34" t="str">
+        <f t="shared" ref="D34:D46" si="6">D33</f>
+        <v>ko</v>
+      </c>
+      <c r="E34">
+        <f t="shared" ref="E34" si="7">E33</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A35" t="str">
+        <f t="shared" si="4"/>
+        <v>190205_a-synKO_AMPH1.csv</v>
+      </c>
+      <c r="B35">
+        <f t="shared" si="5"/>
+        <v>4</v>
+      </c>
+      <c r="C35">
+        <f t="shared" ref="C35:C45" si="8">C34+1200</f>
+        <v>3701</v>
+      </c>
+      <c r="D35" t="str">
+        <f t="shared" si="6"/>
+        <v>ko</v>
+      </c>
+      <c r="E35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A36" t="str">
+        <f t="shared" si="4"/>
+        <v>190205_a-synKO_AMPH1.csv</v>
+      </c>
+      <c r="B36">
+        <f t="shared" si="5"/>
+        <v>5</v>
+      </c>
+      <c r="C36">
+        <f t="shared" si="8"/>
+        <v>4901</v>
+      </c>
+      <c r="D36" t="str">
+        <f t="shared" si="6"/>
+        <v>ko</v>
+      </c>
+      <c r="E36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A37" t="str">
+        <f t="shared" si="4"/>
+        <v>190205_a-synKO_AMPH1.csv</v>
+      </c>
+      <c r="B37">
+        <f t="shared" si="5"/>
+        <v>6</v>
+      </c>
+      <c r="C37">
+        <v>6099</v>
+      </c>
+      <c r="D37" t="str">
+        <f t="shared" si="6"/>
+        <v>ko</v>
+      </c>
+      <c r="E37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A38" t="str">
+        <f t="shared" si="4"/>
+        <v>190205_a-synKO_AMPH1.csv</v>
+      </c>
+      <c r="B38">
+        <f t="shared" si="5"/>
+        <v>7</v>
+      </c>
+      <c r="C38">
+        <f t="shared" si="8"/>
+        <v>7299</v>
+      </c>
+      <c r="D38" t="str">
+        <f t="shared" si="6"/>
+        <v>ko</v>
+      </c>
+      <c r="E38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A39" t="str">
+        <f t="shared" si="4"/>
+        <v>190205_a-synKO_AMPH1.csv</v>
+      </c>
+      <c r="B39">
+        <f t="shared" si="5"/>
+        <v>8</v>
+      </c>
+      <c r="C39">
+        <f t="shared" si="8"/>
+        <v>8499</v>
+      </c>
+      <c r="D39" t="str">
+        <f t="shared" si="6"/>
+        <v>ko</v>
+      </c>
+      <c r="E39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A40" t="str">
+        <f t="shared" si="4"/>
+        <v>190205_a-synKO_AMPH1.csv</v>
+      </c>
+      <c r="B40">
+        <f t="shared" si="5"/>
+        <v>9</v>
+      </c>
+      <c r="C40">
+        <f t="shared" si="8"/>
+        <v>9699</v>
+      </c>
+      <c r="D40" t="str">
+        <f t="shared" si="6"/>
+        <v>ko</v>
+      </c>
+      <c r="E40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A41" t="str">
+        <f t="shared" si="4"/>
+        <v>190205_a-synKO_AMPH1.csv</v>
+      </c>
+      <c r="B41">
+        <f t="shared" si="5"/>
+        <v>10</v>
+      </c>
+      <c r="C41">
+        <v>10900</v>
+      </c>
+      <c r="D41" t="str">
+        <f t="shared" si="6"/>
+        <v>ko</v>
+      </c>
+      <c r="E41">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A42" t="str">
+        <f t="shared" si="4"/>
+        <v>190205_a-synKO_AMPH1.csv</v>
+      </c>
+      <c r="B42">
+        <f t="shared" si="5"/>
+        <v>11</v>
+      </c>
+      <c r="C42">
+        <v>12099</v>
+      </c>
+      <c r="D42" t="str">
+        <f t="shared" si="6"/>
+        <v>ko</v>
+      </c>
+      <c r="E42">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A43" t="str">
+        <f t="shared" si="4"/>
+        <v>190205_a-synKO_AMPH1.csv</v>
+      </c>
+      <c r="B43">
+        <f t="shared" si="5"/>
+        <v>12</v>
+      </c>
+      <c r="C43">
+        <v>13301</v>
+      </c>
+      <c r="D43" t="str">
+        <f t="shared" si="6"/>
+        <v>ko</v>
+      </c>
+      <c r="E43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A44" t="str">
+        <f t="shared" si="4"/>
+        <v>190205_a-synKO_AMPH1.csv</v>
+      </c>
+      <c r="B44">
+        <f t="shared" si="5"/>
+        <v>13</v>
+      </c>
+      <c r="C44">
+        <f t="shared" si="8"/>
+        <v>14501</v>
+      </c>
+      <c r="D44" t="str">
+        <f t="shared" si="6"/>
+        <v>ko</v>
+      </c>
+      <c r="E44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A45" t="str">
+        <f t="shared" si="4"/>
+        <v>190205_a-synKO_AMPH1.csv</v>
+      </c>
+      <c r="B45">
+        <f t="shared" si="5"/>
+        <v>14</v>
+      </c>
+      <c r="C45">
+        <f t="shared" si="8"/>
+        <v>15701</v>
+      </c>
+      <c r="D45" t="str">
+        <f t="shared" si="6"/>
+        <v>ko</v>
+      </c>
+      <c r="E45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A46" t="str">
+        <f t="shared" si="4"/>
+        <v>190205_a-synKO_AMPH1.csv</v>
+      </c>
+      <c r="B46">
+        <f t="shared" si="5"/>
+        <v>15</v>
+      </c>
+      <c r="C46">
+        <v>16900</v>
+      </c>
+      <c r="D46" t="str">
+        <f t="shared" si="6"/>
+        <v>ko</v>
+      </c>
+      <c r="E46">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>10</v>
+      </c>
+      <c r="B47">
+        <v>1</v>
+      </c>
+      <c r="C47">
+        <v>100</v>
+      </c>
+      <c r="D47" t="s">
+        <v>9</v>
+      </c>
+      <c r="E47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A48" t="str">
+        <f>A47</f>
+        <v>190205_a-synKO_AMPH2.csv</v>
+      </c>
+      <c r="B48">
+        <f>B47+1</f>
+        <v>2</v>
+      </c>
+      <c r="C48">
+        <f>C47+1200</f>
+        <v>1300</v>
+      </c>
+      <c r="D48" t="str">
+        <f>D47</f>
+        <v>ko</v>
+      </c>
+      <c r="E48">
+        <f>E47</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A49" t="str">
+        <f t="shared" ref="A49:A71" si="9">A48</f>
+        <v>190205_a-synKO_AMPH2.csv</v>
+      </c>
+      <c r="B49">
+        <f t="shared" ref="B49:B71" si="10">B48+1</f>
+        <v>3</v>
+      </c>
+      <c r="C49">
+        <f t="shared" ref="C49:C71" si="11">C48+1200</f>
+        <v>2500</v>
+      </c>
+      <c r="D49" t="str">
+        <f t="shared" ref="D49:D71" si="12">D48</f>
+        <v>ko</v>
+      </c>
+      <c r="E49">
+        <f t="shared" ref="E49:E71" si="13">E48</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A50" t="str">
+        <f t="shared" si="9"/>
+        <v>190205_a-synKO_AMPH2.csv</v>
+      </c>
+      <c r="B50">
+        <f t="shared" si="10"/>
+        <v>4</v>
+      </c>
+      <c r="C50">
+        <f t="shared" si="11"/>
+        <v>3700</v>
+      </c>
+      <c r="D50" t="str">
+        <f t="shared" si="12"/>
+        <v>ko</v>
+      </c>
+      <c r="E50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A51" t="str">
+        <f t="shared" si="9"/>
+        <v>190205_a-synKO_AMPH2.csv</v>
+      </c>
+      <c r="B51">
+        <f t="shared" si="10"/>
+        <v>5</v>
+      </c>
+      <c r="C51">
+        <f t="shared" si="11"/>
+        <v>4900</v>
+      </c>
+      <c r="D51" t="str">
+        <f t="shared" si="12"/>
+        <v>ko</v>
+      </c>
+      <c r="E51">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A52" t="str">
+        <f t="shared" si="9"/>
+        <v>190205_a-synKO_AMPH2.csv</v>
+      </c>
+      <c r="B52">
+        <f t="shared" si="10"/>
+        <v>6</v>
+      </c>
+      <c r="C52">
+        <f t="shared" si="11"/>
+        <v>6100</v>
+      </c>
+      <c r="D52" t="str">
+        <f t="shared" si="12"/>
+        <v>ko</v>
+      </c>
+      <c r="E52">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A53" t="str">
+        <f t="shared" si="9"/>
+        <v>190205_a-synKO_AMPH2.csv</v>
+      </c>
+      <c r="B53">
+        <f t="shared" si="10"/>
+        <v>7</v>
+      </c>
+      <c r="C53">
+        <f t="shared" si="11"/>
+        <v>7300</v>
+      </c>
+      <c r="D53" t="str">
+        <f t="shared" si="12"/>
+        <v>ko</v>
+      </c>
+      <c r="E53">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A54" t="str">
+        <f t="shared" si="9"/>
+        <v>190205_a-synKO_AMPH2.csv</v>
+      </c>
+      <c r="B54">
+        <f t="shared" si="10"/>
+        <v>8</v>
+      </c>
+      <c r="C54">
+        <f t="shared" si="11"/>
+        <v>8500</v>
+      </c>
+      <c r="D54" t="str">
+        <f t="shared" si="12"/>
+        <v>ko</v>
+      </c>
+      <c r="E54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A55" t="str">
+        <f t="shared" si="9"/>
+        <v>190205_a-synKO_AMPH2.csv</v>
+      </c>
+      <c r="B55">
+        <f t="shared" si="10"/>
+        <v>9</v>
+      </c>
+      <c r="C55">
+        <f t="shared" si="11"/>
+        <v>9700</v>
+      </c>
+      <c r="D55" t="str">
+        <f t="shared" si="12"/>
+        <v>ko</v>
+      </c>
+      <c r="E55">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A56" t="str">
+        <f t="shared" si="9"/>
+        <v>190205_a-synKO_AMPH2.csv</v>
+      </c>
+      <c r="B56">
+        <f t="shared" si="10"/>
+        <v>10</v>
+      </c>
+      <c r="C56">
+        <f t="shared" si="11"/>
+        <v>10900</v>
+      </c>
+      <c r="D56" t="str">
+        <f t="shared" si="12"/>
+        <v>ko</v>
+      </c>
+      <c r="E56">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A57" t="str">
+        <f t="shared" si="9"/>
+        <v>190205_a-synKO_AMPH2.csv</v>
+      </c>
+      <c r="B57">
+        <f t="shared" si="10"/>
+        <v>11</v>
+      </c>
+      <c r="C57">
+        <f t="shared" si="11"/>
+        <v>12100</v>
+      </c>
+      <c r="D57" t="str">
+        <f t="shared" si="12"/>
+        <v>ko</v>
+      </c>
+      <c r="E57">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A58" t="str">
+        <f t="shared" si="9"/>
+        <v>190205_a-synKO_AMPH2.csv</v>
+      </c>
+      <c r="B58">
+        <f t="shared" si="10"/>
+        <v>12</v>
+      </c>
+      <c r="C58">
+        <v>13299</v>
+      </c>
+      <c r="D58" t="str">
+        <f t="shared" si="12"/>
+        <v>ko</v>
+      </c>
+      <c r="E58">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A59" t="str">
+        <f t="shared" si="9"/>
+        <v>190205_a-synKO_AMPH2.csv</v>
+      </c>
+      <c r="B59">
+        <f t="shared" si="10"/>
+        <v>13</v>
+      </c>
+      <c r="C59">
+        <f t="shared" si="11"/>
+        <v>14499</v>
+      </c>
+      <c r="D59" t="str">
+        <f t="shared" si="12"/>
+        <v>ko</v>
+      </c>
+      <c r="E59">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A60" t="str">
+        <f t="shared" si="9"/>
+        <v>190205_a-synKO_AMPH2.csv</v>
+      </c>
+      <c r="B60">
+        <f t="shared" si="10"/>
+        <v>14</v>
+      </c>
+      <c r="C60">
+        <f t="shared" si="11"/>
+        <v>15699</v>
+      </c>
+      <c r="D60" t="str">
+        <f t="shared" si="12"/>
+        <v>ko</v>
+      </c>
+      <c r="E60">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A61" t="str">
+        <f t="shared" si="9"/>
+        <v>190205_a-synKO_AMPH2.csv</v>
+      </c>
+      <c r="B61">
+        <f t="shared" si="10"/>
+        <v>15</v>
+      </c>
+      <c r="C61">
+        <f t="shared" si="11"/>
+        <v>16899</v>
+      </c>
+      <c r="D61" t="str">
+        <f t="shared" si="12"/>
+        <v>ko</v>
+      </c>
+      <c r="E61">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
3 WT, 2 KO
</commit_message>
<xml_diff>
--- a/scripts/file_params.xlsx
+++ b/scripts/file_params.xlsx
@@ -15,7 +15,7 @@
     <sheet name="file_params" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">file_params!$A$1:$A$61</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">file_params!$A$1:$A$76</definedName>
   </definedNames>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="29">
   <si>
     <t>filename</t>
   </si>
@@ -114,6 +114,9 @@
   </si>
   <si>
     <t>fall</t>
+  </si>
+  <si>
+    <t>180921_10mg-kgAMPH-1.csv</t>
   </si>
 </sst>
 </file>
@@ -452,13 +455,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U61"/>
+  <sheetPr filterMode="1" enableFormatConditionsCalculation="0"/>
+  <dimension ref="A1:U76"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="T64" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" sqref="A1:I6"/>
+      <selection pane="bottomRight" activeCell="U67" sqref="U67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -551,7 +555,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -617,7 +621,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -661,7 +665,7 @@
         <v>4</v>
       </c>
       <c r="O3">
-        <f t="shared" ref="O3:O61" si="0">2.7*10^-6</f>
+        <f t="shared" ref="O3:O66" si="0">2.7*10^-6</f>
         <v>2.7E-6</v>
       </c>
       <c r="P3" t="b">
@@ -683,7 +687,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -749,7 +753,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -815,7 +819,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -881,7 +885,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>3</v>
       </c>
@@ -948,7 +952,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>3</v>
       </c>
@@ -1015,7 +1019,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>3</v>
       </c>
@@ -1082,7 +1086,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>3</v>
       </c>
@@ -1149,7 +1153,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>3</v>
       </c>
@@ -1216,7 +1220,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>3</v>
       </c>
@@ -1283,7 +1287,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>3</v>
       </c>
@@ -1350,7 +1354,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>3</v>
       </c>
@@ -1417,7 +1421,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>3</v>
       </c>
@@ -1483,7 +1487,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>3</v>
       </c>
@@ -1550,7 +1554,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>4</v>
       </c>
@@ -1616,7 +1620,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
       <c r="A18" t="str">
         <f>A17</f>
         <v>180920_10mg-kgAMPH_2.csv</v>
@@ -1685,7 +1689,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
       <c r="A19" t="str">
         <f t="shared" ref="A19:A31" si="2">A18</f>
         <v>180920_10mg-kgAMPH_2.csv</v>
@@ -1754,7 +1758,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
       <c r="A20" t="str">
         <f t="shared" si="2"/>
         <v>180920_10mg-kgAMPH_2.csv</v>
@@ -1822,7 +1826,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
       <c r="A21" t="str">
         <f t="shared" si="2"/>
         <v>180920_10mg-kgAMPH_2.csv</v>
@@ -1890,7 +1894,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
       <c r="A22" t="str">
         <f t="shared" si="2"/>
         <v>180920_10mg-kgAMPH_2.csv</v>
@@ -1959,7 +1963,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="23" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
       <c r="A23" t="str">
         <f t="shared" si="2"/>
         <v>180920_10mg-kgAMPH_2.csv</v>
@@ -2027,7 +2031,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="24" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
       <c r="A24" t="str">
         <f t="shared" si="2"/>
         <v>180920_10mg-kgAMPH_2.csv</v>
@@ -2095,7 +2099,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="25" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
       <c r="A25" t="str">
         <f t="shared" si="2"/>
         <v>180920_10mg-kgAMPH_2.csv</v>
@@ -2164,7 +2168,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="26" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
       <c r="A26" t="str">
         <f t="shared" si="2"/>
         <v>180920_10mg-kgAMPH_2.csv</v>
@@ -2232,7 +2236,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="27" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
       <c r="A27" t="str">
         <f t="shared" si="2"/>
         <v>180920_10mg-kgAMPH_2.csv</v>
@@ -2300,7 +2304,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="28" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
       <c r="A28" t="str">
         <f t="shared" si="2"/>
         <v>180920_10mg-kgAMPH_2.csv</v>
@@ -2368,7 +2372,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="29" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
       <c r="A29" t="str">
         <f t="shared" si="2"/>
         <v>180920_10mg-kgAMPH_2.csv</v>
@@ -2437,7 +2441,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="30" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
       <c r="A30" t="str">
         <f t="shared" si="2"/>
         <v>180920_10mg-kgAMPH_2.csv</v>
@@ -2506,7 +2510,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="31" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
       <c r="A31" t="str">
         <f t="shared" si="2"/>
         <v>180920_10mg-kgAMPH_2.csv</v>
@@ -2574,7 +2578,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="32" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>5</v>
       </c>
@@ -2640,7 +2644,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="33" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
       <c r="A33" t="str">
         <f>A32</f>
         <v>190205_a-synKO_AMPH1.csv</v>
@@ -2711,7 +2715,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="34" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
       <c r="A34" t="str">
         <f t="shared" ref="A34:A46" si="5">A33</f>
         <v>190205_a-synKO_AMPH1.csv</v>
@@ -2781,7 +2785,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="35" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
       <c r="A35" t="str">
         <f t="shared" si="5"/>
         <v>190205_a-synKO_AMPH1.csv</v>
@@ -2851,7 +2855,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="36" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
       <c r="A36" t="str">
         <f t="shared" si="5"/>
         <v>190205_a-synKO_AMPH1.csv</v>
@@ -2921,7 +2925,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="37" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
       <c r="A37" t="str">
         <f t="shared" si="5"/>
         <v>190205_a-synKO_AMPH1.csv</v>
@@ -2990,7 +2994,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="38" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
       <c r="A38" t="str">
         <f t="shared" si="5"/>
         <v>190205_a-synKO_AMPH1.csv</v>
@@ -3060,7 +3064,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="39" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
       <c r="A39" t="str">
         <f t="shared" si="5"/>
         <v>190205_a-synKO_AMPH1.csv</v>
@@ -3130,7 +3134,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="40" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
       <c r="A40" t="str">
         <f t="shared" si="5"/>
         <v>190205_a-synKO_AMPH1.csv</v>
@@ -3200,7 +3204,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="41" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
       <c r="A41" t="str">
         <f t="shared" si="5"/>
         <v>190205_a-synKO_AMPH1.csv</v>
@@ -3269,7 +3273,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="42" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
       <c r="A42" t="str">
         <f t="shared" si="5"/>
         <v>190205_a-synKO_AMPH1.csv</v>
@@ -3338,7 +3342,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="43" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
       <c r="A43" t="str">
         <f t="shared" si="5"/>
         <v>190205_a-synKO_AMPH1.csv</v>
@@ -3407,7 +3411,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="44" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
       <c r="A44" t="str">
         <f t="shared" si="5"/>
         <v>190205_a-synKO_AMPH1.csv</v>
@@ -3477,7 +3481,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="45" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
       <c r="A45" t="str">
         <f t="shared" si="5"/>
         <v>190205_a-synKO_AMPH1.csv</v>
@@ -3547,7 +3551,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="46" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
       <c r="A46" t="str">
         <f t="shared" si="5"/>
         <v>190205_a-synKO_AMPH1.csv</v>
@@ -3616,7 +3620,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="47" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>10</v>
       </c>
@@ -3682,7 +3686,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="48" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
       <c r="A48" t="str">
         <f>A47</f>
         <v>190205_a-synKO_AMPH2.csv</v>
@@ -3753,7 +3757,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="49" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
       <c r="A49" t="str">
         <f t="shared" ref="A49:A61" si="10">A48</f>
         <v>190205_a-synKO_AMPH2.csv</v>
@@ -3824,7 +3828,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="50" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
       <c r="A50" t="str">
         <f t="shared" si="10"/>
         <v>190205_a-synKO_AMPH2.csv</v>
@@ -3894,7 +3898,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="51" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
       <c r="A51" t="str">
         <f t="shared" si="10"/>
         <v>190205_a-synKO_AMPH2.csv</v>
@@ -3964,7 +3968,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="52" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
       <c r="A52" t="str">
         <f t="shared" si="10"/>
         <v>190205_a-synKO_AMPH2.csv</v>
@@ -4034,7 +4038,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="53" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
       <c r="A53" t="str">
         <f t="shared" si="10"/>
         <v>190205_a-synKO_AMPH2.csv</v>
@@ -4104,7 +4108,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="54" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
       <c r="A54" t="str">
         <f t="shared" si="10"/>
         <v>190205_a-synKO_AMPH2.csv</v>
@@ -4174,7 +4178,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="55" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
       <c r="A55" t="str">
         <f t="shared" si="10"/>
         <v>190205_a-synKO_AMPH2.csv</v>
@@ -4244,7 +4248,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="56" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
       <c r="A56" t="str">
         <f t="shared" si="10"/>
         <v>190205_a-synKO_AMPH2.csv</v>
@@ -4314,7 +4318,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="57" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
       <c r="A57" t="str">
         <f t="shared" si="10"/>
         <v>190205_a-synKO_AMPH2.csv</v>
@@ -4384,7 +4388,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="58" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
       <c r="A58" t="str">
         <f t="shared" si="10"/>
         <v>190205_a-synKO_AMPH2.csv</v>
@@ -4453,7 +4457,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="59" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
       <c r="A59" t="str">
         <f t="shared" si="10"/>
         <v>190205_a-synKO_AMPH2.csv</v>
@@ -4523,7 +4527,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="60" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
       <c r="A60" t="str">
         <f t="shared" si="10"/>
         <v>190205_a-synKO_AMPH2.csv</v>
@@ -4593,7 +4597,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="61" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
       <c r="A61" t="str">
         <f t="shared" si="10"/>
         <v>190205_a-synKO_AMPH2.csv</v>
@@ -4663,8 +4667,1032 @@
         <v>110</v>
       </c>
     </row>
+    <row r="62" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
+        <v>28</v>
+      </c>
+      <c r="B62">
+        <v>1</v>
+      </c>
+      <c r="C62">
+        <v>100</v>
+      </c>
+      <c r="D62" t="s">
+        <v>8</v>
+      </c>
+      <c r="E62">
+        <v>0</v>
+      </c>
+      <c r="F62">
+        <v>100</v>
+      </c>
+      <c r="G62">
+        <v>2.4</v>
+      </c>
+      <c r="H62">
+        <v>4.8</v>
+      </c>
+      <c r="I62">
+        <v>2.1</v>
+      </c>
+      <c r="J62">
+        <v>30</v>
+      </c>
+      <c r="K62">
+        <v>50</v>
+      </c>
+      <c r="L62">
+        <v>2</v>
+      </c>
+      <c r="M62">
+        <v>1000</v>
+      </c>
+      <c r="N62">
+        <v>4</v>
+      </c>
+      <c r="O62">
+        <f t="shared" si="0"/>
+        <v>2.7E-6</v>
+      </c>
+      <c r="P62" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q62">
+        <v>7000</v>
+      </c>
+      <c r="R62">
+        <v>5</v>
+      </c>
+      <c r="S62" t="s">
+        <v>27</v>
+      </c>
+      <c r="T62">
+        <v>0.05</v>
+      </c>
+      <c r="U62">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="63" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
+        <v>28</v>
+      </c>
+      <c r="B63">
+        <f>B62+1</f>
+        <v>2</v>
+      </c>
+      <c r="C63">
+        <f>C62+1200</f>
+        <v>1300</v>
+      </c>
+      <c r="D63" t="s">
+        <v>8</v>
+      </c>
+      <c r="E63">
+        <v>0</v>
+      </c>
+      <c r="F63">
+        <v>100</v>
+      </c>
+      <c r="G63">
+        <v>2.4</v>
+      </c>
+      <c r="H63">
+        <v>4.8</v>
+      </c>
+      <c r="I63">
+        <v>2.1</v>
+      </c>
+      <c r="J63">
+        <v>30</v>
+      </c>
+      <c r="K63">
+        <v>50</v>
+      </c>
+      <c r="L63">
+        <v>2</v>
+      </c>
+      <c r="M63">
+        <v>1000</v>
+      </c>
+      <c r="N63">
+        <v>4</v>
+      </c>
+      <c r="O63">
+        <f t="shared" si="0"/>
+        <v>2.7E-6</v>
+      </c>
+      <c r="P63" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q63">
+        <v>7000</v>
+      </c>
+      <c r="R63">
+        <v>5</v>
+      </c>
+      <c r="S63" t="s">
+        <v>27</v>
+      </c>
+      <c r="T63">
+        <v>0.05</v>
+      </c>
+      <c r="U63">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="64" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
+        <v>28</v>
+      </c>
+      <c r="B64">
+        <f t="shared" ref="B64:B81" si="15">B63+1</f>
+        <v>3</v>
+      </c>
+      <c r="C64">
+        <f t="shared" ref="C64:C76" si="16">C63+1200</f>
+        <v>2500</v>
+      </c>
+      <c r="D64" t="s">
+        <v>8</v>
+      </c>
+      <c r="E64">
+        <v>0</v>
+      </c>
+      <c r="F64">
+        <v>100</v>
+      </c>
+      <c r="G64">
+        <v>2.4</v>
+      </c>
+      <c r="H64">
+        <v>4.8</v>
+      </c>
+      <c r="I64">
+        <v>2.1</v>
+      </c>
+      <c r="J64">
+        <v>30</v>
+      </c>
+      <c r="K64">
+        <v>50</v>
+      </c>
+      <c r="L64">
+        <v>2</v>
+      </c>
+      <c r="M64">
+        <v>1000</v>
+      </c>
+      <c r="N64">
+        <v>4</v>
+      </c>
+      <c r="O64">
+        <f t="shared" si="0"/>
+        <v>2.7E-6</v>
+      </c>
+      <c r="P64" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q64">
+        <v>7000</v>
+      </c>
+      <c r="R64">
+        <v>5</v>
+      </c>
+      <c r="S64" t="s">
+        <v>27</v>
+      </c>
+      <c r="T64">
+        <v>0.05</v>
+      </c>
+      <c r="U64">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="65" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A65" t="s">
+        <v>28</v>
+      </c>
+      <c r="B65">
+        <f t="shared" si="15"/>
+        <v>4</v>
+      </c>
+      <c r="C65">
+        <f t="shared" si="16"/>
+        <v>3700</v>
+      </c>
+      <c r="D65" t="s">
+        <v>8</v>
+      </c>
+      <c r="E65">
+        <v>1</v>
+      </c>
+      <c r="F65">
+        <v>100</v>
+      </c>
+      <c r="G65">
+        <v>2.4</v>
+      </c>
+      <c r="H65">
+        <v>4.8</v>
+      </c>
+      <c r="I65">
+        <v>2.1</v>
+      </c>
+      <c r="J65">
+        <v>30</v>
+      </c>
+      <c r="K65">
+        <v>50</v>
+      </c>
+      <c r="L65">
+        <v>2</v>
+      </c>
+      <c r="M65">
+        <v>1000</v>
+      </c>
+      <c r="N65">
+        <v>4</v>
+      </c>
+      <c r="O65">
+        <f t="shared" si="0"/>
+        <v>2.7E-6</v>
+      </c>
+      <c r="P65" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q65">
+        <v>7000</v>
+      </c>
+      <c r="R65">
+        <v>5</v>
+      </c>
+      <c r="S65" t="s">
+        <v>27</v>
+      </c>
+      <c r="T65">
+        <v>0.05</v>
+      </c>
+      <c r="U65">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="66" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
+        <v>28</v>
+      </c>
+      <c r="B66">
+        <f t="shared" si="15"/>
+        <v>5</v>
+      </c>
+      <c r="C66">
+        <f t="shared" si="16"/>
+        <v>4900</v>
+      </c>
+      <c r="D66" t="s">
+        <v>8</v>
+      </c>
+      <c r="E66">
+        <v>1</v>
+      </c>
+      <c r="F66">
+        <v>100</v>
+      </c>
+      <c r="G66">
+        <v>2.4</v>
+      </c>
+      <c r="H66">
+        <v>4.8</v>
+      </c>
+      <c r="I66">
+        <v>2.1</v>
+      </c>
+      <c r="J66">
+        <v>30</v>
+      </c>
+      <c r="K66">
+        <v>50</v>
+      </c>
+      <c r="L66">
+        <v>2</v>
+      </c>
+      <c r="M66">
+        <v>1000</v>
+      </c>
+      <c r="N66">
+        <v>4</v>
+      </c>
+      <c r="O66">
+        <f t="shared" si="0"/>
+        <v>2.7E-6</v>
+      </c>
+      <c r="P66" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q66">
+        <v>7000</v>
+      </c>
+      <c r="R66">
+        <v>5</v>
+      </c>
+      <c r="S66" t="s">
+        <v>27</v>
+      </c>
+      <c r="T66">
+        <v>0.05</v>
+      </c>
+      <c r="U66">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="67" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
+        <v>28</v>
+      </c>
+      <c r="B67">
+        <f t="shared" si="15"/>
+        <v>6</v>
+      </c>
+      <c r="C67">
+        <f t="shared" si="16"/>
+        <v>6100</v>
+      </c>
+      <c r="D67" t="s">
+        <v>8</v>
+      </c>
+      <c r="E67">
+        <v>1</v>
+      </c>
+      <c r="F67">
+        <v>100</v>
+      </c>
+      <c r="G67">
+        <v>2.4</v>
+      </c>
+      <c r="H67">
+        <v>4.8</v>
+      </c>
+      <c r="I67">
+        <v>2.1</v>
+      </c>
+      <c r="J67">
+        <v>30</v>
+      </c>
+      <c r="K67">
+        <v>50</v>
+      </c>
+      <c r="L67">
+        <v>2</v>
+      </c>
+      <c r="M67">
+        <v>1000</v>
+      </c>
+      <c r="N67">
+        <v>4</v>
+      </c>
+      <c r="O67">
+        <f t="shared" ref="O67:O81" si="17">2.7*10^-6</f>
+        <v>2.7E-6</v>
+      </c>
+      <c r="P67" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q67">
+        <v>7000</v>
+      </c>
+      <c r="R67">
+        <v>5</v>
+      </c>
+      <c r="S67" t="s">
+        <v>27</v>
+      </c>
+      <c r="T67">
+        <v>0.05</v>
+      </c>
+      <c r="U67">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="68" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A68" t="s">
+        <v>28</v>
+      </c>
+      <c r="B68">
+        <f t="shared" si="15"/>
+        <v>7</v>
+      </c>
+      <c r="C68">
+        <f t="shared" si="16"/>
+        <v>7300</v>
+      </c>
+      <c r="D68" t="s">
+        <v>8</v>
+      </c>
+      <c r="E68">
+        <v>1</v>
+      </c>
+      <c r="F68">
+        <v>100</v>
+      </c>
+      <c r="G68">
+        <v>2.4</v>
+      </c>
+      <c r="H68">
+        <v>4.8</v>
+      </c>
+      <c r="I68">
+        <v>2.1</v>
+      </c>
+      <c r="J68">
+        <v>30</v>
+      </c>
+      <c r="K68">
+        <v>50</v>
+      </c>
+      <c r="L68">
+        <v>2</v>
+      </c>
+      <c r="M68">
+        <v>1000</v>
+      </c>
+      <c r="N68">
+        <v>4</v>
+      </c>
+      <c r="O68">
+        <f t="shared" si="17"/>
+        <v>2.7E-6</v>
+      </c>
+      <c r="P68" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q68">
+        <v>7000</v>
+      </c>
+      <c r="R68">
+        <v>5</v>
+      </c>
+      <c r="S68" t="s">
+        <v>27</v>
+      </c>
+      <c r="T68">
+        <v>0.05</v>
+      </c>
+      <c r="U68">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="69" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A69" t="s">
+        <v>28</v>
+      </c>
+      <c r="B69">
+        <f t="shared" si="15"/>
+        <v>8</v>
+      </c>
+      <c r="C69">
+        <f t="shared" si="16"/>
+        <v>8500</v>
+      </c>
+      <c r="D69" t="s">
+        <v>8</v>
+      </c>
+      <c r="E69">
+        <v>1</v>
+      </c>
+      <c r="F69">
+        <v>100</v>
+      </c>
+      <c r="G69">
+        <v>2.4</v>
+      </c>
+      <c r="H69">
+        <v>4.8</v>
+      </c>
+      <c r="I69">
+        <v>2.1</v>
+      </c>
+      <c r="J69">
+        <v>30</v>
+      </c>
+      <c r="K69">
+        <v>50</v>
+      </c>
+      <c r="L69">
+        <v>2</v>
+      </c>
+      <c r="M69">
+        <v>1000</v>
+      </c>
+      <c r="N69">
+        <v>4</v>
+      </c>
+      <c r="O69">
+        <f t="shared" si="17"/>
+        <v>2.7E-6</v>
+      </c>
+      <c r="P69" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q69">
+        <v>7000</v>
+      </c>
+      <c r="R69">
+        <v>5</v>
+      </c>
+      <c r="S69" t="s">
+        <v>27</v>
+      </c>
+      <c r="T69">
+        <v>0.05</v>
+      </c>
+      <c r="U69">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="70" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A70" t="s">
+        <v>28</v>
+      </c>
+      <c r="B70">
+        <f t="shared" si="15"/>
+        <v>9</v>
+      </c>
+      <c r="C70">
+        <f t="shared" si="16"/>
+        <v>9700</v>
+      </c>
+      <c r="D70" t="s">
+        <v>8</v>
+      </c>
+      <c r="E70">
+        <v>1</v>
+      </c>
+      <c r="F70">
+        <v>100</v>
+      </c>
+      <c r="G70">
+        <v>2.4</v>
+      </c>
+      <c r="H70">
+        <v>4.8</v>
+      </c>
+      <c r="I70">
+        <v>2.1</v>
+      </c>
+      <c r="J70">
+        <v>30</v>
+      </c>
+      <c r="K70">
+        <v>50</v>
+      </c>
+      <c r="L70">
+        <v>2</v>
+      </c>
+      <c r="M70">
+        <v>1000</v>
+      </c>
+      <c r="N70">
+        <v>4</v>
+      </c>
+      <c r="O70">
+        <f t="shared" si="17"/>
+        <v>2.7E-6</v>
+      </c>
+      <c r="P70" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q70">
+        <v>7000</v>
+      </c>
+      <c r="R70">
+        <v>5</v>
+      </c>
+      <c r="S70" t="s">
+        <v>27</v>
+      </c>
+      <c r="T70">
+        <v>0.05</v>
+      </c>
+      <c r="U70">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="71" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A71" t="s">
+        <v>28</v>
+      </c>
+      <c r="B71">
+        <f t="shared" si="15"/>
+        <v>10</v>
+      </c>
+      <c r="C71">
+        <f t="shared" si="16"/>
+        <v>10900</v>
+      </c>
+      <c r="D71" t="s">
+        <v>8</v>
+      </c>
+      <c r="E71">
+        <v>1</v>
+      </c>
+      <c r="F71">
+        <v>100</v>
+      </c>
+      <c r="G71">
+        <v>2.4</v>
+      </c>
+      <c r="H71">
+        <v>4.8</v>
+      </c>
+      <c r="I71">
+        <v>2.1</v>
+      </c>
+      <c r="J71">
+        <v>30</v>
+      </c>
+      <c r="K71">
+        <v>50</v>
+      </c>
+      <c r="L71">
+        <v>2</v>
+      </c>
+      <c r="M71">
+        <v>1000</v>
+      </c>
+      <c r="N71">
+        <v>4</v>
+      </c>
+      <c r="O71">
+        <f t="shared" si="17"/>
+        <v>2.7E-6</v>
+      </c>
+      <c r="P71" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q71">
+        <v>7000</v>
+      </c>
+      <c r="R71">
+        <v>5</v>
+      </c>
+      <c r="S71" t="s">
+        <v>27</v>
+      </c>
+      <c r="T71">
+        <v>0.05</v>
+      </c>
+      <c r="U71">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="72" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A72" t="s">
+        <v>28</v>
+      </c>
+      <c r="B72">
+        <f t="shared" si="15"/>
+        <v>11</v>
+      </c>
+      <c r="C72">
+        <f t="shared" si="16"/>
+        <v>12100</v>
+      </c>
+      <c r="D72" t="s">
+        <v>8</v>
+      </c>
+      <c r="E72">
+        <v>1</v>
+      </c>
+      <c r="F72">
+        <v>100</v>
+      </c>
+      <c r="G72">
+        <v>2.4</v>
+      </c>
+      <c r="H72">
+        <v>4.8</v>
+      </c>
+      <c r="I72">
+        <v>2.1</v>
+      </c>
+      <c r="J72">
+        <v>30</v>
+      </c>
+      <c r="K72">
+        <v>50</v>
+      </c>
+      <c r="L72">
+        <v>2</v>
+      </c>
+      <c r="M72">
+        <v>1000</v>
+      </c>
+      <c r="N72">
+        <v>4</v>
+      </c>
+      <c r="O72">
+        <f t="shared" si="17"/>
+        <v>2.7E-6</v>
+      </c>
+      <c r="P72" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q72">
+        <v>7000</v>
+      </c>
+      <c r="R72">
+        <v>5</v>
+      </c>
+      <c r="S72" t="s">
+        <v>27</v>
+      </c>
+      <c r="T72">
+        <v>0.05</v>
+      </c>
+      <c r="U72">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="73" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A73" t="s">
+        <v>28</v>
+      </c>
+      <c r="B73">
+        <f t="shared" si="15"/>
+        <v>12</v>
+      </c>
+      <c r="C73">
+        <f t="shared" si="16"/>
+        <v>13300</v>
+      </c>
+      <c r="D73" t="s">
+        <v>8</v>
+      </c>
+      <c r="E73">
+        <v>1</v>
+      </c>
+      <c r="F73">
+        <v>100</v>
+      </c>
+      <c r="G73">
+        <v>2.4</v>
+      </c>
+      <c r="H73">
+        <v>4.8</v>
+      </c>
+      <c r="I73">
+        <v>2.1</v>
+      </c>
+      <c r="J73">
+        <v>30</v>
+      </c>
+      <c r="K73">
+        <v>50</v>
+      </c>
+      <c r="L73">
+        <v>2</v>
+      </c>
+      <c r="M73">
+        <v>1000</v>
+      </c>
+      <c r="N73">
+        <v>4</v>
+      </c>
+      <c r="O73">
+        <f t="shared" si="17"/>
+        <v>2.7E-6</v>
+      </c>
+      <c r="P73" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q73">
+        <v>7000</v>
+      </c>
+      <c r="R73">
+        <v>5</v>
+      </c>
+      <c r="S73" t="s">
+        <v>27</v>
+      </c>
+      <c r="T73">
+        <v>0.05</v>
+      </c>
+      <c r="U73">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="74" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A74" t="s">
+        <v>28</v>
+      </c>
+      <c r="B74">
+        <f t="shared" si="15"/>
+        <v>13</v>
+      </c>
+      <c r="C74">
+        <f t="shared" si="16"/>
+        <v>14500</v>
+      </c>
+      <c r="D74" t="s">
+        <v>8</v>
+      </c>
+      <c r="E74">
+        <v>1</v>
+      </c>
+      <c r="F74">
+        <v>100</v>
+      </c>
+      <c r="G74">
+        <v>2.4</v>
+      </c>
+      <c r="H74">
+        <v>4.8</v>
+      </c>
+      <c r="I74">
+        <v>2.1</v>
+      </c>
+      <c r="J74">
+        <v>30</v>
+      </c>
+      <c r="K74">
+        <v>50</v>
+      </c>
+      <c r="L74">
+        <v>2</v>
+      </c>
+      <c r="M74">
+        <v>1000</v>
+      </c>
+      <c r="N74">
+        <v>4</v>
+      </c>
+      <c r="O74">
+        <f t="shared" si="17"/>
+        <v>2.7E-6</v>
+      </c>
+      <c r="P74" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q74">
+        <v>7000</v>
+      </c>
+      <c r="R74">
+        <v>5</v>
+      </c>
+      <c r="S74" t="s">
+        <v>27</v>
+      </c>
+      <c r="T74">
+        <v>0.05</v>
+      </c>
+      <c r="U74">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="75" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A75" t="s">
+        <v>28</v>
+      </c>
+      <c r="B75">
+        <f t="shared" si="15"/>
+        <v>14</v>
+      </c>
+      <c r="C75">
+        <f t="shared" si="16"/>
+        <v>15700</v>
+      </c>
+      <c r="D75" t="s">
+        <v>8</v>
+      </c>
+      <c r="E75">
+        <v>1</v>
+      </c>
+      <c r="F75">
+        <v>100</v>
+      </c>
+      <c r="G75">
+        <v>2.4</v>
+      </c>
+      <c r="H75">
+        <v>4.8</v>
+      </c>
+      <c r="I75">
+        <v>2.1</v>
+      </c>
+      <c r="J75">
+        <v>30</v>
+      </c>
+      <c r="K75">
+        <v>50</v>
+      </c>
+      <c r="L75">
+        <v>2</v>
+      </c>
+      <c r="M75">
+        <v>1000</v>
+      </c>
+      <c r="N75">
+        <v>4</v>
+      </c>
+      <c r="O75">
+        <f t="shared" si="17"/>
+        <v>2.7E-6</v>
+      </c>
+      <c r="P75" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q75">
+        <v>7000</v>
+      </c>
+      <c r="R75">
+        <v>5</v>
+      </c>
+      <c r="S75" t="s">
+        <v>27</v>
+      </c>
+      <c r="T75">
+        <v>0.05</v>
+      </c>
+      <c r="U75">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="76" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A76" t="s">
+        <v>28</v>
+      </c>
+      <c r="B76">
+        <f t="shared" si="15"/>
+        <v>15</v>
+      </c>
+      <c r="C76">
+        <f t="shared" si="16"/>
+        <v>16900</v>
+      </c>
+      <c r="D76" t="s">
+        <v>8</v>
+      </c>
+      <c r="E76">
+        <v>1</v>
+      </c>
+      <c r="F76">
+        <v>100</v>
+      </c>
+      <c r="G76">
+        <v>2.4</v>
+      </c>
+      <c r="H76">
+        <v>4.8</v>
+      </c>
+      <c r="I76">
+        <v>2.1</v>
+      </c>
+      <c r="J76">
+        <v>30</v>
+      </c>
+      <c r="K76">
+        <v>50</v>
+      </c>
+      <c r="L76">
+        <v>2</v>
+      </c>
+      <c r="M76">
+        <v>1000</v>
+      </c>
+      <c r="N76">
+        <v>4</v>
+      </c>
+      <c r="O76">
+        <f t="shared" si="17"/>
+        <v>2.7E-6</v>
+      </c>
+      <c r="P76" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q76">
+        <v>7000</v>
+      </c>
+      <c r="R76">
+        <v>5</v>
+      </c>
+      <c r="S76" t="s">
+        <v>27</v>
+      </c>
+      <c r="T76">
+        <v>0.05</v>
+      </c>
+      <c r="U76">
+        <v>110</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:A61"/>
+  <autoFilter ref="A1:A76">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="180921_10mg-kgAMPH-1.csv"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
4 WT, 2 KO
</commit_message>
<xml_diff>
--- a/scripts/file_params.xlsx
+++ b/scripts/file_params.xlsx
@@ -15,7 +15,7 @@
     <sheet name="file_params" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">file_params!$A$1:$A$76</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">file_params!$A$1:$A$91</definedName>
   </definedNames>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="30">
   <si>
     <t>filename</t>
   </si>
@@ -117,6 +117,9 @@
   </si>
   <si>
     <t>180921_10mg-kgAMPH-1.csv</t>
+  </si>
+  <si>
+    <t>180921_10mg-kgAMPH-2.csv</t>
   </si>
 </sst>
 </file>
@@ -455,14 +458,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr filterMode="1" enableFormatConditionsCalculation="0"/>
-  <dimension ref="A1:U76"/>
+  <dimension ref="A1:U91"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="T64" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C75" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="U67" sqref="U67"/>
+      <selection pane="bottomRight" activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -555,7 +557,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -621,7 +623,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="3" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -687,7 +689,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="4" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -753,7 +755,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="5" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -819,7 +821,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="6" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -885,7 +887,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="7" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>3</v>
       </c>
@@ -952,7 +954,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="8" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>3</v>
       </c>
@@ -1019,7 +1021,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="9" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>3</v>
       </c>
@@ -1086,7 +1088,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="10" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>3</v>
       </c>
@@ -1153,7 +1155,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="11" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>3</v>
       </c>
@@ -1220,7 +1222,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="12" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>3</v>
       </c>
@@ -1287,7 +1289,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="13" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>3</v>
       </c>
@@ -1354,7 +1356,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="14" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>3</v>
       </c>
@@ -1421,7 +1423,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="15" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>3</v>
       </c>
@@ -1487,7 +1489,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="16" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>3</v>
       </c>
@@ -1554,7 +1556,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="17" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>4</v>
       </c>
@@ -1620,7 +1622,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="18" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A18" t="str">
         <f>A17</f>
         <v>180920_10mg-kgAMPH_2.csv</v>
@@ -1689,7 +1691,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="19" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A19" t="str">
         <f t="shared" ref="A19:A31" si="2">A18</f>
         <v>180920_10mg-kgAMPH_2.csv</v>
@@ -1758,7 +1760,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="20" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A20" t="str">
         <f t="shared" si="2"/>
         <v>180920_10mg-kgAMPH_2.csv</v>
@@ -1826,7 +1828,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="21" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A21" t="str">
         <f t="shared" si="2"/>
         <v>180920_10mg-kgAMPH_2.csv</v>
@@ -1894,7 +1896,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="22" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A22" t="str">
         <f t="shared" si="2"/>
         <v>180920_10mg-kgAMPH_2.csv</v>
@@ -1963,7 +1965,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="23" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A23" t="str">
         <f t="shared" si="2"/>
         <v>180920_10mg-kgAMPH_2.csv</v>
@@ -2031,7 +2033,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="24" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A24" t="str">
         <f t="shared" si="2"/>
         <v>180920_10mg-kgAMPH_2.csv</v>
@@ -2099,7 +2101,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="25" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A25" t="str">
         <f t="shared" si="2"/>
         <v>180920_10mg-kgAMPH_2.csv</v>
@@ -2168,7 +2170,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="26" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A26" t="str">
         <f t="shared" si="2"/>
         <v>180920_10mg-kgAMPH_2.csv</v>
@@ -2236,7 +2238,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="27" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A27" t="str">
         <f t="shared" si="2"/>
         <v>180920_10mg-kgAMPH_2.csv</v>
@@ -2304,7 +2306,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="28" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A28" t="str">
         <f t="shared" si="2"/>
         <v>180920_10mg-kgAMPH_2.csv</v>
@@ -2372,7 +2374,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="29" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A29" t="str">
         <f t="shared" si="2"/>
         <v>180920_10mg-kgAMPH_2.csv</v>
@@ -2441,7 +2443,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="30" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A30" t="str">
         <f t="shared" si="2"/>
         <v>180920_10mg-kgAMPH_2.csv</v>
@@ -2510,7 +2512,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="31" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A31" t="str">
         <f t="shared" si="2"/>
         <v>180920_10mg-kgAMPH_2.csv</v>
@@ -2578,7 +2580,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="32" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>5</v>
       </c>
@@ -2644,7 +2646,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="33" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A33" t="str">
         <f>A32</f>
         <v>190205_a-synKO_AMPH1.csv</v>
@@ -2715,7 +2717,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="34" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A34" t="str">
         <f t="shared" ref="A34:A46" si="5">A33</f>
         <v>190205_a-synKO_AMPH1.csv</v>
@@ -2785,7 +2787,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="35" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A35" t="str">
         <f t="shared" si="5"/>
         <v>190205_a-synKO_AMPH1.csv</v>
@@ -2855,7 +2857,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="36" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A36" t="str">
         <f t="shared" si="5"/>
         <v>190205_a-synKO_AMPH1.csv</v>
@@ -2925,7 +2927,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="37" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A37" t="str">
         <f t="shared" si="5"/>
         <v>190205_a-synKO_AMPH1.csv</v>
@@ -2994,7 +2996,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="38" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A38" t="str">
         <f t="shared" si="5"/>
         <v>190205_a-synKO_AMPH1.csv</v>
@@ -3064,7 +3066,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="39" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A39" t="str">
         <f t="shared" si="5"/>
         <v>190205_a-synKO_AMPH1.csv</v>
@@ -3134,7 +3136,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="40" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A40" t="str">
         <f t="shared" si="5"/>
         <v>190205_a-synKO_AMPH1.csv</v>
@@ -3204,7 +3206,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="41" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A41" t="str">
         <f t="shared" si="5"/>
         <v>190205_a-synKO_AMPH1.csv</v>
@@ -3273,7 +3275,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="42" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A42" t="str">
         <f t="shared" si="5"/>
         <v>190205_a-synKO_AMPH1.csv</v>
@@ -3342,7 +3344,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="43" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A43" t="str">
         <f t="shared" si="5"/>
         <v>190205_a-synKO_AMPH1.csv</v>
@@ -3411,7 +3413,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="44" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A44" t="str">
         <f t="shared" si="5"/>
         <v>190205_a-synKO_AMPH1.csv</v>
@@ -3481,7 +3483,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="45" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A45" t="str">
         <f t="shared" si="5"/>
         <v>190205_a-synKO_AMPH1.csv</v>
@@ -3551,7 +3553,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="46" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A46" t="str">
         <f t="shared" si="5"/>
         <v>190205_a-synKO_AMPH1.csv</v>
@@ -3620,7 +3622,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="47" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>10</v>
       </c>
@@ -3686,7 +3688,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="48" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A48" t="str">
         <f>A47</f>
         <v>190205_a-synKO_AMPH2.csv</v>
@@ -3757,7 +3759,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="49" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A49" t="str">
         <f t="shared" ref="A49:A61" si="10">A48</f>
         <v>190205_a-synKO_AMPH2.csv</v>
@@ -3828,7 +3830,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="50" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A50" t="str">
         <f t="shared" si="10"/>
         <v>190205_a-synKO_AMPH2.csv</v>
@@ -3898,7 +3900,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="51" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A51" t="str">
         <f t="shared" si="10"/>
         <v>190205_a-synKO_AMPH2.csv</v>
@@ -3968,7 +3970,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="52" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A52" t="str">
         <f t="shared" si="10"/>
         <v>190205_a-synKO_AMPH2.csv</v>
@@ -4038,7 +4040,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="53" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A53" t="str">
         <f t="shared" si="10"/>
         <v>190205_a-synKO_AMPH2.csv</v>
@@ -4108,7 +4110,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="54" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A54" t="str">
         <f t="shared" si="10"/>
         <v>190205_a-synKO_AMPH2.csv</v>
@@ -4178,7 +4180,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="55" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A55" t="str">
         <f t="shared" si="10"/>
         <v>190205_a-synKO_AMPH2.csv</v>
@@ -4248,7 +4250,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="56" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A56" t="str">
         <f t="shared" si="10"/>
         <v>190205_a-synKO_AMPH2.csv</v>
@@ -4318,7 +4320,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="57" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A57" t="str">
         <f t="shared" si="10"/>
         <v>190205_a-synKO_AMPH2.csv</v>
@@ -4388,7 +4390,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="58" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A58" t="str">
         <f t="shared" si="10"/>
         <v>190205_a-synKO_AMPH2.csv</v>
@@ -4457,7 +4459,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="59" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A59" t="str">
         <f t="shared" si="10"/>
         <v>190205_a-synKO_AMPH2.csv</v>
@@ -4527,7 +4529,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="60" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A60" t="str">
         <f t="shared" si="10"/>
         <v>190205_a-synKO_AMPH2.csv</v>
@@ -4597,7 +4599,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="61" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A61" t="str">
         <f t="shared" si="10"/>
         <v>190205_a-synKO_AMPH2.csv</v>
@@ -5051,7 +5053,7 @@
         <v>4</v>
       </c>
       <c r="O67">
-        <f t="shared" ref="O67:O81" si="17">2.7*10^-6</f>
+        <f t="shared" ref="O67:O95" si="17">2.7*10^-6</f>
         <v>2.7E-6</v>
       </c>
       <c r="P67" t="b">
@@ -5685,14 +5687,1026 @@
         <v>110</v>
       </c>
     </row>
+    <row r="77" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A77" t="s">
+        <v>29</v>
+      </c>
+      <c r="B77">
+        <v>1</v>
+      </c>
+      <c r="C77">
+        <v>100</v>
+      </c>
+      <c r="D77" t="s">
+        <v>8</v>
+      </c>
+      <c r="E77">
+        <v>1</v>
+      </c>
+      <c r="F77">
+        <v>100</v>
+      </c>
+      <c r="G77">
+        <v>2.4</v>
+      </c>
+      <c r="H77">
+        <v>4.8</v>
+      </c>
+      <c r="I77">
+        <v>2.1</v>
+      </c>
+      <c r="J77">
+        <v>30</v>
+      </c>
+      <c r="K77">
+        <v>50</v>
+      </c>
+      <c r="L77">
+        <v>2</v>
+      </c>
+      <c r="M77">
+        <v>1000</v>
+      </c>
+      <c r="N77">
+        <v>4</v>
+      </c>
+      <c r="O77">
+        <f t="shared" si="17"/>
+        <v>2.7E-6</v>
+      </c>
+      <c r="P77" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q77">
+        <v>7000</v>
+      </c>
+      <c r="R77">
+        <v>5</v>
+      </c>
+      <c r="S77" t="s">
+        <v>27</v>
+      </c>
+      <c r="T77">
+        <v>0.05</v>
+      </c>
+      <c r="U77">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="78" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A78" t="s">
+        <v>29</v>
+      </c>
+      <c r="B78">
+        <f>B77+1</f>
+        <v>2</v>
+      </c>
+      <c r="C78">
+        <f>C77+1200</f>
+        <v>1300</v>
+      </c>
+      <c r="D78" t="s">
+        <v>8</v>
+      </c>
+      <c r="E78">
+        <v>1</v>
+      </c>
+      <c r="F78">
+        <v>100</v>
+      </c>
+      <c r="G78">
+        <v>2.4</v>
+      </c>
+      <c r="H78">
+        <v>4.8</v>
+      </c>
+      <c r="I78">
+        <v>2.1</v>
+      </c>
+      <c r="J78">
+        <v>30</v>
+      </c>
+      <c r="K78">
+        <v>50</v>
+      </c>
+      <c r="L78">
+        <v>2</v>
+      </c>
+      <c r="M78">
+        <v>1000</v>
+      </c>
+      <c r="N78">
+        <v>4</v>
+      </c>
+      <c r="O78">
+        <f t="shared" si="17"/>
+        <v>2.7E-6</v>
+      </c>
+      <c r="P78" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q78">
+        <v>7000</v>
+      </c>
+      <c r="R78">
+        <v>5</v>
+      </c>
+      <c r="S78" t="s">
+        <v>27</v>
+      </c>
+      <c r="T78">
+        <v>0.05</v>
+      </c>
+      <c r="U78">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="79" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A79" t="s">
+        <v>29</v>
+      </c>
+      <c r="B79">
+        <f t="shared" ref="B79:B95" si="18">B78+1</f>
+        <v>3</v>
+      </c>
+      <c r="C79">
+        <f t="shared" ref="C79:C95" si="19">C78+1200</f>
+        <v>2500</v>
+      </c>
+      <c r="D79" t="s">
+        <v>8</v>
+      </c>
+      <c r="E79">
+        <v>1</v>
+      </c>
+      <c r="F79">
+        <v>100</v>
+      </c>
+      <c r="G79">
+        <v>2.4</v>
+      </c>
+      <c r="H79">
+        <v>4.8</v>
+      </c>
+      <c r="I79">
+        <v>2.1</v>
+      </c>
+      <c r="J79">
+        <v>30</v>
+      </c>
+      <c r="K79">
+        <v>50</v>
+      </c>
+      <c r="L79">
+        <v>2</v>
+      </c>
+      <c r="M79">
+        <v>1000</v>
+      </c>
+      <c r="N79">
+        <v>4</v>
+      </c>
+      <c r="O79">
+        <f t="shared" si="17"/>
+        <v>2.7E-6</v>
+      </c>
+      <c r="P79" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q79">
+        <v>7000</v>
+      </c>
+      <c r="R79">
+        <v>5</v>
+      </c>
+      <c r="S79" t="s">
+        <v>27</v>
+      </c>
+      <c r="T79">
+        <v>0.05</v>
+      </c>
+      <c r="U79">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="80" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A80" t="s">
+        <v>29</v>
+      </c>
+      <c r="B80">
+        <f t="shared" si="18"/>
+        <v>4</v>
+      </c>
+      <c r="C80">
+        <f t="shared" si="19"/>
+        <v>3700</v>
+      </c>
+      <c r="D80" t="s">
+        <v>8</v>
+      </c>
+      <c r="E80">
+        <v>1</v>
+      </c>
+      <c r="F80">
+        <v>100</v>
+      </c>
+      <c r="G80">
+        <v>2.4</v>
+      </c>
+      <c r="H80">
+        <v>4.8</v>
+      </c>
+      <c r="I80">
+        <v>2.1</v>
+      </c>
+      <c r="J80">
+        <v>30</v>
+      </c>
+      <c r="K80">
+        <v>50</v>
+      </c>
+      <c r="L80">
+        <v>2</v>
+      </c>
+      <c r="M80">
+        <v>1000</v>
+      </c>
+      <c r="N80">
+        <v>4</v>
+      </c>
+      <c r="O80">
+        <f t="shared" si="17"/>
+        <v>2.7E-6</v>
+      </c>
+      <c r="P80" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q80">
+        <v>7000</v>
+      </c>
+      <c r="R80">
+        <v>5</v>
+      </c>
+      <c r="S80" t="s">
+        <v>27</v>
+      </c>
+      <c r="T80">
+        <v>0.05</v>
+      </c>
+      <c r="U80">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="81" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A81" t="s">
+        <v>29</v>
+      </c>
+      <c r="B81">
+        <f t="shared" si="18"/>
+        <v>5</v>
+      </c>
+      <c r="C81">
+        <f t="shared" si="19"/>
+        <v>4900</v>
+      </c>
+      <c r="D81" t="s">
+        <v>8</v>
+      </c>
+      <c r="E81">
+        <v>1</v>
+      </c>
+      <c r="F81">
+        <v>100</v>
+      </c>
+      <c r="G81">
+        <v>2.4</v>
+      </c>
+      <c r="H81">
+        <v>4.8</v>
+      </c>
+      <c r="I81">
+        <v>2.1</v>
+      </c>
+      <c r="J81">
+        <v>30</v>
+      </c>
+      <c r="K81">
+        <v>50</v>
+      </c>
+      <c r="L81">
+        <v>2</v>
+      </c>
+      <c r="M81">
+        <v>1000</v>
+      </c>
+      <c r="N81">
+        <v>4</v>
+      </c>
+      <c r="O81">
+        <f t="shared" si="17"/>
+        <v>2.7E-6</v>
+      </c>
+      <c r="P81" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q81">
+        <v>7000</v>
+      </c>
+      <c r="R81">
+        <v>5</v>
+      </c>
+      <c r="S81" t="s">
+        <v>27</v>
+      </c>
+      <c r="T81">
+        <v>0.05</v>
+      </c>
+      <c r="U81">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="82" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A82" t="s">
+        <v>29</v>
+      </c>
+      <c r="B82">
+        <f t="shared" si="18"/>
+        <v>6</v>
+      </c>
+      <c r="C82">
+        <f t="shared" si="19"/>
+        <v>6100</v>
+      </c>
+      <c r="D82" t="s">
+        <v>8</v>
+      </c>
+      <c r="E82">
+        <v>1</v>
+      </c>
+      <c r="F82">
+        <v>100</v>
+      </c>
+      <c r="G82">
+        <v>2.4</v>
+      </c>
+      <c r="H82">
+        <v>4.8</v>
+      </c>
+      <c r="I82">
+        <v>2.1</v>
+      </c>
+      <c r="J82">
+        <v>30</v>
+      </c>
+      <c r="K82">
+        <v>50</v>
+      </c>
+      <c r="L82">
+        <v>2</v>
+      </c>
+      <c r="M82">
+        <v>1000</v>
+      </c>
+      <c r="N82">
+        <v>4</v>
+      </c>
+      <c r="O82">
+        <f t="shared" si="17"/>
+        <v>2.7E-6</v>
+      </c>
+      <c r="P82" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q82">
+        <v>7000</v>
+      </c>
+      <c r="R82">
+        <v>5</v>
+      </c>
+      <c r="S82" t="s">
+        <v>27</v>
+      </c>
+      <c r="T82">
+        <v>0.05</v>
+      </c>
+      <c r="U82">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="83" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A83" t="s">
+        <v>29</v>
+      </c>
+      <c r="B83">
+        <f t="shared" si="18"/>
+        <v>7</v>
+      </c>
+      <c r="C83">
+        <f t="shared" si="19"/>
+        <v>7300</v>
+      </c>
+      <c r="D83" t="s">
+        <v>8</v>
+      </c>
+      <c r="E83">
+        <v>1</v>
+      </c>
+      <c r="F83">
+        <v>100</v>
+      </c>
+      <c r="G83">
+        <v>2.4</v>
+      </c>
+      <c r="H83">
+        <v>4.8</v>
+      </c>
+      <c r="I83">
+        <v>2.1</v>
+      </c>
+      <c r="J83">
+        <v>30</v>
+      </c>
+      <c r="K83">
+        <v>50</v>
+      </c>
+      <c r="L83">
+        <v>2</v>
+      </c>
+      <c r="M83">
+        <v>1000</v>
+      </c>
+      <c r="N83">
+        <v>4</v>
+      </c>
+      <c r="O83">
+        <f t="shared" si="17"/>
+        <v>2.7E-6</v>
+      </c>
+      <c r="P83" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q83">
+        <v>7000</v>
+      </c>
+      <c r="R83">
+        <v>5</v>
+      </c>
+      <c r="S83" t="s">
+        <v>27</v>
+      </c>
+      <c r="T83">
+        <v>0.05</v>
+      </c>
+      <c r="U83">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="84" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A84" t="s">
+        <v>29</v>
+      </c>
+      <c r="B84">
+        <f t="shared" si="18"/>
+        <v>8</v>
+      </c>
+      <c r="C84">
+        <f t="shared" si="19"/>
+        <v>8500</v>
+      </c>
+      <c r="D84" t="s">
+        <v>8</v>
+      </c>
+      <c r="E84">
+        <v>1</v>
+      </c>
+      <c r="F84">
+        <v>100</v>
+      </c>
+      <c r="G84">
+        <v>2.4</v>
+      </c>
+      <c r="H84">
+        <v>4.8</v>
+      </c>
+      <c r="I84">
+        <v>2.1</v>
+      </c>
+      <c r="J84">
+        <v>30</v>
+      </c>
+      <c r="K84">
+        <v>50</v>
+      </c>
+      <c r="L84">
+        <v>2</v>
+      </c>
+      <c r="M84">
+        <v>1000</v>
+      </c>
+      <c r="N84">
+        <v>4</v>
+      </c>
+      <c r="O84">
+        <f t="shared" si="17"/>
+        <v>2.7E-6</v>
+      </c>
+      <c r="P84" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q84">
+        <v>7000</v>
+      </c>
+      <c r="R84">
+        <v>5</v>
+      </c>
+      <c r="S84" t="s">
+        <v>27</v>
+      </c>
+      <c r="T84">
+        <v>0.05</v>
+      </c>
+      <c r="U84">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="85" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A85" t="s">
+        <v>29</v>
+      </c>
+      <c r="B85">
+        <f t="shared" si="18"/>
+        <v>9</v>
+      </c>
+      <c r="C85">
+        <f t="shared" si="19"/>
+        <v>9700</v>
+      </c>
+      <c r="D85" t="s">
+        <v>8</v>
+      </c>
+      <c r="E85">
+        <v>1</v>
+      </c>
+      <c r="F85">
+        <v>100</v>
+      </c>
+      <c r="G85">
+        <v>2.4</v>
+      </c>
+      <c r="H85">
+        <v>4.8</v>
+      </c>
+      <c r="I85">
+        <v>2.1</v>
+      </c>
+      <c r="J85">
+        <v>30</v>
+      </c>
+      <c r="K85">
+        <v>50</v>
+      </c>
+      <c r="L85">
+        <v>2</v>
+      </c>
+      <c r="M85">
+        <v>1000</v>
+      </c>
+      <c r="N85">
+        <v>4</v>
+      </c>
+      <c r="O85">
+        <f t="shared" si="17"/>
+        <v>2.7E-6</v>
+      </c>
+      <c r="P85" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q85">
+        <v>7000</v>
+      </c>
+      <c r="R85">
+        <v>5</v>
+      </c>
+      <c r="S85" t="s">
+        <v>27</v>
+      </c>
+      <c r="T85">
+        <v>0.05</v>
+      </c>
+      <c r="U85">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="86" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A86" t="s">
+        <v>29</v>
+      </c>
+      <c r="B86">
+        <f t="shared" si="18"/>
+        <v>10</v>
+      </c>
+      <c r="C86">
+        <f t="shared" si="19"/>
+        <v>10900</v>
+      </c>
+      <c r="D86" t="s">
+        <v>8</v>
+      </c>
+      <c r="E86">
+        <v>1</v>
+      </c>
+      <c r="F86">
+        <v>100</v>
+      </c>
+      <c r="G86">
+        <v>2.4</v>
+      </c>
+      <c r="H86">
+        <v>4.8</v>
+      </c>
+      <c r="I86">
+        <v>2.1</v>
+      </c>
+      <c r="J86">
+        <v>30</v>
+      </c>
+      <c r="K86">
+        <v>50</v>
+      </c>
+      <c r="L86">
+        <v>2</v>
+      </c>
+      <c r="M86">
+        <v>1000</v>
+      </c>
+      <c r="N86">
+        <v>4</v>
+      </c>
+      <c r="O86">
+        <f t="shared" si="17"/>
+        <v>2.7E-6</v>
+      </c>
+      <c r="P86" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q86">
+        <v>7000</v>
+      </c>
+      <c r="R86">
+        <v>5</v>
+      </c>
+      <c r="S86" t="s">
+        <v>27</v>
+      </c>
+      <c r="T86">
+        <v>0.05</v>
+      </c>
+      <c r="U86">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="87" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A87" t="s">
+        <v>29</v>
+      </c>
+      <c r="B87">
+        <f t="shared" si="18"/>
+        <v>11</v>
+      </c>
+      <c r="C87">
+        <f t="shared" si="19"/>
+        <v>12100</v>
+      </c>
+      <c r="D87" t="s">
+        <v>8</v>
+      </c>
+      <c r="E87">
+        <v>1</v>
+      </c>
+      <c r="F87">
+        <v>100</v>
+      </c>
+      <c r="G87">
+        <v>2.4</v>
+      </c>
+      <c r="H87">
+        <v>4.8</v>
+      </c>
+      <c r="I87">
+        <v>2.1</v>
+      </c>
+      <c r="J87">
+        <v>30</v>
+      </c>
+      <c r="K87">
+        <v>50</v>
+      </c>
+      <c r="L87">
+        <v>2</v>
+      </c>
+      <c r="M87">
+        <v>1000</v>
+      </c>
+      <c r="N87">
+        <v>4</v>
+      </c>
+      <c r="O87">
+        <f t="shared" si="17"/>
+        <v>2.7E-6</v>
+      </c>
+      <c r="P87" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q87">
+        <v>7000</v>
+      </c>
+      <c r="R87">
+        <v>5</v>
+      </c>
+      <c r="S87" t="s">
+        <v>27</v>
+      </c>
+      <c r="T87">
+        <v>0.05</v>
+      </c>
+      <c r="U87">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="88" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A88" t="s">
+        <v>29</v>
+      </c>
+      <c r="B88">
+        <f t="shared" si="18"/>
+        <v>12</v>
+      </c>
+      <c r="C88">
+        <f t="shared" si="19"/>
+        <v>13300</v>
+      </c>
+      <c r="D88" t="s">
+        <v>8</v>
+      </c>
+      <c r="E88">
+        <v>1</v>
+      </c>
+      <c r="F88">
+        <v>100</v>
+      </c>
+      <c r="G88">
+        <v>2.4</v>
+      </c>
+      <c r="H88">
+        <v>4.8</v>
+      </c>
+      <c r="I88">
+        <v>2.1</v>
+      </c>
+      <c r="J88">
+        <v>30</v>
+      </c>
+      <c r="K88">
+        <v>50</v>
+      </c>
+      <c r="L88">
+        <v>2</v>
+      </c>
+      <c r="M88">
+        <v>1000</v>
+      </c>
+      <c r="N88">
+        <v>4</v>
+      </c>
+      <c r="O88">
+        <f t="shared" si="17"/>
+        <v>2.7E-6</v>
+      </c>
+      <c r="P88" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q88">
+        <v>7000</v>
+      </c>
+      <c r="R88">
+        <v>5</v>
+      </c>
+      <c r="S88" t="s">
+        <v>27</v>
+      </c>
+      <c r="T88">
+        <v>0.05</v>
+      </c>
+      <c r="U88">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="89" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A89" t="s">
+        <v>29</v>
+      </c>
+      <c r="B89">
+        <f t="shared" si="18"/>
+        <v>13</v>
+      </c>
+      <c r="C89">
+        <f t="shared" si="19"/>
+        <v>14500</v>
+      </c>
+      <c r="D89" t="s">
+        <v>8</v>
+      </c>
+      <c r="E89">
+        <v>1</v>
+      </c>
+      <c r="F89">
+        <v>100</v>
+      </c>
+      <c r="G89">
+        <v>2.4</v>
+      </c>
+      <c r="H89">
+        <v>4.8</v>
+      </c>
+      <c r="I89">
+        <v>2.1</v>
+      </c>
+      <c r="J89">
+        <v>30</v>
+      </c>
+      <c r="K89">
+        <v>50</v>
+      </c>
+      <c r="L89">
+        <v>2</v>
+      </c>
+      <c r="M89">
+        <v>1000</v>
+      </c>
+      <c r="N89">
+        <v>4</v>
+      </c>
+      <c r="O89">
+        <f t="shared" si="17"/>
+        <v>2.7E-6</v>
+      </c>
+      <c r="P89" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q89">
+        <v>7000</v>
+      </c>
+      <c r="R89">
+        <v>5</v>
+      </c>
+      <c r="S89" t="s">
+        <v>27</v>
+      </c>
+      <c r="T89">
+        <v>0.05</v>
+      </c>
+      <c r="U89">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="90" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A90" t="s">
+        <v>29</v>
+      </c>
+      <c r="B90">
+        <f t="shared" si="18"/>
+        <v>14</v>
+      </c>
+      <c r="C90">
+        <f t="shared" si="19"/>
+        <v>15700</v>
+      </c>
+      <c r="D90" t="s">
+        <v>8</v>
+      </c>
+      <c r="E90">
+        <v>1</v>
+      </c>
+      <c r="F90">
+        <v>100</v>
+      </c>
+      <c r="G90">
+        <v>2.4</v>
+      </c>
+      <c r="H90">
+        <v>4.8</v>
+      </c>
+      <c r="I90">
+        <v>2.1</v>
+      </c>
+      <c r="J90">
+        <v>30</v>
+      </c>
+      <c r="K90">
+        <v>50</v>
+      </c>
+      <c r="L90">
+        <v>2</v>
+      </c>
+      <c r="M90">
+        <v>1000</v>
+      </c>
+      <c r="N90">
+        <v>4</v>
+      </c>
+      <c r="O90">
+        <f t="shared" si="17"/>
+        <v>2.7E-6</v>
+      </c>
+      <c r="P90" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q90">
+        <v>7000</v>
+      </c>
+      <c r="R90">
+        <v>5</v>
+      </c>
+      <c r="S90" t="s">
+        <v>27</v>
+      </c>
+      <c r="T90">
+        <v>0.05</v>
+      </c>
+      <c r="U90">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="91" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A91" t="s">
+        <v>29</v>
+      </c>
+      <c r="B91">
+        <f t="shared" si="18"/>
+        <v>15</v>
+      </c>
+      <c r="C91">
+        <f t="shared" si="19"/>
+        <v>16900</v>
+      </c>
+      <c r="D91" t="s">
+        <v>8</v>
+      </c>
+      <c r="E91">
+        <v>1</v>
+      </c>
+      <c r="F91">
+        <v>100</v>
+      </c>
+      <c r="G91">
+        <v>2.4</v>
+      </c>
+      <c r="H91">
+        <v>4.8</v>
+      </c>
+      <c r="I91">
+        <v>2.1</v>
+      </c>
+      <c r="J91">
+        <v>30</v>
+      </c>
+      <c r="K91">
+        <v>50</v>
+      </c>
+      <c r="L91">
+        <v>2</v>
+      </c>
+      <c r="M91">
+        <v>1000</v>
+      </c>
+      <c r="N91">
+        <v>4</v>
+      </c>
+      <c r="O91">
+        <f t="shared" si="17"/>
+        <v>2.7E-6</v>
+      </c>
+      <c r="P91" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q91">
+        <v>7000</v>
+      </c>
+      <c r="R91">
+        <v>5</v>
+      </c>
+      <c r="S91" t="s">
+        <v>27</v>
+      </c>
+      <c r="T91">
+        <v>0.05</v>
+      </c>
+      <c r="U91">
+        <v>110</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:A76">
-    <filterColumn colId="0">
-      <filters>
-        <filter val="180921_10mg-kgAMPH-1.csv"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:A91"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
4 WT, 4 KO
</commit_message>
<xml_diff>
--- a/scripts/file_params.xlsx
+++ b/scripts/file_params.xlsx
@@ -9,13 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="8660" yWindow="2820" windowWidth="18560" windowHeight="13040" tabRatio="500"/>
+    <workbookView xWindow="9780" yWindow="2720" windowWidth="18560" windowHeight="13040" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="file_params" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">file_params!$A$1:$A$91</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">file_params!$A$1:$B$106</definedName>
   </definedNames>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="35">
   <si>
     <t>filename</t>
   </si>
@@ -120,6 +120,21 @@
   </si>
   <si>
     <t>180921_10mg-kgAMPH-2.csv</t>
+  </si>
+  <si>
+    <t>190205_a-synKO_2_AMPH_1.csv</t>
+  </si>
+  <si>
+    <t>comment</t>
+  </si>
+  <si>
+    <t>Drop produces false baseline.</t>
+  </si>
+  <si>
+    <t>all</t>
+  </si>
+  <si>
+    <t>190205_a-synKO_2_AMPH_2.csv</t>
   </si>
 </sst>
 </file>
@@ -458,18 +473,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U91"/>
+  <dimension ref="A1:V121"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C75" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C102" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A7" sqref="A7"/>
+      <selection pane="bottomRight" activeCell="B110" sqref="B110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="25.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="30" customWidth="1"/>
     <col min="2" max="2" width="8" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="6.1640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.6640625" bestFit="1" customWidth="1"/>
@@ -492,7 +507,7 @@
     <col min="21" max="21" width="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -556,8 +571,11 @@
       <c r="U1" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="V1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -623,7 +641,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -689,7 +707,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -755,7 +773,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -821,7 +839,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -887,7 +905,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>3</v>
       </c>
@@ -954,7 +972,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>3</v>
       </c>
@@ -1021,7 +1039,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>3</v>
       </c>
@@ -1088,7 +1106,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>3</v>
       </c>
@@ -1155,7 +1173,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>3</v>
       </c>
@@ -1222,7 +1240,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>3</v>
       </c>
@@ -1289,7 +1307,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>3</v>
       </c>
@@ -1356,7 +1374,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>3</v>
       </c>
@@ -1423,7 +1441,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>3</v>
       </c>
@@ -1489,7 +1507,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>3</v>
       </c>
@@ -1570,7 +1588,7 @@
         <v>8</v>
       </c>
       <c r="E17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F17">
         <v>100</v>
@@ -1639,7 +1657,7 @@
         <v>8</v>
       </c>
       <c r="E18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F18">
         <v>100</v>
@@ -1708,7 +1726,7 @@
         <v>8</v>
       </c>
       <c r="E19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F19">
         <v>100</v>
@@ -3636,7 +3654,7 @@
         <v>9</v>
       </c>
       <c r="E47">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F47">
         <v>100</v>
@@ -3706,8 +3724,7 @@
         <v>ko</v>
       </c>
       <c r="E48">
-        <f>E47</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F48">
         <v>100</v>
@@ -3777,8 +3794,7 @@
         <v>ko</v>
       </c>
       <c r="E49">
-        <f t="shared" ref="E49" si="14">E48</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F49">
         <v>100</v>
@@ -4808,11 +4824,11 @@
         <v>28</v>
       </c>
       <c r="B64">
-        <f t="shared" ref="B64:B81" si="15">B63+1</f>
+        <f t="shared" ref="B64:B81" si="14">B63+1</f>
         <v>3</v>
       </c>
       <c r="C64">
-        <f t="shared" ref="C64:C76" si="16">C63+1200</f>
+        <f t="shared" ref="C64:C76" si="15">C63+1200</f>
         <v>2500</v>
       </c>
       <c r="D64" t="s">
@@ -4876,11 +4892,11 @@
         <v>28</v>
       </c>
       <c r="B65">
+        <f t="shared" si="14"/>
+        <v>4</v>
+      </c>
+      <c r="C65">
         <f t="shared" si="15"/>
-        <v>4</v>
-      </c>
-      <c r="C65">
-        <f t="shared" si="16"/>
         <v>3700</v>
       </c>
       <c r="D65" t="s">
@@ -4944,11 +4960,11 @@
         <v>28</v>
       </c>
       <c r="B66">
+        <f t="shared" si="14"/>
+        <v>5</v>
+      </c>
+      <c r="C66">
         <f t="shared" si="15"/>
-        <v>5</v>
-      </c>
-      <c r="C66">
-        <f t="shared" si="16"/>
         <v>4900</v>
       </c>
       <c r="D66" t="s">
@@ -5012,11 +5028,11 @@
         <v>28</v>
       </c>
       <c r="B67">
+        <f t="shared" si="14"/>
+        <v>6</v>
+      </c>
+      <c r="C67">
         <f t="shared" si="15"/>
-        <v>6</v>
-      </c>
-      <c r="C67">
-        <f t="shared" si="16"/>
         <v>6100</v>
       </c>
       <c r="D67" t="s">
@@ -5053,7 +5069,7 @@
         <v>4</v>
       </c>
       <c r="O67">
-        <f t="shared" ref="O67:O95" si="17">2.7*10^-6</f>
+        <f t="shared" ref="O67:O128" si="16">2.7*10^-6</f>
         <v>2.7E-6</v>
       </c>
       <c r="P67" t="b">
@@ -5080,11 +5096,11 @@
         <v>28</v>
       </c>
       <c r="B68">
+        <f t="shared" si="14"/>
+        <v>7</v>
+      </c>
+      <c r="C68">
         <f t="shared" si="15"/>
-        <v>7</v>
-      </c>
-      <c r="C68">
-        <f t="shared" si="16"/>
         <v>7300</v>
       </c>
       <c r="D68" t="s">
@@ -5121,7 +5137,7 @@
         <v>4</v>
       </c>
       <c r="O68">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v>2.7E-6</v>
       </c>
       <c r="P68" t="b">
@@ -5148,11 +5164,11 @@
         <v>28</v>
       </c>
       <c r="B69">
+        <f t="shared" si="14"/>
+        <v>8</v>
+      </c>
+      <c r="C69">
         <f t="shared" si="15"/>
-        <v>8</v>
-      </c>
-      <c r="C69">
-        <f t="shared" si="16"/>
         <v>8500</v>
       </c>
       <c r="D69" t="s">
@@ -5189,7 +5205,7 @@
         <v>4</v>
       </c>
       <c r="O69">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v>2.7E-6</v>
       </c>
       <c r="P69" t="b">
@@ -5216,11 +5232,11 @@
         <v>28</v>
       </c>
       <c r="B70">
+        <f t="shared" si="14"/>
+        <v>9</v>
+      </c>
+      <c r="C70">
         <f t="shared" si="15"/>
-        <v>9</v>
-      </c>
-      <c r="C70">
-        <f t="shared" si="16"/>
         <v>9700</v>
       </c>
       <c r="D70" t="s">
@@ -5257,7 +5273,7 @@
         <v>4</v>
       </c>
       <c r="O70">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v>2.7E-6</v>
       </c>
       <c r="P70" t="b">
@@ -5284,11 +5300,11 @@
         <v>28</v>
       </c>
       <c r="B71">
+        <f t="shared" si="14"/>
+        <v>10</v>
+      </c>
+      <c r="C71">
         <f t="shared" si="15"/>
-        <v>10</v>
-      </c>
-      <c r="C71">
-        <f t="shared" si="16"/>
         <v>10900</v>
       </c>
       <c r="D71" t="s">
@@ -5325,7 +5341,7 @@
         <v>4</v>
       </c>
       <c r="O71">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v>2.7E-6</v>
       </c>
       <c r="P71" t="b">
@@ -5352,11 +5368,11 @@
         <v>28</v>
       </c>
       <c r="B72">
+        <f t="shared" si="14"/>
+        <v>11</v>
+      </c>
+      <c r="C72">
         <f t="shared" si="15"/>
-        <v>11</v>
-      </c>
-      <c r="C72">
-        <f t="shared" si="16"/>
         <v>12100</v>
       </c>
       <c r="D72" t="s">
@@ -5393,7 +5409,7 @@
         <v>4</v>
       </c>
       <c r="O72">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v>2.7E-6</v>
       </c>
       <c r="P72" t="b">
@@ -5420,11 +5436,11 @@
         <v>28</v>
       </c>
       <c r="B73">
+        <f t="shared" si="14"/>
+        <v>12</v>
+      </c>
+      <c r="C73">
         <f t="shared" si="15"/>
-        <v>12</v>
-      </c>
-      <c r="C73">
-        <f t="shared" si="16"/>
         <v>13300</v>
       </c>
       <c r="D73" t="s">
@@ -5461,7 +5477,7 @@
         <v>4</v>
       </c>
       <c r="O73">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v>2.7E-6</v>
       </c>
       <c r="P73" t="b">
@@ -5488,11 +5504,11 @@
         <v>28</v>
       </c>
       <c r="B74">
+        <f t="shared" si="14"/>
+        <v>13</v>
+      </c>
+      <c r="C74">
         <f t="shared" si="15"/>
-        <v>13</v>
-      </c>
-      <c r="C74">
-        <f t="shared" si="16"/>
         <v>14500</v>
       </c>
       <c r="D74" t="s">
@@ -5529,7 +5545,7 @@
         <v>4</v>
       </c>
       <c r="O74">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v>2.7E-6</v>
       </c>
       <c r="P74" t="b">
@@ -5556,11 +5572,11 @@
         <v>28</v>
       </c>
       <c r="B75">
+        <f t="shared" si="14"/>
+        <v>14</v>
+      </c>
+      <c r="C75">
         <f t="shared" si="15"/>
-        <v>14</v>
-      </c>
-      <c r="C75">
-        <f t="shared" si="16"/>
         <v>15700</v>
       </c>
       <c r="D75" t="s">
@@ -5597,7 +5613,7 @@
         <v>4</v>
       </c>
       <c r="O75">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v>2.7E-6</v>
       </c>
       <c r="P75" t="b">
@@ -5624,11 +5640,11 @@
         <v>28</v>
       </c>
       <c r="B76">
+        <f t="shared" si="14"/>
+        <v>15</v>
+      </c>
+      <c r="C76">
         <f t="shared" si="15"/>
-        <v>15</v>
-      </c>
-      <c r="C76">
-        <f t="shared" si="16"/>
         <v>16900</v>
       </c>
       <c r="D76" t="s">
@@ -5665,7 +5681,7 @@
         <v>4</v>
       </c>
       <c r="O76">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v>2.7E-6</v>
       </c>
       <c r="P76" t="b">
@@ -5731,7 +5747,7 @@
         <v>4</v>
       </c>
       <c r="O77">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v>2.7E-6</v>
       </c>
       <c r="P77" t="b">
@@ -5799,7 +5815,7 @@
         <v>4</v>
       </c>
       <c r="O78">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v>2.7E-6</v>
       </c>
       <c r="P78" t="b">
@@ -5826,11 +5842,11 @@
         <v>29</v>
       </c>
       <c r="B79">
-        <f t="shared" ref="B79:B95" si="18">B78+1</f>
+        <f t="shared" ref="B79:B95" si="17">B78+1</f>
         <v>3</v>
       </c>
       <c r="C79">
-        <f t="shared" ref="C79:C95" si="19">C78+1200</f>
+        <f t="shared" ref="C79:C95" si="18">C78+1200</f>
         <v>2500</v>
       </c>
       <c r="D79" t="s">
@@ -5867,7 +5883,7 @@
         <v>4</v>
       </c>
       <c r="O79">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v>2.7E-6</v>
       </c>
       <c r="P79" t="b">
@@ -5894,11 +5910,11 @@
         <v>29</v>
       </c>
       <c r="B80">
+        <f t="shared" si="17"/>
+        <v>4</v>
+      </c>
+      <c r="C80">
         <f t="shared" si="18"/>
-        <v>4</v>
-      </c>
-      <c r="C80">
-        <f t="shared" si="19"/>
         <v>3700</v>
       </c>
       <c r="D80" t="s">
@@ -5935,7 +5951,7 @@
         <v>4</v>
       </c>
       <c r="O80">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v>2.7E-6</v>
       </c>
       <c r="P80" t="b">
@@ -5957,16 +5973,16 @@
         <v>110</v>
       </c>
     </row>
-    <row r="81" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>29</v>
       </c>
       <c r="B81">
+        <f t="shared" si="17"/>
+        <v>5</v>
+      </c>
+      <c r="C81">
         <f t="shared" si="18"/>
-        <v>5</v>
-      </c>
-      <c r="C81">
-        <f t="shared" si="19"/>
         <v>4900</v>
       </c>
       <c r="D81" t="s">
@@ -6003,7 +6019,7 @@
         <v>4</v>
       </c>
       <c r="O81">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v>2.7E-6</v>
       </c>
       <c r="P81" t="b">
@@ -6025,16 +6041,16 @@
         <v>110</v>
       </c>
     </row>
-    <row r="82" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>29</v>
       </c>
       <c r="B82">
+        <f t="shared" si="17"/>
+        <v>6</v>
+      </c>
+      <c r="C82">
         <f t="shared" si="18"/>
-        <v>6</v>
-      </c>
-      <c r="C82">
-        <f t="shared" si="19"/>
         <v>6100</v>
       </c>
       <c r="D82" t="s">
@@ -6071,7 +6087,7 @@
         <v>4</v>
       </c>
       <c r="O82">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v>2.7E-6</v>
       </c>
       <c r="P82" t="b">
@@ -6093,16 +6109,16 @@
         <v>110</v>
       </c>
     </row>
-    <row r="83" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>29</v>
       </c>
       <c r="B83">
+        <f t="shared" si="17"/>
+        <v>7</v>
+      </c>
+      <c r="C83">
         <f t="shared" si="18"/>
-        <v>7</v>
-      </c>
-      <c r="C83">
-        <f t="shared" si="19"/>
         <v>7300</v>
       </c>
       <c r="D83" t="s">
@@ -6139,7 +6155,7 @@
         <v>4</v>
       </c>
       <c r="O83">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v>2.7E-6</v>
       </c>
       <c r="P83" t="b">
@@ -6161,16 +6177,16 @@
         <v>110</v>
       </c>
     </row>
-    <row r="84" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>29</v>
       </c>
       <c r="B84">
+        <f t="shared" si="17"/>
+        <v>8</v>
+      </c>
+      <c r="C84">
         <f t="shared" si="18"/>
-        <v>8</v>
-      </c>
-      <c r="C84">
-        <f t="shared" si="19"/>
         <v>8500</v>
       </c>
       <c r="D84" t="s">
@@ -6207,7 +6223,7 @@
         <v>4</v>
       </c>
       <c r="O84">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v>2.7E-6</v>
       </c>
       <c r="P84" t="b">
@@ -6229,16 +6245,16 @@
         <v>110</v>
       </c>
     </row>
-    <row r="85" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>29</v>
       </c>
       <c r="B85">
+        <f t="shared" si="17"/>
+        <v>9</v>
+      </c>
+      <c r="C85">
         <f t="shared" si="18"/>
-        <v>9</v>
-      </c>
-      <c r="C85">
-        <f t="shared" si="19"/>
         <v>9700</v>
       </c>
       <c r="D85" t="s">
@@ -6275,7 +6291,7 @@
         <v>4</v>
       </c>
       <c r="O85">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v>2.7E-6</v>
       </c>
       <c r="P85" t="b">
@@ -6297,16 +6313,16 @@
         <v>110</v>
       </c>
     </row>
-    <row r="86" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>29</v>
       </c>
       <c r="B86">
+        <f t="shared" si="17"/>
+        <v>10</v>
+      </c>
+      <c r="C86">
         <f t="shared" si="18"/>
-        <v>10</v>
-      </c>
-      <c r="C86">
-        <f t="shared" si="19"/>
         <v>10900</v>
       </c>
       <c r="D86" t="s">
@@ -6343,7 +6359,7 @@
         <v>4</v>
       </c>
       <c r="O86">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v>2.7E-6</v>
       </c>
       <c r="P86" t="b">
@@ -6365,16 +6381,16 @@
         <v>110</v>
       </c>
     </row>
-    <row r="87" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>29</v>
       </c>
       <c r="B87">
+        <f t="shared" si="17"/>
+        <v>11</v>
+      </c>
+      <c r="C87">
         <f t="shared" si="18"/>
-        <v>11</v>
-      </c>
-      <c r="C87">
-        <f t="shared" si="19"/>
         <v>12100</v>
       </c>
       <c r="D87" t="s">
@@ -6411,7 +6427,7 @@
         <v>4</v>
       </c>
       <c r="O87">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v>2.7E-6</v>
       </c>
       <c r="P87" t="b">
@@ -6433,16 +6449,16 @@
         <v>110</v>
       </c>
     </row>
-    <row r="88" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>29</v>
       </c>
       <c r="B88">
+        <f t="shared" si="17"/>
+        <v>12</v>
+      </c>
+      <c r="C88">
         <f t="shared" si="18"/>
-        <v>12</v>
-      </c>
-      <c r="C88">
-        <f t="shared" si="19"/>
         <v>13300</v>
       </c>
       <c r="D88" t="s">
@@ -6479,7 +6495,7 @@
         <v>4</v>
       </c>
       <c r="O88">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v>2.7E-6</v>
       </c>
       <c r="P88" t="b">
@@ -6501,16 +6517,16 @@
         <v>110</v>
       </c>
     </row>
-    <row r="89" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>29</v>
       </c>
       <c r="B89">
+        <f t="shared" si="17"/>
+        <v>13</v>
+      </c>
+      <c r="C89">
         <f t="shared" si="18"/>
-        <v>13</v>
-      </c>
-      <c r="C89">
-        <f t="shared" si="19"/>
         <v>14500</v>
       </c>
       <c r="D89" t="s">
@@ -6547,7 +6563,7 @@
         <v>4</v>
       </c>
       <c r="O89">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v>2.7E-6</v>
       </c>
       <c r="P89" t="b">
@@ -6569,16 +6585,16 @@
         <v>110</v>
       </c>
     </row>
-    <row r="90" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>29</v>
       </c>
       <c r="B90">
+        <f t="shared" si="17"/>
+        <v>14</v>
+      </c>
+      <c r="C90">
         <f t="shared" si="18"/>
-        <v>14</v>
-      </c>
-      <c r="C90">
-        <f t="shared" si="19"/>
         <v>15700</v>
       </c>
       <c r="D90" t="s">
@@ -6615,7 +6631,7 @@
         <v>4</v>
       </c>
       <c r="O90">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v>2.7E-6</v>
       </c>
       <c r="P90" t="b">
@@ -6637,16 +6653,16 @@
         <v>110</v>
       </c>
     </row>
-    <row r="91" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>29</v>
       </c>
       <c r="B91">
+        <f t="shared" si="17"/>
+        <v>15</v>
+      </c>
+      <c r="C91">
         <f t="shared" si="18"/>
-        <v>15</v>
-      </c>
-      <c r="C91">
-        <f t="shared" si="19"/>
         <v>16900</v>
       </c>
       <c r="D91" t="s">
@@ -6683,7 +6699,7 @@
         <v>4</v>
       </c>
       <c r="O91">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v>2.7E-6</v>
       </c>
       <c r="P91" t="b">
@@ -6705,8 +6721,2046 @@
         <v>110</v>
       </c>
     </row>
+    <row r="92" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A92" t="s">
+        <v>30</v>
+      </c>
+      <c r="B92">
+        <v>1</v>
+      </c>
+      <c r="C92">
+        <v>100</v>
+      </c>
+      <c r="D92" t="s">
+        <v>9</v>
+      </c>
+      <c r="E92">
+        <v>0</v>
+      </c>
+      <c r="F92">
+        <v>100</v>
+      </c>
+      <c r="G92">
+        <v>2.4</v>
+      </c>
+      <c r="H92">
+        <v>4.8</v>
+      </c>
+      <c r="I92">
+        <v>2.1</v>
+      </c>
+      <c r="J92">
+        <v>30</v>
+      </c>
+      <c r="K92">
+        <v>50</v>
+      </c>
+      <c r="L92">
+        <v>2</v>
+      </c>
+      <c r="M92">
+        <v>1000</v>
+      </c>
+      <c r="N92">
+        <v>4</v>
+      </c>
+      <c r="O92">
+        <f t="shared" si="16"/>
+        <v>2.7E-6</v>
+      </c>
+      <c r="P92" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q92">
+        <v>10400</v>
+      </c>
+      <c r="R92">
+        <v>5</v>
+      </c>
+      <c r="S92" t="s">
+        <v>27</v>
+      </c>
+      <c r="T92">
+        <v>0.05</v>
+      </c>
+      <c r="U92">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="93" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A93" t="s">
+        <v>30</v>
+      </c>
+      <c r="B93">
+        <f>B92+1</f>
+        <v>2</v>
+      </c>
+      <c r="C93">
+        <f>C92+1200</f>
+        <v>1300</v>
+      </c>
+      <c r="D93" t="s">
+        <v>9</v>
+      </c>
+      <c r="E93">
+        <v>0</v>
+      </c>
+      <c r="F93">
+        <v>100</v>
+      </c>
+      <c r="G93">
+        <v>2.4</v>
+      </c>
+      <c r="H93">
+        <v>4.8</v>
+      </c>
+      <c r="I93">
+        <v>2.1</v>
+      </c>
+      <c r="J93">
+        <v>30</v>
+      </c>
+      <c r="K93">
+        <v>50</v>
+      </c>
+      <c r="L93">
+        <v>2</v>
+      </c>
+      <c r="M93">
+        <v>1000</v>
+      </c>
+      <c r="N93">
+        <v>4</v>
+      </c>
+      <c r="O93">
+        <f t="shared" si="16"/>
+        <v>2.7E-6</v>
+      </c>
+      <c r="P93" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q93">
+        <v>10400</v>
+      </c>
+      <c r="R93">
+        <v>5</v>
+      </c>
+      <c r="S93" t="s">
+        <v>33</v>
+      </c>
+      <c r="T93">
+        <v>0.05</v>
+      </c>
+      <c r="U93">
+        <v>110</v>
+      </c>
+      <c r="V93" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="94" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A94" t="s">
+        <v>30</v>
+      </c>
+      <c r="B94">
+        <f t="shared" ref="B94:B111" si="19">B93+1</f>
+        <v>3</v>
+      </c>
+      <c r="C94">
+        <f t="shared" ref="C94:C111" si="20">C93+1200</f>
+        <v>2500</v>
+      </c>
+      <c r="D94" t="s">
+        <v>9</v>
+      </c>
+      <c r="E94">
+        <v>0</v>
+      </c>
+      <c r="F94">
+        <v>100</v>
+      </c>
+      <c r="G94">
+        <v>2.4</v>
+      </c>
+      <c r="H94">
+        <v>4.8</v>
+      </c>
+      <c r="I94">
+        <v>2.1</v>
+      </c>
+      <c r="J94">
+        <v>30</v>
+      </c>
+      <c r="K94">
+        <v>50</v>
+      </c>
+      <c r="L94">
+        <v>2</v>
+      </c>
+      <c r="M94">
+        <v>1000</v>
+      </c>
+      <c r="N94">
+        <v>4</v>
+      </c>
+      <c r="O94">
+        <f t="shared" si="16"/>
+        <v>2.7E-6</v>
+      </c>
+      <c r="P94" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q94">
+        <v>10400</v>
+      </c>
+      <c r="R94">
+        <v>5</v>
+      </c>
+      <c r="S94" t="s">
+        <v>27</v>
+      </c>
+      <c r="T94">
+        <v>0.05</v>
+      </c>
+      <c r="U94">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="95" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A95" t="s">
+        <v>30</v>
+      </c>
+      <c r="B95">
+        <f t="shared" si="19"/>
+        <v>4</v>
+      </c>
+      <c r="C95">
+        <f t="shared" si="20"/>
+        <v>3700</v>
+      </c>
+      <c r="D95" t="s">
+        <v>9</v>
+      </c>
+      <c r="E95">
+        <v>1</v>
+      </c>
+      <c r="F95">
+        <v>100</v>
+      </c>
+      <c r="G95">
+        <v>2.4</v>
+      </c>
+      <c r="H95">
+        <v>4.8</v>
+      </c>
+      <c r="I95">
+        <v>2.1</v>
+      </c>
+      <c r="J95">
+        <v>30</v>
+      </c>
+      <c r="K95">
+        <v>50</v>
+      </c>
+      <c r="L95">
+        <v>2</v>
+      </c>
+      <c r="M95">
+        <v>1000</v>
+      </c>
+      <c r="N95">
+        <v>4</v>
+      </c>
+      <c r="O95">
+        <f t="shared" si="16"/>
+        <v>2.7E-6</v>
+      </c>
+      <c r="P95" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q95">
+        <v>10400</v>
+      </c>
+      <c r="R95">
+        <v>5</v>
+      </c>
+      <c r="S95" t="s">
+        <v>27</v>
+      </c>
+      <c r="T95">
+        <v>0.05</v>
+      </c>
+      <c r="U95">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="96" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A96" t="s">
+        <v>30</v>
+      </c>
+      <c r="B96">
+        <f t="shared" si="19"/>
+        <v>5</v>
+      </c>
+      <c r="C96">
+        <f t="shared" si="20"/>
+        <v>4900</v>
+      </c>
+      <c r="D96" t="s">
+        <v>9</v>
+      </c>
+      <c r="E96">
+        <v>1</v>
+      </c>
+      <c r="F96">
+        <v>100</v>
+      </c>
+      <c r="G96">
+        <v>2.4</v>
+      </c>
+      <c r="H96">
+        <v>4.8</v>
+      </c>
+      <c r="I96">
+        <v>2.1</v>
+      </c>
+      <c r="J96">
+        <v>30</v>
+      </c>
+      <c r="K96">
+        <v>50</v>
+      </c>
+      <c r="L96">
+        <v>2</v>
+      </c>
+      <c r="M96">
+        <v>1000</v>
+      </c>
+      <c r="N96">
+        <v>4</v>
+      </c>
+      <c r="O96">
+        <f t="shared" si="16"/>
+        <v>2.7E-6</v>
+      </c>
+      <c r="P96" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q96">
+        <v>10400</v>
+      </c>
+      <c r="R96">
+        <v>5</v>
+      </c>
+      <c r="S96" t="s">
+        <v>27</v>
+      </c>
+      <c r="T96">
+        <v>0.05</v>
+      </c>
+      <c r="U96">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="97" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A97" t="s">
+        <v>30</v>
+      </c>
+      <c r="B97">
+        <f t="shared" si="19"/>
+        <v>6</v>
+      </c>
+      <c r="C97">
+        <f t="shared" si="20"/>
+        <v>6100</v>
+      </c>
+      <c r="D97" t="s">
+        <v>9</v>
+      </c>
+      <c r="E97">
+        <v>1</v>
+      </c>
+      <c r="F97">
+        <v>100</v>
+      </c>
+      <c r="G97">
+        <v>2.4</v>
+      </c>
+      <c r="H97">
+        <v>4.8</v>
+      </c>
+      <c r="I97">
+        <v>2.1</v>
+      </c>
+      <c r="J97">
+        <v>30</v>
+      </c>
+      <c r="K97">
+        <v>50</v>
+      </c>
+      <c r="L97">
+        <v>2</v>
+      </c>
+      <c r="M97">
+        <v>1000</v>
+      </c>
+      <c r="N97">
+        <v>4</v>
+      </c>
+      <c r="O97">
+        <f t="shared" si="16"/>
+        <v>2.7E-6</v>
+      </c>
+      <c r="P97" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q97">
+        <v>10400</v>
+      </c>
+      <c r="R97">
+        <v>5</v>
+      </c>
+      <c r="S97" t="s">
+        <v>27</v>
+      </c>
+      <c r="T97">
+        <v>0.05</v>
+      </c>
+      <c r="U97">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="98" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A98" t="s">
+        <v>30</v>
+      </c>
+      <c r="B98">
+        <f t="shared" si="19"/>
+        <v>7</v>
+      </c>
+      <c r="C98">
+        <f t="shared" si="20"/>
+        <v>7300</v>
+      </c>
+      <c r="D98" t="s">
+        <v>9</v>
+      </c>
+      <c r="E98">
+        <v>1</v>
+      </c>
+      <c r="F98">
+        <v>100</v>
+      </c>
+      <c r="G98">
+        <v>2.4</v>
+      </c>
+      <c r="H98">
+        <v>4.8</v>
+      </c>
+      <c r="I98">
+        <v>2.1</v>
+      </c>
+      <c r="J98">
+        <v>30</v>
+      </c>
+      <c r="K98">
+        <v>50</v>
+      </c>
+      <c r="L98">
+        <v>2</v>
+      </c>
+      <c r="M98">
+        <v>1000</v>
+      </c>
+      <c r="N98">
+        <v>4</v>
+      </c>
+      <c r="O98">
+        <f t="shared" si="16"/>
+        <v>2.7E-6</v>
+      </c>
+      <c r="P98" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q98">
+        <v>10400</v>
+      </c>
+      <c r="R98">
+        <v>5</v>
+      </c>
+      <c r="S98" t="s">
+        <v>27</v>
+      </c>
+      <c r="T98">
+        <v>0.05</v>
+      </c>
+      <c r="U98">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="99" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A99" t="s">
+        <v>30</v>
+      </c>
+      <c r="B99">
+        <f t="shared" si="19"/>
+        <v>8</v>
+      </c>
+      <c r="C99">
+        <f t="shared" si="20"/>
+        <v>8500</v>
+      </c>
+      <c r="D99" t="s">
+        <v>9</v>
+      </c>
+      <c r="E99">
+        <v>1</v>
+      </c>
+      <c r="F99">
+        <v>100</v>
+      </c>
+      <c r="G99">
+        <v>2.4</v>
+      </c>
+      <c r="H99">
+        <v>4.8</v>
+      </c>
+      <c r="I99">
+        <v>2.1</v>
+      </c>
+      <c r="J99">
+        <v>30</v>
+      </c>
+      <c r="K99">
+        <v>50</v>
+      </c>
+      <c r="L99">
+        <v>2</v>
+      </c>
+      <c r="M99">
+        <v>1000</v>
+      </c>
+      <c r="N99">
+        <v>4</v>
+      </c>
+      <c r="O99">
+        <f t="shared" si="16"/>
+        <v>2.7E-6</v>
+      </c>
+      <c r="P99" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q99">
+        <v>10400</v>
+      </c>
+      <c r="R99">
+        <v>5</v>
+      </c>
+      <c r="S99" t="s">
+        <v>27</v>
+      </c>
+      <c r="T99">
+        <v>0.05</v>
+      </c>
+      <c r="U99">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="100" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A100" t="s">
+        <v>30</v>
+      </c>
+      <c r="B100">
+        <f t="shared" si="19"/>
+        <v>9</v>
+      </c>
+      <c r="C100">
+        <f t="shared" si="20"/>
+        <v>9700</v>
+      </c>
+      <c r="D100" t="s">
+        <v>9</v>
+      </c>
+      <c r="E100">
+        <v>1</v>
+      </c>
+      <c r="F100">
+        <v>100</v>
+      </c>
+      <c r="G100">
+        <v>2.4</v>
+      </c>
+      <c r="H100">
+        <v>4.8</v>
+      </c>
+      <c r="I100">
+        <v>2.1</v>
+      </c>
+      <c r="J100">
+        <v>30</v>
+      </c>
+      <c r="K100">
+        <v>50</v>
+      </c>
+      <c r="L100">
+        <v>2</v>
+      </c>
+      <c r="M100">
+        <v>1000</v>
+      </c>
+      <c r="N100">
+        <v>4</v>
+      </c>
+      <c r="O100">
+        <f t="shared" si="16"/>
+        <v>2.7E-6</v>
+      </c>
+      <c r="P100" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q100">
+        <v>10400</v>
+      </c>
+      <c r="R100">
+        <v>5</v>
+      </c>
+      <c r="S100" t="s">
+        <v>27</v>
+      </c>
+      <c r="T100">
+        <v>0.05</v>
+      </c>
+      <c r="U100">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="101" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A101" t="s">
+        <v>30</v>
+      </c>
+      <c r="B101">
+        <f t="shared" si="19"/>
+        <v>10</v>
+      </c>
+      <c r="C101">
+        <f t="shared" si="20"/>
+        <v>10900</v>
+      </c>
+      <c r="D101" t="s">
+        <v>9</v>
+      </c>
+      <c r="E101">
+        <v>1</v>
+      </c>
+      <c r="F101">
+        <v>100</v>
+      </c>
+      <c r="G101">
+        <v>2.4</v>
+      </c>
+      <c r="H101">
+        <v>4.8</v>
+      </c>
+      <c r="I101">
+        <v>2.1</v>
+      </c>
+      <c r="J101">
+        <v>30</v>
+      </c>
+      <c r="K101">
+        <v>50</v>
+      </c>
+      <c r="L101">
+        <v>2</v>
+      </c>
+      <c r="M101">
+        <v>1000</v>
+      </c>
+      <c r="N101">
+        <v>4</v>
+      </c>
+      <c r="O101">
+        <f t="shared" si="16"/>
+        <v>2.7E-6</v>
+      </c>
+      <c r="P101" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q101">
+        <v>10400</v>
+      </c>
+      <c r="R101">
+        <v>5</v>
+      </c>
+      <c r="S101" t="s">
+        <v>27</v>
+      </c>
+      <c r="T101">
+        <v>0.05</v>
+      </c>
+      <c r="U101">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="102" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A102" t="s">
+        <v>30</v>
+      </c>
+      <c r="B102">
+        <f t="shared" si="19"/>
+        <v>11</v>
+      </c>
+      <c r="C102">
+        <f t="shared" si="20"/>
+        <v>12100</v>
+      </c>
+      <c r="D102" t="s">
+        <v>9</v>
+      </c>
+      <c r="E102">
+        <v>1</v>
+      </c>
+      <c r="F102">
+        <v>100</v>
+      </c>
+      <c r="G102">
+        <v>2.4</v>
+      </c>
+      <c r="H102">
+        <v>4.8</v>
+      </c>
+      <c r="I102">
+        <v>2.1</v>
+      </c>
+      <c r="J102">
+        <v>30</v>
+      </c>
+      <c r="K102">
+        <v>50</v>
+      </c>
+      <c r="L102">
+        <v>2</v>
+      </c>
+      <c r="M102">
+        <v>1000</v>
+      </c>
+      <c r="N102">
+        <v>4</v>
+      </c>
+      <c r="O102">
+        <f t="shared" si="16"/>
+        <v>2.7E-6</v>
+      </c>
+      <c r="P102" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q102">
+        <v>10400</v>
+      </c>
+      <c r="R102">
+        <v>5</v>
+      </c>
+      <c r="S102" t="s">
+        <v>27</v>
+      </c>
+      <c r="T102">
+        <v>0.05</v>
+      </c>
+      <c r="U102">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="103" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A103" t="s">
+        <v>30</v>
+      </c>
+      <c r="B103">
+        <f t="shared" si="19"/>
+        <v>12</v>
+      </c>
+      <c r="C103">
+        <f t="shared" si="20"/>
+        <v>13300</v>
+      </c>
+      <c r="D103" t="s">
+        <v>9</v>
+      </c>
+      <c r="E103">
+        <v>1</v>
+      </c>
+      <c r="F103">
+        <v>100</v>
+      </c>
+      <c r="G103">
+        <v>2.4</v>
+      </c>
+      <c r="H103">
+        <v>4.8</v>
+      </c>
+      <c r="I103">
+        <v>2.1</v>
+      </c>
+      <c r="J103">
+        <v>30</v>
+      </c>
+      <c r="K103">
+        <v>50</v>
+      </c>
+      <c r="L103">
+        <v>2</v>
+      </c>
+      <c r="M103">
+        <v>1000</v>
+      </c>
+      <c r="N103">
+        <v>4</v>
+      </c>
+      <c r="O103">
+        <f t="shared" si="16"/>
+        <v>2.7E-6</v>
+      </c>
+      <c r="P103" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q103">
+        <v>10400</v>
+      </c>
+      <c r="R103">
+        <v>5</v>
+      </c>
+      <c r="S103" t="s">
+        <v>27</v>
+      </c>
+      <c r="T103">
+        <v>0.05</v>
+      </c>
+      <c r="U103">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="104" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A104" t="s">
+        <v>30</v>
+      </c>
+      <c r="B104">
+        <f t="shared" si="19"/>
+        <v>13</v>
+      </c>
+      <c r="C104">
+        <f t="shared" si="20"/>
+        <v>14500</v>
+      </c>
+      <c r="D104" t="s">
+        <v>9</v>
+      </c>
+      <c r="E104">
+        <v>1</v>
+      </c>
+      <c r="F104">
+        <v>100</v>
+      </c>
+      <c r="G104">
+        <v>2.4</v>
+      </c>
+      <c r="H104">
+        <v>4.8</v>
+      </c>
+      <c r="I104">
+        <v>2.1</v>
+      </c>
+      <c r="J104">
+        <v>30</v>
+      </c>
+      <c r="K104">
+        <v>50</v>
+      </c>
+      <c r="L104">
+        <v>2</v>
+      </c>
+      <c r="M104">
+        <v>1000</v>
+      </c>
+      <c r="N104">
+        <v>4</v>
+      </c>
+      <c r="O104">
+        <f t="shared" si="16"/>
+        <v>2.7E-6</v>
+      </c>
+      <c r="P104" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q104">
+        <v>10400</v>
+      </c>
+      <c r="R104">
+        <v>5</v>
+      </c>
+      <c r="S104" t="s">
+        <v>27</v>
+      </c>
+      <c r="T104">
+        <v>0.05</v>
+      </c>
+      <c r="U104">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="105" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A105" t="s">
+        <v>30</v>
+      </c>
+      <c r="B105">
+        <f t="shared" si="19"/>
+        <v>14</v>
+      </c>
+      <c r="C105">
+        <f t="shared" si="20"/>
+        <v>15700</v>
+      </c>
+      <c r="D105" t="s">
+        <v>9</v>
+      </c>
+      <c r="E105">
+        <v>1</v>
+      </c>
+      <c r="F105">
+        <v>100</v>
+      </c>
+      <c r="G105">
+        <v>2.4</v>
+      </c>
+      <c r="H105">
+        <v>4.8</v>
+      </c>
+      <c r="I105">
+        <v>2.1</v>
+      </c>
+      <c r="J105">
+        <v>30</v>
+      </c>
+      <c r="K105">
+        <v>50</v>
+      </c>
+      <c r="L105">
+        <v>2</v>
+      </c>
+      <c r="M105">
+        <v>1000</v>
+      </c>
+      <c r="N105">
+        <v>4</v>
+      </c>
+      <c r="O105">
+        <f t="shared" si="16"/>
+        <v>2.7E-6</v>
+      </c>
+      <c r="P105" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q105">
+        <v>10400</v>
+      </c>
+      <c r="R105">
+        <v>5</v>
+      </c>
+      <c r="S105" t="s">
+        <v>27</v>
+      </c>
+      <c r="T105">
+        <v>0.05</v>
+      </c>
+      <c r="U105">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="106" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A106" t="s">
+        <v>30</v>
+      </c>
+      <c r="B106">
+        <f t="shared" si="19"/>
+        <v>15</v>
+      </c>
+      <c r="C106">
+        <f t="shared" si="20"/>
+        <v>16900</v>
+      </c>
+      <c r="D106" t="s">
+        <v>9</v>
+      </c>
+      <c r="E106">
+        <v>1</v>
+      </c>
+      <c r="F106">
+        <v>100</v>
+      </c>
+      <c r="G106">
+        <v>2.4</v>
+      </c>
+      <c r="H106">
+        <v>4.8</v>
+      </c>
+      <c r="I106">
+        <v>2.1</v>
+      </c>
+      <c r="J106">
+        <v>30</v>
+      </c>
+      <c r="K106">
+        <v>50</v>
+      </c>
+      <c r="L106">
+        <v>2</v>
+      </c>
+      <c r="M106">
+        <v>1000</v>
+      </c>
+      <c r="N106">
+        <v>4</v>
+      </c>
+      <c r="O106">
+        <f t="shared" si="16"/>
+        <v>2.7E-6</v>
+      </c>
+      <c r="P106" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q106">
+        <v>10400</v>
+      </c>
+      <c r="R106">
+        <v>5</v>
+      </c>
+      <c r="S106" t="s">
+        <v>27</v>
+      </c>
+      <c r="T106">
+        <v>0.05</v>
+      </c>
+      <c r="U106">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="107" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A107" t="s">
+        <v>34</v>
+      </c>
+      <c r="B107">
+        <v>1</v>
+      </c>
+      <c r="C107">
+        <v>100</v>
+      </c>
+      <c r="D107" t="s">
+        <v>9</v>
+      </c>
+      <c r="E107">
+        <v>1</v>
+      </c>
+      <c r="F107">
+        <v>100</v>
+      </c>
+      <c r="G107">
+        <v>2.4</v>
+      </c>
+      <c r="H107">
+        <v>4.8</v>
+      </c>
+      <c r="I107">
+        <v>2.1</v>
+      </c>
+      <c r="J107">
+        <v>30</v>
+      </c>
+      <c r="K107">
+        <v>50</v>
+      </c>
+      <c r="L107">
+        <v>2</v>
+      </c>
+      <c r="M107">
+        <v>1000</v>
+      </c>
+      <c r="N107">
+        <v>4</v>
+      </c>
+      <c r="O107">
+        <f t="shared" si="16"/>
+        <v>2.7E-6</v>
+      </c>
+      <c r="P107" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q107">
+        <v>10400</v>
+      </c>
+      <c r="R107">
+        <v>5</v>
+      </c>
+      <c r="S107" t="s">
+        <v>27</v>
+      </c>
+      <c r="T107">
+        <v>0.05</v>
+      </c>
+      <c r="U107">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="108" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A108" t="s">
+        <v>34</v>
+      </c>
+      <c r="B108">
+        <f>B107+1</f>
+        <v>2</v>
+      </c>
+      <c r="C108">
+        <f>C107+1200</f>
+        <v>1300</v>
+      </c>
+      <c r="D108" t="s">
+        <v>9</v>
+      </c>
+      <c r="E108">
+        <v>1</v>
+      </c>
+      <c r="F108">
+        <v>100</v>
+      </c>
+      <c r="G108">
+        <v>2.4</v>
+      </c>
+      <c r="H108">
+        <v>4.8</v>
+      </c>
+      <c r="I108">
+        <v>2.1</v>
+      </c>
+      <c r="J108">
+        <v>30</v>
+      </c>
+      <c r="K108">
+        <v>50</v>
+      </c>
+      <c r="L108">
+        <v>2</v>
+      </c>
+      <c r="M108">
+        <v>1000</v>
+      </c>
+      <c r="N108">
+        <v>4</v>
+      </c>
+      <c r="O108">
+        <f t="shared" si="16"/>
+        <v>2.7E-6</v>
+      </c>
+      <c r="P108" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q108">
+        <v>10400</v>
+      </c>
+      <c r="R108">
+        <v>5</v>
+      </c>
+      <c r="S108" t="s">
+        <v>27</v>
+      </c>
+      <c r="T108">
+        <v>0.05</v>
+      </c>
+      <c r="U108">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="109" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A109" t="s">
+        <v>34</v>
+      </c>
+      <c r="B109">
+        <f t="shared" ref="B109:B128" si="21">B108+1</f>
+        <v>3</v>
+      </c>
+      <c r="C109">
+        <f t="shared" ref="C109:C128" si="22">C108+1200</f>
+        <v>2500</v>
+      </c>
+      <c r="D109" t="s">
+        <v>9</v>
+      </c>
+      <c r="E109">
+        <v>1</v>
+      </c>
+      <c r="F109">
+        <v>100</v>
+      </c>
+      <c r="G109">
+        <v>2.4</v>
+      </c>
+      <c r="H109">
+        <v>4.8</v>
+      </c>
+      <c r="I109">
+        <v>2.1</v>
+      </c>
+      <c r="J109">
+        <v>30</v>
+      </c>
+      <c r="K109">
+        <v>50</v>
+      </c>
+      <c r="L109">
+        <v>2</v>
+      </c>
+      <c r="M109">
+        <v>1000</v>
+      </c>
+      <c r="N109">
+        <v>4</v>
+      </c>
+      <c r="O109">
+        <f t="shared" si="16"/>
+        <v>2.7E-6</v>
+      </c>
+      <c r="P109" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q109">
+        <v>10400</v>
+      </c>
+      <c r="R109">
+        <v>5</v>
+      </c>
+      <c r="S109" t="s">
+        <v>27</v>
+      </c>
+      <c r="T109">
+        <v>0.05</v>
+      </c>
+      <c r="U109">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="110" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A110" t="s">
+        <v>34</v>
+      </c>
+      <c r="B110">
+        <f t="shared" si="21"/>
+        <v>4</v>
+      </c>
+      <c r="C110">
+        <f t="shared" si="22"/>
+        <v>3700</v>
+      </c>
+      <c r="D110" t="s">
+        <v>9</v>
+      </c>
+      <c r="E110">
+        <v>1</v>
+      </c>
+      <c r="F110">
+        <v>100</v>
+      </c>
+      <c r="G110">
+        <v>2.4</v>
+      </c>
+      <c r="H110">
+        <v>4.8</v>
+      </c>
+      <c r="I110">
+        <v>2.1</v>
+      </c>
+      <c r="J110">
+        <v>30</v>
+      </c>
+      <c r="K110">
+        <v>50</v>
+      </c>
+      <c r="L110">
+        <v>2</v>
+      </c>
+      <c r="M110">
+        <v>1000</v>
+      </c>
+      <c r="N110">
+        <v>4</v>
+      </c>
+      <c r="O110">
+        <f t="shared" si="16"/>
+        <v>2.7E-6</v>
+      </c>
+      <c r="P110" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q110">
+        <v>10400</v>
+      </c>
+      <c r="R110">
+        <v>5</v>
+      </c>
+      <c r="S110" t="s">
+        <v>27</v>
+      </c>
+      <c r="T110">
+        <v>0.05</v>
+      </c>
+      <c r="U110">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="111" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A111" t="s">
+        <v>34</v>
+      </c>
+      <c r="B111">
+        <f t="shared" si="21"/>
+        <v>5</v>
+      </c>
+      <c r="C111">
+        <f t="shared" si="22"/>
+        <v>4900</v>
+      </c>
+      <c r="D111" t="s">
+        <v>9</v>
+      </c>
+      <c r="E111">
+        <v>1</v>
+      </c>
+      <c r="F111">
+        <v>100</v>
+      </c>
+      <c r="G111">
+        <v>2.4</v>
+      </c>
+      <c r="H111">
+        <v>4.8</v>
+      </c>
+      <c r="I111">
+        <v>2.1</v>
+      </c>
+      <c r="J111">
+        <v>30</v>
+      </c>
+      <c r="K111">
+        <v>50</v>
+      </c>
+      <c r="L111">
+        <v>2</v>
+      </c>
+      <c r="M111">
+        <v>1000</v>
+      </c>
+      <c r="N111">
+        <v>4</v>
+      </c>
+      <c r="O111">
+        <f t="shared" si="16"/>
+        <v>2.7E-6</v>
+      </c>
+      <c r="P111" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q111">
+        <v>10400</v>
+      </c>
+      <c r="R111">
+        <v>5</v>
+      </c>
+      <c r="S111" t="s">
+        <v>27</v>
+      </c>
+      <c r="T111">
+        <v>0.05</v>
+      </c>
+      <c r="U111">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="112" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A112" t="s">
+        <v>34</v>
+      </c>
+      <c r="B112">
+        <f t="shared" si="21"/>
+        <v>6</v>
+      </c>
+      <c r="C112">
+        <f t="shared" si="22"/>
+        <v>6100</v>
+      </c>
+      <c r="D112" t="s">
+        <v>9</v>
+      </c>
+      <c r="E112">
+        <v>1</v>
+      </c>
+      <c r="F112">
+        <v>100</v>
+      </c>
+      <c r="G112">
+        <v>2.4</v>
+      </c>
+      <c r="H112">
+        <v>4.8</v>
+      </c>
+      <c r="I112">
+        <v>2.1</v>
+      </c>
+      <c r="J112">
+        <v>30</v>
+      </c>
+      <c r="K112">
+        <v>50</v>
+      </c>
+      <c r="L112">
+        <v>2</v>
+      </c>
+      <c r="M112">
+        <v>1000</v>
+      </c>
+      <c r="N112">
+        <v>4</v>
+      </c>
+      <c r="O112">
+        <f t="shared" si="16"/>
+        <v>2.7E-6</v>
+      </c>
+      <c r="P112" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q112">
+        <v>10400</v>
+      </c>
+      <c r="R112">
+        <v>5</v>
+      </c>
+      <c r="S112" t="s">
+        <v>27</v>
+      </c>
+      <c r="T112">
+        <v>0.05</v>
+      </c>
+      <c r="U112">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="113" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A113" t="s">
+        <v>34</v>
+      </c>
+      <c r="B113">
+        <f t="shared" si="21"/>
+        <v>7</v>
+      </c>
+      <c r="C113">
+        <f t="shared" si="22"/>
+        <v>7300</v>
+      </c>
+      <c r="D113" t="s">
+        <v>9</v>
+      </c>
+      <c r="E113">
+        <v>1</v>
+      </c>
+      <c r="F113">
+        <v>100</v>
+      </c>
+      <c r="G113">
+        <v>2.4</v>
+      </c>
+      <c r="H113">
+        <v>4.8</v>
+      </c>
+      <c r="I113">
+        <v>2.1</v>
+      </c>
+      <c r="J113">
+        <v>30</v>
+      </c>
+      <c r="K113">
+        <v>50</v>
+      </c>
+      <c r="L113">
+        <v>2</v>
+      </c>
+      <c r="M113">
+        <v>1000</v>
+      </c>
+      <c r="N113">
+        <v>4</v>
+      </c>
+      <c r="O113">
+        <f t="shared" si="16"/>
+        <v>2.7E-6</v>
+      </c>
+      <c r="P113" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q113">
+        <v>10400</v>
+      </c>
+      <c r="R113">
+        <v>5</v>
+      </c>
+      <c r="S113" t="s">
+        <v>27</v>
+      </c>
+      <c r="T113">
+        <v>0.05</v>
+      </c>
+      <c r="U113">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="114" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A114" t="s">
+        <v>34</v>
+      </c>
+      <c r="B114">
+        <f t="shared" si="21"/>
+        <v>8</v>
+      </c>
+      <c r="C114">
+        <f t="shared" si="22"/>
+        <v>8500</v>
+      </c>
+      <c r="D114" t="s">
+        <v>9</v>
+      </c>
+      <c r="E114">
+        <v>1</v>
+      </c>
+      <c r="F114">
+        <v>100</v>
+      </c>
+      <c r="G114">
+        <v>2.4</v>
+      </c>
+      <c r="H114">
+        <v>4.8</v>
+      </c>
+      <c r="I114">
+        <v>2.1</v>
+      </c>
+      <c r="J114">
+        <v>30</v>
+      </c>
+      <c r="K114">
+        <v>50</v>
+      </c>
+      <c r="L114">
+        <v>2</v>
+      </c>
+      <c r="M114">
+        <v>1000</v>
+      </c>
+      <c r="N114">
+        <v>4</v>
+      </c>
+      <c r="O114">
+        <f t="shared" si="16"/>
+        <v>2.7E-6</v>
+      </c>
+      <c r="P114" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q114">
+        <v>10400</v>
+      </c>
+      <c r="R114">
+        <v>5</v>
+      </c>
+      <c r="S114" t="s">
+        <v>27</v>
+      </c>
+      <c r="T114">
+        <v>0.05</v>
+      </c>
+      <c r="U114">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="115" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A115" t="s">
+        <v>34</v>
+      </c>
+      <c r="B115">
+        <f t="shared" si="21"/>
+        <v>9</v>
+      </c>
+      <c r="C115">
+        <f t="shared" si="22"/>
+        <v>9700</v>
+      </c>
+      <c r="D115" t="s">
+        <v>9</v>
+      </c>
+      <c r="E115">
+        <v>1</v>
+      </c>
+      <c r="F115">
+        <v>100</v>
+      </c>
+      <c r="G115">
+        <v>2.4</v>
+      </c>
+      <c r="H115">
+        <v>4.8</v>
+      </c>
+      <c r="I115">
+        <v>2.1</v>
+      </c>
+      <c r="J115">
+        <v>30</v>
+      </c>
+      <c r="K115">
+        <v>50</v>
+      </c>
+      <c r="L115">
+        <v>2</v>
+      </c>
+      <c r="M115">
+        <v>1000</v>
+      </c>
+      <c r="N115">
+        <v>4</v>
+      </c>
+      <c r="O115">
+        <f t="shared" si="16"/>
+        <v>2.7E-6</v>
+      </c>
+      <c r="P115" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q115">
+        <v>10400</v>
+      </c>
+      <c r="R115">
+        <v>5</v>
+      </c>
+      <c r="S115" t="s">
+        <v>27</v>
+      </c>
+      <c r="T115">
+        <v>0.05</v>
+      </c>
+      <c r="U115">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="116" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A116" t="s">
+        <v>34</v>
+      </c>
+      <c r="B116">
+        <f t="shared" si="21"/>
+        <v>10</v>
+      </c>
+      <c r="C116">
+        <f t="shared" si="22"/>
+        <v>10900</v>
+      </c>
+      <c r="D116" t="s">
+        <v>9</v>
+      </c>
+      <c r="E116">
+        <v>1</v>
+      </c>
+      <c r="F116">
+        <v>100</v>
+      </c>
+      <c r="G116">
+        <v>2.4</v>
+      </c>
+      <c r="H116">
+        <v>4.8</v>
+      </c>
+      <c r="I116">
+        <v>2.1</v>
+      </c>
+      <c r="J116">
+        <v>30</v>
+      </c>
+      <c r="K116">
+        <v>50</v>
+      </c>
+      <c r="L116">
+        <v>2</v>
+      </c>
+      <c r="M116">
+        <v>1000</v>
+      </c>
+      <c r="N116">
+        <v>4</v>
+      </c>
+      <c r="O116">
+        <f t="shared" si="16"/>
+        <v>2.7E-6</v>
+      </c>
+      <c r="P116" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q116">
+        <v>10400</v>
+      </c>
+      <c r="R116">
+        <v>5</v>
+      </c>
+      <c r="S116" t="s">
+        <v>27</v>
+      </c>
+      <c r="T116">
+        <v>0.05</v>
+      </c>
+      <c r="U116">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="117" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A117" t="s">
+        <v>34</v>
+      </c>
+      <c r="B117">
+        <f t="shared" si="21"/>
+        <v>11</v>
+      </c>
+      <c r="C117">
+        <f t="shared" si="22"/>
+        <v>12100</v>
+      </c>
+      <c r="D117" t="s">
+        <v>9</v>
+      </c>
+      <c r="E117">
+        <v>1</v>
+      </c>
+      <c r="F117">
+        <v>100</v>
+      </c>
+      <c r="G117">
+        <v>2.4</v>
+      </c>
+      <c r="H117">
+        <v>4.8</v>
+      </c>
+      <c r="I117">
+        <v>2.1</v>
+      </c>
+      <c r="J117">
+        <v>30</v>
+      </c>
+      <c r="K117">
+        <v>50</v>
+      </c>
+      <c r="L117">
+        <v>2</v>
+      </c>
+      <c r="M117">
+        <v>1000</v>
+      </c>
+      <c r="N117">
+        <v>4</v>
+      </c>
+      <c r="O117">
+        <f t="shared" si="16"/>
+        <v>2.7E-6</v>
+      </c>
+      <c r="P117" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q117">
+        <v>10400</v>
+      </c>
+      <c r="R117">
+        <v>5</v>
+      </c>
+      <c r="S117" t="s">
+        <v>27</v>
+      </c>
+      <c r="T117">
+        <v>0.05</v>
+      </c>
+      <c r="U117">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="118" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A118" t="s">
+        <v>34</v>
+      </c>
+      <c r="B118">
+        <f t="shared" si="21"/>
+        <v>12</v>
+      </c>
+      <c r="C118">
+        <f t="shared" si="22"/>
+        <v>13300</v>
+      </c>
+      <c r="D118" t="s">
+        <v>9</v>
+      </c>
+      <c r="E118">
+        <v>1</v>
+      </c>
+      <c r="F118">
+        <v>100</v>
+      </c>
+      <c r="G118">
+        <v>2.4</v>
+      </c>
+      <c r="H118">
+        <v>4.8</v>
+      </c>
+      <c r="I118">
+        <v>2.1</v>
+      </c>
+      <c r="J118">
+        <v>30</v>
+      </c>
+      <c r="K118">
+        <v>50</v>
+      </c>
+      <c r="L118">
+        <v>2</v>
+      </c>
+      <c r="M118">
+        <v>1000</v>
+      </c>
+      <c r="N118">
+        <v>4</v>
+      </c>
+      <c r="O118">
+        <f t="shared" si="16"/>
+        <v>2.7E-6</v>
+      </c>
+      <c r="P118" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q118">
+        <v>10400</v>
+      </c>
+      <c r="R118">
+        <v>5</v>
+      </c>
+      <c r="S118" t="s">
+        <v>27</v>
+      </c>
+      <c r="T118">
+        <v>0.05</v>
+      </c>
+      <c r="U118">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="119" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A119" t="s">
+        <v>34</v>
+      </c>
+      <c r="B119">
+        <f t="shared" si="21"/>
+        <v>13</v>
+      </c>
+      <c r="C119">
+        <f t="shared" si="22"/>
+        <v>14500</v>
+      </c>
+      <c r="D119" t="s">
+        <v>9</v>
+      </c>
+      <c r="E119">
+        <v>1</v>
+      </c>
+      <c r="F119">
+        <v>100</v>
+      </c>
+      <c r="G119">
+        <v>2.4</v>
+      </c>
+      <c r="H119">
+        <v>4.8</v>
+      </c>
+      <c r="I119">
+        <v>2.1</v>
+      </c>
+      <c r="J119">
+        <v>30</v>
+      </c>
+      <c r="K119">
+        <v>50</v>
+      </c>
+      <c r="L119">
+        <v>2</v>
+      </c>
+      <c r="M119">
+        <v>1000</v>
+      </c>
+      <c r="N119">
+        <v>4</v>
+      </c>
+      <c r="O119">
+        <f t="shared" si="16"/>
+        <v>2.7E-6</v>
+      </c>
+      <c r="P119" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q119">
+        <v>10400</v>
+      </c>
+      <c r="R119">
+        <v>5</v>
+      </c>
+      <c r="S119" t="s">
+        <v>27</v>
+      </c>
+      <c r="T119">
+        <v>0.05</v>
+      </c>
+      <c r="U119">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="120" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A120" t="s">
+        <v>34</v>
+      </c>
+      <c r="B120">
+        <f t="shared" si="21"/>
+        <v>14</v>
+      </c>
+      <c r="C120">
+        <f t="shared" si="22"/>
+        <v>15700</v>
+      </c>
+      <c r="D120" t="s">
+        <v>9</v>
+      </c>
+      <c r="E120">
+        <v>1</v>
+      </c>
+      <c r="F120">
+        <v>100</v>
+      </c>
+      <c r="G120">
+        <v>2.4</v>
+      </c>
+      <c r="H120">
+        <v>4.8</v>
+      </c>
+      <c r="I120">
+        <v>2.1</v>
+      </c>
+      <c r="J120">
+        <v>30</v>
+      </c>
+      <c r="K120">
+        <v>50</v>
+      </c>
+      <c r="L120">
+        <v>2</v>
+      </c>
+      <c r="M120">
+        <v>1000</v>
+      </c>
+      <c r="N120">
+        <v>4</v>
+      </c>
+      <c r="O120">
+        <f t="shared" si="16"/>
+        <v>2.7E-6</v>
+      </c>
+      <c r="P120" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q120">
+        <v>10400</v>
+      </c>
+      <c r="R120">
+        <v>5</v>
+      </c>
+      <c r="S120" t="s">
+        <v>27</v>
+      </c>
+      <c r="T120">
+        <v>0.05</v>
+      </c>
+      <c r="U120">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="121" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A121" t="s">
+        <v>34</v>
+      </c>
+      <c r="B121">
+        <f t="shared" si="21"/>
+        <v>15</v>
+      </c>
+      <c r="C121">
+        <f t="shared" si="22"/>
+        <v>16900</v>
+      </c>
+      <c r="D121" t="s">
+        <v>9</v>
+      </c>
+      <c r="E121">
+        <v>1</v>
+      </c>
+      <c r="F121">
+        <v>100</v>
+      </c>
+      <c r="G121">
+        <v>2.4</v>
+      </c>
+      <c r="H121">
+        <v>4.8</v>
+      </c>
+      <c r="I121">
+        <v>2.1</v>
+      </c>
+      <c r="J121">
+        <v>30</v>
+      </c>
+      <c r="K121">
+        <v>50</v>
+      </c>
+      <c r="L121">
+        <v>2</v>
+      </c>
+      <c r="M121">
+        <v>1000</v>
+      </c>
+      <c r="N121">
+        <v>4</v>
+      </c>
+      <c r="O121">
+        <f t="shared" si="16"/>
+        <v>2.7E-6</v>
+      </c>
+      <c r="P121" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q121">
+        <v>10400</v>
+      </c>
+      <c r="R121">
+        <v>5</v>
+      </c>
+      <c r="S121" t="s">
+        <v>27</v>
+      </c>
+      <c r="T121">
+        <v>0.05</v>
+      </c>
+      <c r="U121">
+        <v>110</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:A91"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Code off get_stim_start(). 7 WT, 4 KO.
</commit_message>
<xml_diff>
--- a/scripts/file_params.xlsx
+++ b/scripts/file_params.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="391" uniqueCount="38">
   <si>
     <t>filename</t>
   </si>
@@ -135,6 +135,15 @@
   </si>
   <si>
     <t>190205_a-synKO_2_AMPH_2.csv</t>
+  </si>
+  <si>
+    <t>190409_10mg-kg AMPH_1.csv</t>
+  </si>
+  <si>
+    <t>190409_10mg-kg AMPH_2.csv</t>
+  </si>
+  <si>
+    <t>190409_10mg-kg AMPH_3.csv</t>
   </si>
 </sst>
 </file>
@@ -473,13 +482,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V121"/>
+  <dimension ref="A1:V147"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C102" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="P134" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B110" sqref="B110"/>
+      <selection pane="bottomRight" activeCell="A141" sqref="A141"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4824,7 +4833,7 @@
         <v>28</v>
       </c>
       <c r="B64">
-        <f t="shared" ref="B64:B81" si="14">B63+1</f>
+        <f t="shared" ref="B64:B76" si="14">B63+1</f>
         <v>3</v>
       </c>
       <c r="C64">
@@ -5069,7 +5078,7 @@
         <v>4</v>
       </c>
       <c r="O67">
-        <f t="shared" ref="O67:O128" si="16">2.7*10^-6</f>
+        <f t="shared" ref="O67:O144" si="16">2.7*10^-6</f>
         <v>2.7E-6</v>
       </c>
       <c r="P67" t="b">
@@ -5842,11 +5851,11 @@
         <v>29</v>
       </c>
       <c r="B79">
-        <f t="shared" ref="B79:B95" si="17">B78+1</f>
+        <f t="shared" ref="B79:B91" si="17">B78+1</f>
         <v>3</v>
       </c>
       <c r="C79">
-        <f t="shared" ref="C79:C95" si="18">C78+1200</f>
+        <f t="shared" ref="C79:C91" si="18">C78+1200</f>
         <v>2500</v>
       </c>
       <c r="D79" t="s">
@@ -6863,11 +6872,11 @@
         <v>30</v>
       </c>
       <c r="B94">
-        <f t="shared" ref="B94:B111" si="19">B93+1</f>
+        <f t="shared" ref="B94:B106" si="19">B93+1</f>
         <v>3</v>
       </c>
       <c r="C94">
-        <f t="shared" ref="C94:C111" si="20">C93+1200</f>
+        <f t="shared" ref="C94:C106" si="20">C93+1200</f>
         <v>2500</v>
       </c>
       <c r="D94" t="s">
@@ -7881,11 +7890,11 @@
         <v>34</v>
       </c>
       <c r="B109">
-        <f t="shared" ref="B109:B128" si="21">B108+1</f>
+        <f t="shared" ref="B109:B121" si="21">B108+1</f>
         <v>3</v>
       </c>
       <c r="C109">
-        <f t="shared" ref="C109:C128" si="22">C108+1200</f>
+        <f t="shared" ref="C109:C121" si="22">C108+1200</f>
         <v>2500</v>
       </c>
       <c r="D109" t="s">
@@ -8757,6 +8766,1768 @@
         <v>0.05</v>
       </c>
       <c r="U121">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="122" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A122" t="s">
+        <v>35</v>
+      </c>
+      <c r="B122">
+        <v>1</v>
+      </c>
+      <c r="C122">
+        <v>100</v>
+      </c>
+      <c r="D122" t="s">
+        <v>8</v>
+      </c>
+      <c r="E122">
+        <v>0</v>
+      </c>
+      <c r="F122">
+        <v>100</v>
+      </c>
+      <c r="G122">
+        <v>2.4</v>
+      </c>
+      <c r="H122">
+        <v>4.8</v>
+      </c>
+      <c r="I122">
+        <v>2.1</v>
+      </c>
+      <c r="J122">
+        <v>30</v>
+      </c>
+      <c r="K122">
+        <v>50</v>
+      </c>
+      <c r="L122">
+        <v>2</v>
+      </c>
+      <c r="M122">
+        <v>1000</v>
+      </c>
+      <c r="N122">
+        <v>4</v>
+      </c>
+      <c r="O122">
+        <f t="shared" si="16"/>
+        <v>2.7E-6</v>
+      </c>
+      <c r="P122" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q122">
+        <v>10900</v>
+      </c>
+      <c r="R122">
+        <v>5</v>
+      </c>
+      <c r="S122" t="s">
+        <v>27</v>
+      </c>
+      <c r="T122">
+        <v>0.05</v>
+      </c>
+      <c r="U122">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="123" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A123" t="s">
+        <v>35</v>
+      </c>
+      <c r="B123">
+        <f>B122+1</f>
+        <v>2</v>
+      </c>
+      <c r="C123">
+        <f>C122+1200</f>
+        <v>1300</v>
+      </c>
+      <c r="D123" t="s">
+        <v>8</v>
+      </c>
+      <c r="E123">
+        <v>0</v>
+      </c>
+      <c r="F123">
+        <v>100</v>
+      </c>
+      <c r="G123">
+        <v>2.4</v>
+      </c>
+      <c r="H123">
+        <v>4.8</v>
+      </c>
+      <c r="I123">
+        <v>2.1</v>
+      </c>
+      <c r="J123">
+        <v>30</v>
+      </c>
+      <c r="K123">
+        <v>50</v>
+      </c>
+      <c r="L123">
+        <v>2</v>
+      </c>
+      <c r="M123">
+        <v>1000</v>
+      </c>
+      <c r="N123">
+        <v>4</v>
+      </c>
+      <c r="O123">
+        <f t="shared" si="16"/>
+        <v>2.7E-6</v>
+      </c>
+      <c r="P123" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q123">
+        <v>10900</v>
+      </c>
+      <c r="R123">
+        <v>5</v>
+      </c>
+      <c r="S123" t="s">
+        <v>27</v>
+      </c>
+      <c r="T123">
+        <v>0.05</v>
+      </c>
+      <c r="U123">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="124" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A124" t="s">
+        <v>35</v>
+      </c>
+      <c r="B124">
+        <f t="shared" ref="B124:B131" si="23">B123+1</f>
+        <v>3</v>
+      </c>
+      <c r="C124">
+        <f t="shared" ref="C124:C131" si="24">C123+1200</f>
+        <v>2500</v>
+      </c>
+      <c r="D124" t="s">
+        <v>8</v>
+      </c>
+      <c r="E124">
+        <v>0</v>
+      </c>
+      <c r="F124">
+        <v>100</v>
+      </c>
+      <c r="G124">
+        <v>2.4</v>
+      </c>
+      <c r="H124">
+        <v>4.8</v>
+      </c>
+      <c r="I124">
+        <v>2.1</v>
+      </c>
+      <c r="J124">
+        <v>30</v>
+      </c>
+      <c r="K124">
+        <v>50</v>
+      </c>
+      <c r="L124">
+        <v>2</v>
+      </c>
+      <c r="M124">
+        <v>1000</v>
+      </c>
+      <c r="N124">
+        <v>4</v>
+      </c>
+      <c r="O124">
+        <f t="shared" si="16"/>
+        <v>2.7E-6</v>
+      </c>
+      <c r="P124" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q124">
+        <v>10900</v>
+      </c>
+      <c r="R124">
+        <v>5</v>
+      </c>
+      <c r="S124" t="s">
+        <v>27</v>
+      </c>
+      <c r="T124">
+        <v>0.05</v>
+      </c>
+      <c r="U124">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="125" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A125" t="s">
+        <v>35</v>
+      </c>
+      <c r="B125">
+        <f t="shared" si="23"/>
+        <v>4</v>
+      </c>
+      <c r="C125">
+        <f t="shared" si="24"/>
+        <v>3700</v>
+      </c>
+      <c r="D125" t="s">
+        <v>8</v>
+      </c>
+      <c r="E125">
+        <v>1</v>
+      </c>
+      <c r="F125">
+        <v>100</v>
+      </c>
+      <c r="G125">
+        <v>2.4</v>
+      </c>
+      <c r="H125">
+        <v>4.8</v>
+      </c>
+      <c r="I125">
+        <v>2.1</v>
+      </c>
+      <c r="J125">
+        <v>30</v>
+      </c>
+      <c r="K125">
+        <v>50</v>
+      </c>
+      <c r="L125">
+        <v>2</v>
+      </c>
+      <c r="M125">
+        <v>1000</v>
+      </c>
+      <c r="N125">
+        <v>4</v>
+      </c>
+      <c r="O125">
+        <f t="shared" si="16"/>
+        <v>2.7E-6</v>
+      </c>
+      <c r="P125" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q125">
+        <v>10900</v>
+      </c>
+      <c r="R125">
+        <v>5</v>
+      </c>
+      <c r="S125" t="s">
+        <v>27</v>
+      </c>
+      <c r="T125">
+        <v>0.05</v>
+      </c>
+      <c r="U125">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="126" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A126" t="s">
+        <v>35</v>
+      </c>
+      <c r="B126">
+        <f t="shared" si="23"/>
+        <v>5</v>
+      </c>
+      <c r="C126">
+        <f t="shared" si="24"/>
+        <v>4900</v>
+      </c>
+      <c r="D126" t="s">
+        <v>8</v>
+      </c>
+      <c r="E126">
+        <v>1</v>
+      </c>
+      <c r="F126">
+        <v>100</v>
+      </c>
+      <c r="G126">
+        <v>2.4</v>
+      </c>
+      <c r="H126">
+        <v>4.8</v>
+      </c>
+      <c r="I126">
+        <v>2.1</v>
+      </c>
+      <c r="J126">
+        <v>30</v>
+      </c>
+      <c r="K126">
+        <v>50</v>
+      </c>
+      <c r="L126">
+        <v>2</v>
+      </c>
+      <c r="M126">
+        <v>1000</v>
+      </c>
+      <c r="N126">
+        <v>4</v>
+      </c>
+      <c r="O126">
+        <f t="shared" si="16"/>
+        <v>2.7E-6</v>
+      </c>
+      <c r="P126" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q126">
+        <v>10900</v>
+      </c>
+      <c r="R126">
+        <v>5</v>
+      </c>
+      <c r="S126" t="s">
+        <v>27</v>
+      </c>
+      <c r="T126">
+        <v>0.05</v>
+      </c>
+      <c r="U126">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="127" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A127" t="s">
+        <v>35</v>
+      </c>
+      <c r="B127">
+        <f t="shared" si="23"/>
+        <v>6</v>
+      </c>
+      <c r="C127">
+        <f t="shared" si="24"/>
+        <v>6100</v>
+      </c>
+      <c r="D127" t="s">
+        <v>8</v>
+      </c>
+      <c r="E127">
+        <v>1</v>
+      </c>
+      <c r="F127">
+        <v>100</v>
+      </c>
+      <c r="G127">
+        <v>2.4</v>
+      </c>
+      <c r="H127">
+        <v>4.8</v>
+      </c>
+      <c r="I127">
+        <v>2.1</v>
+      </c>
+      <c r="J127">
+        <v>30</v>
+      </c>
+      <c r="K127">
+        <v>50</v>
+      </c>
+      <c r="L127">
+        <v>2</v>
+      </c>
+      <c r="M127">
+        <v>1000</v>
+      </c>
+      <c r="N127">
+        <v>4</v>
+      </c>
+      <c r="O127">
+        <f t="shared" si="16"/>
+        <v>2.7E-6</v>
+      </c>
+      <c r="P127" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q127">
+        <v>10900</v>
+      </c>
+      <c r="R127">
+        <v>5</v>
+      </c>
+      <c r="S127" t="s">
+        <v>27</v>
+      </c>
+      <c r="T127">
+        <v>0.05</v>
+      </c>
+      <c r="U127">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="128" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A128" t="s">
+        <v>35</v>
+      </c>
+      <c r="B128">
+        <f t="shared" si="23"/>
+        <v>7</v>
+      </c>
+      <c r="C128">
+        <f t="shared" si="24"/>
+        <v>7300</v>
+      </c>
+      <c r="D128" t="s">
+        <v>8</v>
+      </c>
+      <c r="E128">
+        <v>1</v>
+      </c>
+      <c r="F128">
+        <v>100</v>
+      </c>
+      <c r="G128">
+        <v>2.4</v>
+      </c>
+      <c r="H128">
+        <v>4.8</v>
+      </c>
+      <c r="I128">
+        <v>2.1</v>
+      </c>
+      <c r="J128">
+        <v>30</v>
+      </c>
+      <c r="K128">
+        <v>50</v>
+      </c>
+      <c r="L128">
+        <v>2</v>
+      </c>
+      <c r="M128">
+        <v>1000</v>
+      </c>
+      <c r="N128">
+        <v>4</v>
+      </c>
+      <c r="O128">
+        <f t="shared" si="16"/>
+        <v>2.7E-6</v>
+      </c>
+      <c r="P128" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q128">
+        <v>10900</v>
+      </c>
+      <c r="R128">
+        <v>5</v>
+      </c>
+      <c r="S128" t="s">
+        <v>27</v>
+      </c>
+      <c r="T128">
+        <v>0.05</v>
+      </c>
+      <c r="U128">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="129" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A129" t="s">
+        <v>35</v>
+      </c>
+      <c r="B129">
+        <f t="shared" si="23"/>
+        <v>8</v>
+      </c>
+      <c r="C129">
+        <f t="shared" si="24"/>
+        <v>8500</v>
+      </c>
+      <c r="D129" t="s">
+        <v>8</v>
+      </c>
+      <c r="E129">
+        <v>1</v>
+      </c>
+      <c r="F129">
+        <v>100</v>
+      </c>
+      <c r="G129">
+        <v>2.4</v>
+      </c>
+      <c r="H129">
+        <v>4.8</v>
+      </c>
+      <c r="I129">
+        <v>2.1</v>
+      </c>
+      <c r="J129">
+        <v>30</v>
+      </c>
+      <c r="K129">
+        <v>50</v>
+      </c>
+      <c r="L129">
+        <v>2</v>
+      </c>
+      <c r="M129">
+        <v>1000</v>
+      </c>
+      <c r="N129">
+        <v>4</v>
+      </c>
+      <c r="O129">
+        <f t="shared" si="16"/>
+        <v>2.7E-6</v>
+      </c>
+      <c r="P129" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q129">
+        <v>10900</v>
+      </c>
+      <c r="R129">
+        <v>5</v>
+      </c>
+      <c r="S129" t="s">
+        <v>27</v>
+      </c>
+      <c r="T129">
+        <v>0.05</v>
+      </c>
+      <c r="U129">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="130" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A130" t="s">
+        <v>35</v>
+      </c>
+      <c r="B130">
+        <f t="shared" si="23"/>
+        <v>9</v>
+      </c>
+      <c r="C130">
+        <f t="shared" si="24"/>
+        <v>9700</v>
+      </c>
+      <c r="D130" t="s">
+        <v>8</v>
+      </c>
+      <c r="E130">
+        <v>1</v>
+      </c>
+      <c r="F130">
+        <v>100</v>
+      </c>
+      <c r="G130">
+        <v>2.4</v>
+      </c>
+      <c r="H130">
+        <v>4.8</v>
+      </c>
+      <c r="I130">
+        <v>2.1</v>
+      </c>
+      <c r="J130">
+        <v>30</v>
+      </c>
+      <c r="K130">
+        <v>50</v>
+      </c>
+      <c r="L130">
+        <v>2</v>
+      </c>
+      <c r="M130">
+        <v>1000</v>
+      </c>
+      <c r="N130">
+        <v>4</v>
+      </c>
+      <c r="O130">
+        <f t="shared" si="16"/>
+        <v>2.7E-6</v>
+      </c>
+      <c r="P130" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q130">
+        <v>10900</v>
+      </c>
+      <c r="R130">
+        <v>5</v>
+      </c>
+      <c r="S130" t="s">
+        <v>27</v>
+      </c>
+      <c r="T130">
+        <v>0.05</v>
+      </c>
+      <c r="U130">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="131" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A131" t="s">
+        <v>35</v>
+      </c>
+      <c r="B131">
+        <f t="shared" si="23"/>
+        <v>10</v>
+      </c>
+      <c r="C131">
+        <f t="shared" si="24"/>
+        <v>10900</v>
+      </c>
+      <c r="D131" t="s">
+        <v>8</v>
+      </c>
+      <c r="E131">
+        <v>1</v>
+      </c>
+      <c r="F131">
+        <v>100</v>
+      </c>
+      <c r="G131">
+        <v>2.4</v>
+      </c>
+      <c r="H131">
+        <v>4.8</v>
+      </c>
+      <c r="I131">
+        <v>2.1</v>
+      </c>
+      <c r="J131">
+        <v>30</v>
+      </c>
+      <c r="K131">
+        <v>50</v>
+      </c>
+      <c r="L131">
+        <v>2</v>
+      </c>
+      <c r="M131">
+        <v>1000</v>
+      </c>
+      <c r="N131">
+        <v>4</v>
+      </c>
+      <c r="O131">
+        <f t="shared" si="16"/>
+        <v>2.7E-6</v>
+      </c>
+      <c r="P131" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q131">
+        <v>10900</v>
+      </c>
+      <c r="R131">
+        <v>5</v>
+      </c>
+      <c r="S131" t="s">
+        <v>27</v>
+      </c>
+      <c r="T131">
+        <v>0.05</v>
+      </c>
+      <c r="U131">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="132" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A132" t="s">
+        <v>36</v>
+      </c>
+      <c r="B132">
+        <v>1</v>
+      </c>
+      <c r="C132">
+        <v>100</v>
+      </c>
+      <c r="D132" t="s">
+        <v>8</v>
+      </c>
+      <c r="E132">
+        <v>1</v>
+      </c>
+      <c r="F132">
+        <v>100</v>
+      </c>
+      <c r="G132">
+        <v>2.4</v>
+      </c>
+      <c r="H132">
+        <v>4.8</v>
+      </c>
+      <c r="I132">
+        <v>2.1</v>
+      </c>
+      <c r="J132">
+        <v>30</v>
+      </c>
+      <c r="K132">
+        <v>50</v>
+      </c>
+      <c r="L132">
+        <v>2</v>
+      </c>
+      <c r="M132">
+        <v>1000</v>
+      </c>
+      <c r="N132">
+        <v>4</v>
+      </c>
+      <c r="O132">
+        <f t="shared" si="16"/>
+        <v>2.7E-6</v>
+      </c>
+      <c r="P132" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q132">
+        <v>10900</v>
+      </c>
+      <c r="R132">
+        <v>5</v>
+      </c>
+      <c r="S132" t="s">
+        <v>27</v>
+      </c>
+      <c r="T132">
+        <v>0.05</v>
+      </c>
+      <c r="U132">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="133" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A133" t="s">
+        <v>36</v>
+      </c>
+      <c r="B133">
+        <f>B132+1</f>
+        <v>2</v>
+      </c>
+      <c r="C133">
+        <f>C132+1200</f>
+        <v>1300</v>
+      </c>
+      <c r="D133" t="s">
+        <v>8</v>
+      </c>
+      <c r="E133">
+        <v>1</v>
+      </c>
+      <c r="F133">
+        <v>100</v>
+      </c>
+      <c r="G133">
+        <v>2.4</v>
+      </c>
+      <c r="H133">
+        <v>4.8</v>
+      </c>
+      <c r="I133">
+        <v>2.1</v>
+      </c>
+      <c r="J133">
+        <v>30</v>
+      </c>
+      <c r="K133">
+        <v>50</v>
+      </c>
+      <c r="L133">
+        <v>2</v>
+      </c>
+      <c r="M133">
+        <v>1000</v>
+      </c>
+      <c r="N133">
+        <v>4</v>
+      </c>
+      <c r="O133">
+        <f t="shared" si="16"/>
+        <v>2.7E-6</v>
+      </c>
+      <c r="P133" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q133">
+        <v>10900</v>
+      </c>
+      <c r="R133">
+        <v>5</v>
+      </c>
+      <c r="S133" t="s">
+        <v>27</v>
+      </c>
+      <c r="T133">
+        <v>0.05</v>
+      </c>
+      <c r="U133">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="134" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A134" t="s">
+        <v>36</v>
+      </c>
+      <c r="B134">
+        <f t="shared" ref="B134:B141" si="25">B133+1</f>
+        <v>3</v>
+      </c>
+      <c r="C134">
+        <f t="shared" ref="C134:C141" si="26">C133+1200</f>
+        <v>2500</v>
+      </c>
+      <c r="D134" t="s">
+        <v>8</v>
+      </c>
+      <c r="E134">
+        <v>1</v>
+      </c>
+      <c r="F134">
+        <v>100</v>
+      </c>
+      <c r="G134">
+        <v>2.4</v>
+      </c>
+      <c r="H134">
+        <v>4.8</v>
+      </c>
+      <c r="I134">
+        <v>2.1</v>
+      </c>
+      <c r="J134">
+        <v>30</v>
+      </c>
+      <c r="K134">
+        <v>50</v>
+      </c>
+      <c r="L134">
+        <v>2</v>
+      </c>
+      <c r="M134">
+        <v>1000</v>
+      </c>
+      <c r="N134">
+        <v>4</v>
+      </c>
+      <c r="O134">
+        <f t="shared" si="16"/>
+        <v>2.7E-6</v>
+      </c>
+      <c r="P134" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q134">
+        <v>10900</v>
+      </c>
+      <c r="R134">
+        <v>5</v>
+      </c>
+      <c r="S134" t="s">
+        <v>27</v>
+      </c>
+      <c r="T134">
+        <v>0.05</v>
+      </c>
+      <c r="U134">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="135" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A135" t="s">
+        <v>36</v>
+      </c>
+      <c r="B135">
+        <f t="shared" si="25"/>
+        <v>4</v>
+      </c>
+      <c r="C135">
+        <f t="shared" si="26"/>
+        <v>3700</v>
+      </c>
+      <c r="D135" t="s">
+        <v>8</v>
+      </c>
+      <c r="E135">
+        <v>1</v>
+      </c>
+      <c r="F135">
+        <v>100</v>
+      </c>
+      <c r="G135">
+        <v>2.4</v>
+      </c>
+      <c r="H135">
+        <v>4.8</v>
+      </c>
+      <c r="I135">
+        <v>2.1</v>
+      </c>
+      <c r="J135">
+        <v>30</v>
+      </c>
+      <c r="K135">
+        <v>50</v>
+      </c>
+      <c r="L135">
+        <v>2</v>
+      </c>
+      <c r="M135">
+        <v>1000</v>
+      </c>
+      <c r="N135">
+        <v>4</v>
+      </c>
+      <c r="O135">
+        <f t="shared" si="16"/>
+        <v>2.7E-6</v>
+      </c>
+      <c r="P135" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q135">
+        <v>10900</v>
+      </c>
+      <c r="R135">
+        <v>5</v>
+      </c>
+      <c r="S135" t="s">
+        <v>27</v>
+      </c>
+      <c r="T135">
+        <v>0.05</v>
+      </c>
+      <c r="U135">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="136" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A136" t="s">
+        <v>36</v>
+      </c>
+      <c r="B136">
+        <f t="shared" si="25"/>
+        <v>5</v>
+      </c>
+      <c r="C136">
+        <f t="shared" si="26"/>
+        <v>4900</v>
+      </c>
+      <c r="D136" t="s">
+        <v>8</v>
+      </c>
+      <c r="E136">
+        <v>1</v>
+      </c>
+      <c r="F136">
+        <v>100</v>
+      </c>
+      <c r="G136">
+        <v>2.4</v>
+      </c>
+      <c r="H136">
+        <v>4.8</v>
+      </c>
+      <c r="I136">
+        <v>2.1</v>
+      </c>
+      <c r="J136">
+        <v>30</v>
+      </c>
+      <c r="K136">
+        <v>50</v>
+      </c>
+      <c r="L136">
+        <v>2</v>
+      </c>
+      <c r="M136">
+        <v>1000</v>
+      </c>
+      <c r="N136">
+        <v>4</v>
+      </c>
+      <c r="O136">
+        <f t="shared" si="16"/>
+        <v>2.7E-6</v>
+      </c>
+      <c r="P136" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q136">
+        <v>10900</v>
+      </c>
+      <c r="R136">
+        <v>5</v>
+      </c>
+      <c r="S136" t="s">
+        <v>27</v>
+      </c>
+      <c r="T136">
+        <v>0.05</v>
+      </c>
+      <c r="U136">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="137" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A137" t="s">
+        <v>36</v>
+      </c>
+      <c r="B137">
+        <f t="shared" si="25"/>
+        <v>6</v>
+      </c>
+      <c r="C137">
+        <f t="shared" si="26"/>
+        <v>6100</v>
+      </c>
+      <c r="D137" t="s">
+        <v>8</v>
+      </c>
+      <c r="E137">
+        <v>1</v>
+      </c>
+      <c r="F137">
+        <v>100</v>
+      </c>
+      <c r="G137">
+        <v>2.4</v>
+      </c>
+      <c r="H137">
+        <v>4.8</v>
+      </c>
+      <c r="I137">
+        <v>2.1</v>
+      </c>
+      <c r="J137">
+        <v>30</v>
+      </c>
+      <c r="K137">
+        <v>50</v>
+      </c>
+      <c r="L137">
+        <v>2</v>
+      </c>
+      <c r="M137">
+        <v>1000</v>
+      </c>
+      <c r="N137">
+        <v>4</v>
+      </c>
+      <c r="O137">
+        <f t="shared" si="16"/>
+        <v>2.7E-6</v>
+      </c>
+      <c r="P137" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q137">
+        <v>10900</v>
+      </c>
+      <c r="R137">
+        <v>5</v>
+      </c>
+      <c r="S137" t="s">
+        <v>27</v>
+      </c>
+      <c r="T137">
+        <v>0.05</v>
+      </c>
+      <c r="U137">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="138" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A138" t="s">
+        <v>36</v>
+      </c>
+      <c r="B138">
+        <f t="shared" si="25"/>
+        <v>7</v>
+      </c>
+      <c r="C138">
+        <f t="shared" si="26"/>
+        <v>7300</v>
+      </c>
+      <c r="D138" t="s">
+        <v>8</v>
+      </c>
+      <c r="E138">
+        <v>1</v>
+      </c>
+      <c r="F138">
+        <v>100</v>
+      </c>
+      <c r="G138">
+        <v>2.4</v>
+      </c>
+      <c r="H138">
+        <v>4.8</v>
+      </c>
+      <c r="I138">
+        <v>2.1</v>
+      </c>
+      <c r="J138">
+        <v>30</v>
+      </c>
+      <c r="K138">
+        <v>50</v>
+      </c>
+      <c r="L138">
+        <v>2</v>
+      </c>
+      <c r="M138">
+        <v>1000</v>
+      </c>
+      <c r="N138">
+        <v>4</v>
+      </c>
+      <c r="O138">
+        <f t="shared" si="16"/>
+        <v>2.7E-6</v>
+      </c>
+      <c r="P138" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q138">
+        <v>10900</v>
+      </c>
+      <c r="R138">
+        <v>5</v>
+      </c>
+      <c r="S138" t="s">
+        <v>27</v>
+      </c>
+      <c r="T138">
+        <v>0.05</v>
+      </c>
+      <c r="U138">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="139" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A139" t="s">
+        <v>36</v>
+      </c>
+      <c r="B139">
+        <f t="shared" si="25"/>
+        <v>8</v>
+      </c>
+      <c r="C139">
+        <f t="shared" si="26"/>
+        <v>8500</v>
+      </c>
+      <c r="D139" t="s">
+        <v>8</v>
+      </c>
+      <c r="E139">
+        <v>1</v>
+      </c>
+      <c r="F139">
+        <v>100</v>
+      </c>
+      <c r="G139">
+        <v>2.4</v>
+      </c>
+      <c r="H139">
+        <v>4.8</v>
+      </c>
+      <c r="I139">
+        <v>2.1</v>
+      </c>
+      <c r="J139">
+        <v>30</v>
+      </c>
+      <c r="K139">
+        <v>50</v>
+      </c>
+      <c r="L139">
+        <v>2</v>
+      </c>
+      <c r="M139">
+        <v>1000</v>
+      </c>
+      <c r="N139">
+        <v>4</v>
+      </c>
+      <c r="O139">
+        <f t="shared" si="16"/>
+        <v>2.7E-6</v>
+      </c>
+      <c r="P139" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q139">
+        <v>10900</v>
+      </c>
+      <c r="R139">
+        <v>5</v>
+      </c>
+      <c r="S139" t="s">
+        <v>27</v>
+      </c>
+      <c r="T139">
+        <v>0.05</v>
+      </c>
+      <c r="U139">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="140" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A140" t="s">
+        <v>36</v>
+      </c>
+      <c r="B140">
+        <f t="shared" si="25"/>
+        <v>9</v>
+      </c>
+      <c r="C140">
+        <f t="shared" si="26"/>
+        <v>9700</v>
+      </c>
+      <c r="D140" t="s">
+        <v>8</v>
+      </c>
+      <c r="E140">
+        <v>1</v>
+      </c>
+      <c r="F140">
+        <v>100</v>
+      </c>
+      <c r="G140">
+        <v>2.4</v>
+      </c>
+      <c r="H140">
+        <v>4.8</v>
+      </c>
+      <c r="I140">
+        <v>2.1</v>
+      </c>
+      <c r="J140">
+        <v>30</v>
+      </c>
+      <c r="K140">
+        <v>50</v>
+      </c>
+      <c r="L140">
+        <v>2</v>
+      </c>
+      <c r="M140">
+        <v>1000</v>
+      </c>
+      <c r="N140">
+        <v>4</v>
+      </c>
+      <c r="O140">
+        <f t="shared" si="16"/>
+        <v>2.7E-6</v>
+      </c>
+      <c r="P140" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q140">
+        <v>10900</v>
+      </c>
+      <c r="R140">
+        <v>5</v>
+      </c>
+      <c r="S140" t="s">
+        <v>27</v>
+      </c>
+      <c r="T140">
+        <v>0.05</v>
+      </c>
+      <c r="U140">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="141" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A141" t="s">
+        <v>36</v>
+      </c>
+      <c r="B141">
+        <f t="shared" si="25"/>
+        <v>10</v>
+      </c>
+      <c r="C141">
+        <f t="shared" si="26"/>
+        <v>10900</v>
+      </c>
+      <c r="D141" t="s">
+        <v>8</v>
+      </c>
+      <c r="E141">
+        <v>1</v>
+      </c>
+      <c r="F141">
+        <v>100</v>
+      </c>
+      <c r="G141">
+        <v>2.4</v>
+      </c>
+      <c r="H141">
+        <v>4.8</v>
+      </c>
+      <c r="I141">
+        <v>2.1</v>
+      </c>
+      <c r="J141">
+        <v>30</v>
+      </c>
+      <c r="K141">
+        <v>50</v>
+      </c>
+      <c r="L141">
+        <v>2</v>
+      </c>
+      <c r="M141">
+        <v>1000</v>
+      </c>
+      <c r="N141">
+        <v>4</v>
+      </c>
+      <c r="O141">
+        <f t="shared" si="16"/>
+        <v>2.7E-6</v>
+      </c>
+      <c r="P141" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q141">
+        <v>10900</v>
+      </c>
+      <c r="R141">
+        <v>5</v>
+      </c>
+      <c r="S141" t="s">
+        <v>27</v>
+      </c>
+      <c r="T141">
+        <v>0.05</v>
+      </c>
+      <c r="U141">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="142" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A142" t="s">
+        <v>37</v>
+      </c>
+      <c r="B142">
+        <v>1</v>
+      </c>
+      <c r="C142">
+        <v>100</v>
+      </c>
+      <c r="D142" t="s">
+        <v>8</v>
+      </c>
+      <c r="E142">
+        <v>1</v>
+      </c>
+      <c r="F142">
+        <v>100</v>
+      </c>
+      <c r="G142">
+        <v>2.4</v>
+      </c>
+      <c r="H142">
+        <v>4.8</v>
+      </c>
+      <c r="I142">
+        <v>2.1</v>
+      </c>
+      <c r="J142">
+        <v>30</v>
+      </c>
+      <c r="K142">
+        <v>50</v>
+      </c>
+      <c r="L142">
+        <v>2</v>
+      </c>
+      <c r="M142">
+        <v>1000</v>
+      </c>
+      <c r="N142">
+        <v>4</v>
+      </c>
+      <c r="O142">
+        <f t="shared" si="16"/>
+        <v>2.7E-6</v>
+      </c>
+      <c r="P142" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q142">
+        <v>10900</v>
+      </c>
+      <c r="R142">
+        <v>5</v>
+      </c>
+      <c r="S142" t="s">
+        <v>27</v>
+      </c>
+      <c r="T142">
+        <v>0.05</v>
+      </c>
+      <c r="U142">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="143" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A143" t="s">
+        <v>37</v>
+      </c>
+      <c r="B143">
+        <f>B142+1</f>
+        <v>2</v>
+      </c>
+      <c r="C143">
+        <f>C142+1200</f>
+        <v>1300</v>
+      </c>
+      <c r="D143" t="s">
+        <v>8</v>
+      </c>
+      <c r="E143">
+        <v>1</v>
+      </c>
+      <c r="F143">
+        <v>100</v>
+      </c>
+      <c r="G143">
+        <v>2.4</v>
+      </c>
+      <c r="H143">
+        <v>4.8</v>
+      </c>
+      <c r="I143">
+        <v>2.1</v>
+      </c>
+      <c r="J143">
+        <v>30</v>
+      </c>
+      <c r="K143">
+        <v>50</v>
+      </c>
+      <c r="L143">
+        <v>2</v>
+      </c>
+      <c r="M143">
+        <v>1000</v>
+      </c>
+      <c r="N143">
+        <v>4</v>
+      </c>
+      <c r="O143">
+        <f t="shared" si="16"/>
+        <v>2.7E-6</v>
+      </c>
+      <c r="P143" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q143">
+        <v>10900</v>
+      </c>
+      <c r="R143">
+        <v>5</v>
+      </c>
+      <c r="S143" t="s">
+        <v>27</v>
+      </c>
+      <c r="T143">
+        <v>0.05</v>
+      </c>
+      <c r="U143">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="144" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A144" t="s">
+        <v>37</v>
+      </c>
+      <c r="B144">
+        <f t="shared" ref="B144:B153" si="27">B143+1</f>
+        <v>3</v>
+      </c>
+      <c r="C144">
+        <f t="shared" ref="C144:C153" si="28">C143+1200</f>
+        <v>2500</v>
+      </c>
+      <c r="D144" t="s">
+        <v>8</v>
+      </c>
+      <c r="E144">
+        <v>1</v>
+      </c>
+      <c r="F144">
+        <v>100</v>
+      </c>
+      <c r="G144">
+        <v>2.4</v>
+      </c>
+      <c r="H144">
+        <v>4.8</v>
+      </c>
+      <c r="I144">
+        <v>2.1</v>
+      </c>
+      <c r="J144">
+        <v>30</v>
+      </c>
+      <c r="K144">
+        <v>50</v>
+      </c>
+      <c r="L144">
+        <v>2</v>
+      </c>
+      <c r="M144">
+        <v>1000</v>
+      </c>
+      <c r="N144">
+        <v>4</v>
+      </c>
+      <c r="O144">
+        <f t="shared" si="16"/>
+        <v>2.7E-6</v>
+      </c>
+      <c r="P144" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q144">
+        <v>10900</v>
+      </c>
+      <c r="R144">
+        <v>5</v>
+      </c>
+      <c r="S144" t="s">
+        <v>27</v>
+      </c>
+      <c r="T144">
+        <v>0.05</v>
+      </c>
+      <c r="U144">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="145" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A145" t="s">
+        <v>37</v>
+      </c>
+      <c r="B145">
+        <f t="shared" si="27"/>
+        <v>4</v>
+      </c>
+      <c r="C145">
+        <f t="shared" si="28"/>
+        <v>3700</v>
+      </c>
+      <c r="D145" t="s">
+        <v>8</v>
+      </c>
+      <c r="E145">
+        <v>1</v>
+      </c>
+      <c r="F145">
+        <v>100</v>
+      </c>
+      <c r="G145">
+        <v>2.4</v>
+      </c>
+      <c r="H145">
+        <v>4.8</v>
+      </c>
+      <c r="I145">
+        <v>2.1</v>
+      </c>
+      <c r="J145">
+        <v>30</v>
+      </c>
+      <c r="K145">
+        <v>50</v>
+      </c>
+      <c r="L145">
+        <v>2</v>
+      </c>
+      <c r="M145">
+        <v>1000</v>
+      </c>
+      <c r="N145">
+        <v>4</v>
+      </c>
+      <c r="O145">
+        <f t="shared" ref="O145:O153" si="29">2.7*10^-6</f>
+        <v>2.7E-6</v>
+      </c>
+      <c r="P145" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q145">
+        <v>10900</v>
+      </c>
+      <c r="R145">
+        <v>5</v>
+      </c>
+      <c r="S145" t="s">
+        <v>27</v>
+      </c>
+      <c r="T145">
+        <v>0.05</v>
+      </c>
+      <c r="U145">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="146" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A146" t="s">
+        <v>37</v>
+      </c>
+      <c r="B146">
+        <f t="shared" si="27"/>
+        <v>5</v>
+      </c>
+      <c r="C146">
+        <f t="shared" si="28"/>
+        <v>4900</v>
+      </c>
+      <c r="D146" t="s">
+        <v>8</v>
+      </c>
+      <c r="E146">
+        <v>1</v>
+      </c>
+      <c r="F146">
+        <v>100</v>
+      </c>
+      <c r="G146">
+        <v>2.4</v>
+      </c>
+      <c r="H146">
+        <v>4.8</v>
+      </c>
+      <c r="I146">
+        <v>2.1</v>
+      </c>
+      <c r="J146">
+        <v>30</v>
+      </c>
+      <c r="K146">
+        <v>50</v>
+      </c>
+      <c r="L146">
+        <v>2</v>
+      </c>
+      <c r="M146">
+        <v>1000</v>
+      </c>
+      <c r="N146">
+        <v>4</v>
+      </c>
+      <c r="O146">
+        <f t="shared" si="29"/>
+        <v>2.7E-6</v>
+      </c>
+      <c r="P146" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q146">
+        <v>10900</v>
+      </c>
+      <c r="R146">
+        <v>5</v>
+      </c>
+      <c r="S146" t="s">
+        <v>27</v>
+      </c>
+      <c r="T146">
+        <v>0.05</v>
+      </c>
+      <c r="U146">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="147" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A147" t="s">
+        <v>37</v>
+      </c>
+      <c r="B147">
+        <f t="shared" si="27"/>
+        <v>6</v>
+      </c>
+      <c r="C147">
+        <f t="shared" si="28"/>
+        <v>6100</v>
+      </c>
+      <c r="D147" t="s">
+        <v>8</v>
+      </c>
+      <c r="E147">
+        <v>1</v>
+      </c>
+      <c r="F147">
+        <v>100</v>
+      </c>
+      <c r="G147">
+        <v>2.4</v>
+      </c>
+      <c r="H147">
+        <v>4.8</v>
+      </c>
+      <c r="I147">
+        <v>2.1</v>
+      </c>
+      <c r="J147">
+        <v>30</v>
+      </c>
+      <c r="K147">
+        <v>50</v>
+      </c>
+      <c r="L147">
+        <v>2</v>
+      </c>
+      <c r="M147">
+        <v>1000</v>
+      </c>
+      <c r="N147">
+        <v>4</v>
+      </c>
+      <c r="O147">
+        <f t="shared" si="29"/>
+        <v>2.7E-6</v>
+      </c>
+      <c r="P147" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q147">
+        <v>10900</v>
+      </c>
+      <c r="R147">
+        <v>5</v>
+      </c>
+      <c r="S147" t="s">
+        <v>27</v>
+      </c>
+      <c r="T147">
+        <v>0.05</v>
+      </c>
+      <c r="U147">
         <v>110</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Ignore File 1, Stim 11.
</commit_message>
<xml_diff>
--- a/scripts/file_params.xlsx
+++ b/scripts/file_params.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jai\Documents\Computing\RProg\Columbia\rwalk\scripts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B282E381-E65D-42EE-9842-58B2D56D8CB6}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F7B79C2-71BC-4CF6-B183-FE5926F96977}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1970,14 +1970,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:Y466"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="K467" sqref="K467"/>
+      <selection pane="bottomRight" activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2086,7 +2085,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -2161,7 +2160,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="3" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -2236,7 +2235,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="4" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -2311,7 +2310,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="5" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -2386,7 +2385,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="6" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -2461,7 +2460,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="7" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>3</v>
       </c>
@@ -2536,7 +2535,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="8" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>3</v>
       </c>
@@ -2614,7 +2613,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="9" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>3</v>
       </c>
@@ -2692,7 +2691,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="10" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>3</v>
       </c>
@@ -2768,7 +2767,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="11" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>3</v>
       </c>
@@ -2844,7 +2843,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="12" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>3</v>
       </c>
@@ -2855,7 +2854,7 @@
         <v>11</v>
       </c>
       <c r="D12" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E12">
         <f t="shared" si="1"/>
@@ -2920,7 +2919,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="13" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>3</v>
       </c>
@@ -2996,7 +2995,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="14" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>3</v>
       </c>
@@ -3072,7 +3071,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="15" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>3</v>
       </c>
@@ -3147,7 +3146,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="16" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>3</v>
       </c>
@@ -3222,7 +3221,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="17" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>4</v>
       </c>
@@ -3298,7 +3297,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="18" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A18" t="str">
         <f>A17</f>
         <v>180920_10mg-kgAMPH_2.csv</v>
@@ -3375,7 +3374,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="19" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A19" t="str">
         <f t="shared" ref="A19:A31" si="2">A18</f>
         <v>180920_10mg-kgAMPH_2.csv</v>
@@ -3452,7 +3451,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="20" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A20" t="str">
         <f t="shared" si="2"/>
         <v>180920_10mg-kgAMPH_2.csv</v>
@@ -3529,7 +3528,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="21" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A21" t="str">
         <f t="shared" si="2"/>
         <v>180920_10mg-kgAMPH_2.csv</v>
@@ -3606,7 +3605,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="22" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A22" t="str">
         <f t="shared" si="2"/>
         <v>180920_10mg-kgAMPH_2.csv</v>
@@ -3683,7 +3682,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="23" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A23" t="str">
         <f t="shared" si="2"/>
         <v>180920_10mg-kgAMPH_2.csv</v>
@@ -3760,7 +3759,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="24" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A24" t="str">
         <f t="shared" si="2"/>
         <v>180920_10mg-kgAMPH_2.csv</v>
@@ -3837,7 +3836,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="25" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A25" t="str">
         <f t="shared" si="2"/>
         <v>180920_10mg-kgAMPH_2.csv</v>
@@ -3914,7 +3913,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="26" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A26" t="str">
         <f t="shared" si="2"/>
         <v>180920_10mg-kgAMPH_2.csv</v>
@@ -3991,7 +3990,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="27" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A27" t="str">
         <f t="shared" si="2"/>
         <v>180920_10mg-kgAMPH_2.csv</v>
@@ -4068,7 +4067,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="28" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A28" t="str">
         <f t="shared" si="2"/>
         <v>180920_10mg-kgAMPH_2.csv</v>
@@ -4145,7 +4144,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="29" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A29" t="str">
         <f t="shared" si="2"/>
         <v>180920_10mg-kgAMPH_2.csv</v>
@@ -4222,7 +4221,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="30" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A30" t="str">
         <f t="shared" si="2"/>
         <v>180920_10mg-kgAMPH_2.csv</v>
@@ -4299,7 +4298,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="31" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A31" t="str">
         <f t="shared" si="2"/>
         <v>180920_10mg-kgAMPH_2.csv</v>
@@ -4376,7 +4375,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="32" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>28</v>
       </c>
@@ -4451,7 +4450,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="33" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>28</v>
       </c>
@@ -4527,7 +4526,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="34" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>28</v>
       </c>
@@ -4603,7 +4602,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="35" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>28</v>
       </c>
@@ -4679,7 +4678,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="36" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>28</v>
       </c>
@@ -4755,7 +4754,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="37" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>28</v>
       </c>
@@ -4831,7 +4830,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="38" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>28</v>
       </c>
@@ -4907,7 +4906,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="39" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>28</v>
       </c>
@@ -4983,7 +4982,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="40" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>28</v>
       </c>
@@ -5060,7 +5059,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="41" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>28</v>
       </c>
@@ -5137,7 +5136,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="42" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>28</v>
       </c>
@@ -5214,7 +5213,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="43" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>28</v>
       </c>
@@ -5291,7 +5290,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="44" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>28</v>
       </c>
@@ -5368,7 +5367,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="45" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>28</v>
       </c>
@@ -5445,7 +5444,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="46" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>28</v>
       </c>
@@ -5522,7 +5521,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="47" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>29</v>
       </c>
@@ -5598,7 +5597,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="48" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>29</v>
       </c>
@@ -5674,7 +5673,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="49" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>29</v>
       </c>
@@ -5750,7 +5749,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="50" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>29</v>
       </c>
@@ -5826,7 +5825,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="51" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>29</v>
       </c>
@@ -5902,7 +5901,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="52" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>29</v>
       </c>
@@ -5978,7 +5977,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="53" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>29</v>
       </c>
@@ -6054,7 +6053,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="54" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>29</v>
       </c>
@@ -6130,7 +6129,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="55" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>29</v>
       </c>
@@ -6206,7 +6205,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="56" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>29</v>
       </c>
@@ -6282,7 +6281,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="57" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>29</v>
       </c>
@@ -6358,7 +6357,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="58" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>29</v>
       </c>
@@ -6435,7 +6434,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="59" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>29</v>
       </c>
@@ -6512,7 +6511,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="60" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>29</v>
       </c>
@@ -6589,7 +6588,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="61" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>29</v>
       </c>
@@ -6666,7 +6665,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="62" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>30</v>
       </c>
@@ -6741,7 +6740,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="63" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>30</v>
       </c>
@@ -6817,7 +6816,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="64" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>30</v>
       </c>
@@ -6893,7 +6892,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="65" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>30</v>
       </c>
@@ -6969,7 +6968,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="66" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>30</v>
       </c>
@@ -7045,7 +7044,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="67" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>30</v>
       </c>
@@ -7121,7 +7120,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="68" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>30</v>
       </c>
@@ -7197,7 +7196,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="69" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>30</v>
       </c>
@@ -7273,7 +7272,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="70" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>30</v>
       </c>
@@ -7349,7 +7348,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="71" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>30</v>
       </c>
@@ -7425,7 +7424,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="72" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>30</v>
       </c>
@@ -7501,7 +7500,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="73" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>30</v>
       </c>
@@ -7577,7 +7576,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="74" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>30</v>
       </c>
@@ -7653,7 +7652,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="75" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>30</v>
       </c>
@@ -7729,7 +7728,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="76" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>30</v>
       </c>
@@ -7805,7 +7804,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="77" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>32</v>
       </c>
@@ -7881,7 +7880,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="78" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>32</v>
       </c>
@@ -7957,7 +7956,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="79" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>32</v>
       </c>
@@ -8033,7 +8032,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="80" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>32</v>
       </c>
@@ -8109,7 +8108,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="81" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>32</v>
       </c>
@@ -8185,7 +8184,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="82" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>32</v>
       </c>
@@ -8261,7 +8260,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="83" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>32</v>
       </c>
@@ -8337,7 +8336,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="84" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>32</v>
       </c>
@@ -8413,7 +8412,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="85" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>32</v>
       </c>
@@ -8489,7 +8488,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="86" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>32</v>
       </c>
@@ -8565,7 +8564,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="87" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>32</v>
       </c>
@@ -8641,7 +8640,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="88" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>32</v>
       </c>
@@ -8717,7 +8716,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="89" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>32</v>
       </c>
@@ -8793,7 +8792,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="90" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>32</v>
       </c>
@@ -8869,7 +8868,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="91" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>32</v>
       </c>
@@ -8945,7 +8944,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="92" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>5</v>
       </c>
@@ -9020,7 +9019,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="93" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A93" t="str">
         <f>A92</f>
         <v>190205_a-synKO_AMPH1.csv</v>
@@ -9099,7 +9098,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="94" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A94" t="str">
         <f t="shared" ref="A94:A106" si="11">A93</f>
         <v>190205_a-synKO_AMPH1.csv</v>
@@ -9178,7 +9177,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="95" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A95" t="str">
         <f t="shared" si="11"/>
         <v>190205_a-synKO_AMPH1.csv</v>
@@ -9256,7 +9255,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="96" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A96" t="str">
         <f t="shared" si="11"/>
         <v>190205_a-synKO_AMPH1.csv</v>
@@ -9334,7 +9333,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="97" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A97" t="str">
         <f t="shared" si="11"/>
         <v>190205_a-synKO_AMPH1.csv</v>
@@ -9412,7 +9411,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="98" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A98" t="str">
         <f t="shared" si="11"/>
         <v>190205_a-synKO_AMPH1.csv</v>
@@ -9490,7 +9489,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="99" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A99" t="str">
         <f t="shared" si="11"/>
         <v>190205_a-synKO_AMPH1.csv</v>
@@ -9568,7 +9567,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="100" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A100" t="str">
         <f t="shared" si="11"/>
         <v>190205_a-synKO_AMPH1.csv</v>
@@ -9646,7 +9645,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="101" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A101" t="str">
         <f t="shared" si="11"/>
         <v>190205_a-synKO_AMPH1.csv</v>
@@ -9724,7 +9723,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="102" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A102" t="str">
         <f t="shared" si="11"/>
         <v>190205_a-synKO_AMPH1.csv</v>
@@ -9802,7 +9801,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="103" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A103" t="str">
         <f t="shared" si="11"/>
         <v>190205_a-synKO_AMPH1.csv</v>
@@ -9880,7 +9879,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="104" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A104" t="str">
         <f t="shared" si="11"/>
         <v>190205_a-synKO_AMPH1.csv</v>
@@ -9959,7 +9958,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="105" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A105" t="str">
         <f t="shared" si="11"/>
         <v>190205_a-synKO_AMPH1.csv</v>
@@ -10038,7 +10037,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="106" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A106" t="str">
         <f t="shared" si="11"/>
         <v>190205_a-synKO_AMPH1.csv</v>
@@ -10116,7 +10115,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="107" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>10</v>
       </c>
@@ -10192,7 +10191,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="108" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A108" t="str">
         <f>A107</f>
         <v>190205_a-synKO_AMPH2.csv</v>
@@ -10270,7 +10269,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="109" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A109" t="str">
         <f t="shared" ref="A109:A121" si="16">A108</f>
         <v>190205_a-synKO_AMPH2.csv</v>
@@ -10348,7 +10347,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="110" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A110" t="str">
         <f t="shared" si="16"/>
         <v>190205_a-synKO_AMPH2.csv</v>
@@ -10426,7 +10425,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="111" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A111" t="str">
         <f t="shared" si="16"/>
         <v>190205_a-synKO_AMPH2.csv</v>
@@ -10504,7 +10503,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="112" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A112" t="str">
         <f t="shared" si="16"/>
         <v>190205_a-synKO_AMPH2.csv</v>
@@ -10582,7 +10581,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="113" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A113" t="str">
         <f t="shared" si="16"/>
         <v>190205_a-synKO_AMPH2.csv</v>
@@ -10660,7 +10659,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="114" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A114" t="str">
         <f t="shared" si="16"/>
         <v>190205_a-synKO_AMPH2.csv</v>
@@ -10738,7 +10737,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="115" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A115" t="str">
         <f t="shared" si="16"/>
         <v>190205_a-synKO_AMPH2.csv</v>
@@ -10816,7 +10815,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="116" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A116" t="str">
         <f t="shared" si="16"/>
         <v>190205_a-synKO_AMPH2.csv</v>
@@ -10894,7 +10893,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="117" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A117" t="str">
         <f t="shared" si="16"/>
         <v>190205_a-synKO_AMPH2.csv</v>
@@ -10973,7 +10972,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="118" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A118" t="str">
         <f t="shared" si="16"/>
         <v>190205_a-synKO_AMPH2.csv</v>
@@ -11054,7 +11053,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="119" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A119" t="str">
         <f t="shared" si="16"/>
         <v>190205_a-synKO_AMPH2.csv</v>
@@ -11132,7 +11131,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="120" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A120" t="str">
         <f t="shared" si="16"/>
         <v>190205_a-synKO_AMPH2.csv</v>
@@ -11211,7 +11210,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="121" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A121" t="str">
         <f t="shared" si="16"/>
         <v>190205_a-synKO_AMPH2.csv</v>
@@ -11289,7 +11288,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="122" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>36</v>
       </c>
@@ -11364,7 +11363,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="123" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>36</v>
       </c>
@@ -11438,7 +11437,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="124" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>36</v>
       </c>
@@ -11512,7 +11511,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="125" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>36</v>
       </c>
@@ -11586,7 +11585,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="126" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>36</v>
       </c>
@@ -11660,7 +11659,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="127" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>36</v>
       </c>
@@ -11734,7 +11733,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="128" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>36</v>
       </c>
@@ -11808,7 +11807,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="129" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>36</v>
       </c>
@@ -11882,7 +11881,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="130" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>36</v>
       </c>
@@ -11956,7 +11955,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="131" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>36</v>
       </c>
@@ -12030,7 +12029,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="132" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>36</v>
       </c>
@@ -12104,7 +12103,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="133" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>36</v>
       </c>
@@ -12178,7 +12177,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="134" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>36</v>
       </c>
@@ -12252,7 +12251,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="135" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>36</v>
       </c>
@@ -12326,7 +12325,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="136" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>36</v>
       </c>
@@ -12400,7 +12399,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="137" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>33</v>
       </c>
@@ -12475,7 +12474,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="138" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>33</v>
       </c>
@@ -12551,7 +12550,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="139" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>33</v>
       </c>
@@ -12627,7 +12626,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="140" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>33</v>
       </c>
@@ -12703,7 +12702,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="141" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>33</v>
       </c>
@@ -12779,7 +12778,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="142" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>33</v>
       </c>
@@ -12855,7 +12854,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="143" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>33</v>
       </c>
@@ -12931,7 +12930,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="144" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>33</v>
       </c>
@@ -13007,7 +13006,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="145" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>33</v>
       </c>
@@ -13083,7 +13082,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="146" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>33</v>
       </c>
@@ -13159,7 +13158,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="147" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>34</v>
       </c>
@@ -13235,7 +13234,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="148" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>34</v>
       </c>
@@ -13311,7 +13310,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="149" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>34</v>
       </c>
@@ -13388,7 +13387,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="150" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>34</v>
       </c>
@@ -13465,7 +13464,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="151" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>34</v>
       </c>
@@ -13542,7 +13541,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="152" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>34</v>
       </c>
@@ -13619,7 +13618,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="153" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>34</v>
       </c>
@@ -13693,7 +13692,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="154" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>34</v>
       </c>
@@ -13770,7 +13769,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="155" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>34</v>
       </c>
@@ -13847,7 +13846,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="156" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>34</v>
       </c>
@@ -13924,7 +13923,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="157" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>35</v>
       </c>
@@ -14000,7 +13999,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="158" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>35</v>
       </c>
@@ -14076,7 +14075,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="159" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>35</v>
       </c>
@@ -14152,7 +14151,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="160" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>35</v>
       </c>
@@ -14228,7 +14227,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="161" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>35</v>
       </c>
@@ -14304,7 +14303,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="162" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>35</v>
       </c>
@@ -14380,7 +14379,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="163" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>51</v>
       </c>
@@ -14452,7 +14451,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="164" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>51</v>
       </c>
@@ -14526,7 +14525,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="165" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
         <v>51</v>
       </c>
@@ -14600,7 +14599,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="166" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>51</v>
       </c>
@@ -14674,7 +14673,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="167" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>51</v>
       </c>
@@ -14748,7 +14747,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="168" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>51</v>
       </c>
@@ -14822,7 +14821,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="169" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
         <v>51</v>
       </c>
@@ -14896,7 +14895,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="170" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
         <v>51</v>
       </c>
@@ -14970,7 +14969,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="171" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
         <v>51</v>
       </c>
@@ -15044,7 +15043,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="172" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
         <v>51</v>
       </c>
@@ -15118,7 +15117,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="173" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
         <v>52</v>
       </c>
@@ -15191,7 +15190,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="174" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
         <v>52</v>
       </c>
@@ -15264,7 +15263,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="175" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
         <v>52</v>
       </c>
@@ -15337,7 +15336,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="176" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
         <v>52</v>
       </c>
@@ -15410,7 +15409,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="177" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
         <v>52</v>
       </c>
@@ -15483,7 +15482,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="178" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
         <v>52</v>
       </c>
@@ -15556,7 +15555,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="179" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
         <v>52</v>
       </c>
@@ -15629,7 +15628,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="180" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
         <v>52</v>
       </c>
@@ -15702,7 +15701,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="181" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
         <v>52</v>
       </c>
@@ -15775,7 +15774,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="182" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
         <v>52</v>
       </c>
@@ -15848,7 +15847,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="183" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
         <v>53</v>
       </c>
@@ -15921,7 +15920,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="184" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
         <v>53</v>
       </c>
@@ -15998,7 +15997,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="185" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
         <v>54</v>
       </c>
@@ -16071,7 +16070,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="186" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
         <v>54</v>
       </c>
@@ -16144,7 +16143,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="187" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
         <v>54</v>
       </c>
@@ -16217,7 +16216,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="188" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
         <v>54</v>
       </c>
@@ -16290,7 +16289,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="189" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
         <v>54</v>
       </c>
@@ -16363,7 +16362,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="190" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
         <v>54</v>
       </c>
@@ -16436,7 +16435,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="191" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
         <v>54</v>
       </c>
@@ -16509,7 +16508,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="192" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
         <v>37</v>
       </c>
@@ -16581,7 +16580,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="193" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
         <v>37</v>
       </c>
@@ -16655,7 +16654,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="194" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
         <v>37</v>
       </c>
@@ -16729,7 +16728,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="195" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
         <v>37</v>
       </c>
@@ -16803,7 +16802,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="196" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
         <v>37</v>
       </c>
@@ -16877,7 +16876,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="197" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
         <v>37</v>
       </c>
@@ -16951,7 +16950,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="198" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
         <v>37</v>
       </c>
@@ -17025,7 +17024,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="199" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
         <v>37</v>
       </c>
@@ -17099,7 +17098,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="200" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
         <v>37</v>
       </c>
@@ -17173,7 +17172,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="201" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
         <v>37</v>
       </c>
@@ -17247,7 +17246,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="202" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
         <v>37</v>
       </c>
@@ -17321,7 +17320,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="203" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
         <v>37</v>
       </c>
@@ -17395,7 +17394,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="204" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
         <v>37</v>
       </c>
@@ -17469,7 +17468,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="205" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
         <v>37</v>
       </c>
@@ -17543,7 +17542,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="206" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
         <v>37</v>
       </c>
@@ -17617,7 +17616,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="207" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
         <v>38</v>
       </c>
@@ -17690,7 +17689,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="208" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
         <v>38</v>
       </c>
@@ -17764,7 +17763,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="209" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
         <v>38</v>
       </c>
@@ -17838,7 +17837,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="210" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
         <v>38</v>
       </c>
@@ -17912,7 +17911,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="211" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
         <v>38</v>
       </c>
@@ -17986,7 +17985,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="212" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
         <v>38</v>
       </c>
@@ -18060,7 +18059,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="213" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
         <v>38</v>
       </c>
@@ -18134,7 +18133,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="214" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
         <v>38</v>
       </c>
@@ -18208,7 +18207,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="215" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
         <v>38</v>
       </c>
@@ -18282,7 +18281,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="216" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
         <v>38</v>
       </c>
@@ -18356,7 +18355,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="217" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
         <v>38</v>
       </c>
@@ -18430,7 +18429,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="218" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
         <v>38</v>
       </c>
@@ -18504,7 +18503,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="219" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
         <v>38</v>
       </c>
@@ -18578,7 +18577,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="220" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
         <v>38</v>
       </c>
@@ -18652,7 +18651,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="221" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
         <v>38</v>
       </c>
@@ -18726,7 +18725,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="222" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
         <v>55</v>
       </c>
@@ -18798,7 +18797,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="223" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
         <v>55</v>
       </c>
@@ -18872,7 +18871,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="224" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
         <v>55</v>
       </c>
@@ -18946,7 +18945,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="225" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
         <v>55</v>
       </c>
@@ -19020,7 +19019,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="226" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
         <v>55</v>
       </c>
@@ -19094,7 +19093,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="227" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
         <v>55</v>
       </c>
@@ -19168,7 +19167,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="228" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
         <v>55</v>
       </c>
@@ -19242,7 +19241,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="229" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
         <v>55</v>
       </c>
@@ -19316,7 +19315,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="230" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
         <v>55</v>
       </c>
@@ -19390,7 +19389,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="231" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
         <v>55</v>
       </c>
@@ -19464,7 +19463,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="232" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
         <v>55</v>
       </c>
@@ -19538,7 +19537,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="233" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A233" t="s">
         <v>55</v>
       </c>
@@ -19612,7 +19611,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="234" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A234" t="s">
         <v>55</v>
       </c>
@@ -19686,7 +19685,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="235" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A235" t="s">
         <v>55</v>
       </c>
@@ -19760,7 +19759,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="236" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A236" t="s">
         <v>55</v>
       </c>
@@ -19834,7 +19833,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="237" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A237" t="s">
         <v>56</v>
       </c>
@@ -19907,7 +19906,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="238" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A238" t="s">
         <v>56</v>
       </c>
@@ -19980,7 +19979,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="239" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A239" t="s">
         <v>56</v>
       </c>
@@ -20053,7 +20052,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="240" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A240" t="s">
         <v>56</v>
       </c>
@@ -20126,7 +20125,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="241" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A241" t="s">
         <v>56</v>
       </c>
@@ -20199,7 +20198,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="242" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A242" t="s">
         <v>56</v>
       </c>
@@ -20272,7 +20271,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="243" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A243" t="s">
         <v>56</v>
       </c>
@@ -20345,7 +20344,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="244" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A244" t="s">
         <v>56</v>
       </c>
@@ -20418,7 +20417,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="245" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A245" t="s">
         <v>56</v>
       </c>
@@ -20491,7 +20490,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="246" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A246" t="s">
         <v>56</v>
       </c>
@@ -20564,7 +20563,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="247" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A247" t="s">
         <v>56</v>
       </c>
@@ -20637,7 +20636,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="248" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A248" t="s">
         <v>56</v>
       </c>
@@ -20710,7 +20709,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="249" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A249" t="s">
         <v>56</v>
       </c>
@@ -20783,7 +20782,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="250" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A250" t="s">
         <v>56</v>
       </c>
@@ -20856,7 +20855,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="251" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A251" t="s">
         <v>56</v>
       </c>
@@ -20929,7 +20928,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="252" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A252" t="s">
         <v>62</v>
       </c>
@@ -21001,7 +21000,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="253" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A253" t="s">
         <v>62</v>
       </c>
@@ -21075,7 +21074,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="254" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A254" t="s">
         <v>62</v>
       </c>
@@ -21149,7 +21148,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="255" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A255" t="s">
         <v>62</v>
       </c>
@@ -21223,7 +21222,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="256" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A256" t="s">
         <v>62</v>
       </c>
@@ -21297,7 +21296,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="257" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A257" t="s">
         <v>62</v>
       </c>
@@ -21371,7 +21370,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="258" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A258" t="s">
         <v>62</v>
       </c>
@@ -21445,7 +21444,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="259" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A259" t="s">
         <v>62</v>
       </c>
@@ -21519,7 +21518,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="260" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A260" t="s">
         <v>62</v>
       </c>
@@ -21593,7 +21592,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="261" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A261" t="s">
         <v>62</v>
       </c>
@@ -21667,7 +21666,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="262" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A262" t="s">
         <v>62</v>
       </c>
@@ -21741,7 +21740,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="263" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A263" t="s">
         <v>62</v>
       </c>
@@ -21815,7 +21814,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="264" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A264" t="s">
         <v>62</v>
       </c>
@@ -21889,7 +21888,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="265" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A265" t="s">
         <v>62</v>
       </c>
@@ -21963,7 +21962,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="266" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A266" t="s">
         <v>62</v>
       </c>
@@ -22037,7 +22036,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="267" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A267" t="s">
         <v>73</v>
       </c>
@@ -22110,7 +22109,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="268" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A268" t="s">
         <v>73</v>
       </c>
@@ -22184,7 +22183,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="269" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A269" t="s">
         <v>73</v>
       </c>
@@ -22258,7 +22257,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="270" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A270" t="s">
         <v>73</v>
       </c>
@@ -22332,7 +22331,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="271" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A271" t="s">
         <v>73</v>
       </c>
@@ -22406,7 +22405,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="272" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A272" t="s">
         <v>73</v>
       </c>
@@ -22480,7 +22479,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="273" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A273" t="s">
         <v>73</v>
       </c>
@@ -22554,7 +22553,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="274" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A274" t="s">
         <v>73</v>
       </c>
@@ -22628,7 +22627,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="275" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A275" t="s">
         <v>73</v>
       </c>
@@ -22702,7 +22701,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="276" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A276" t="s">
         <v>73</v>
       </c>
@@ -22776,7 +22775,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="277" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A277" t="s">
         <v>73</v>
       </c>
@@ -22850,7 +22849,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="278" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A278" t="s">
         <v>73</v>
       </c>
@@ -22924,7 +22923,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="279" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A279" t="s">
         <v>73</v>
       </c>
@@ -22998,7 +22997,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="280" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A280" t="s">
         <v>73</v>
       </c>
@@ -23072,7 +23071,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="281" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A281" t="s">
         <v>73</v>
       </c>
@@ -23146,7 +23145,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="282" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A282" t="s">
         <v>57</v>
       </c>
@@ -23218,7 +23217,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="283" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A283" t="s">
         <v>57</v>
       </c>
@@ -23291,7 +23290,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="284" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A284" t="s">
         <v>57</v>
       </c>
@@ -23364,7 +23363,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="285" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A285" t="s">
         <v>57</v>
       </c>
@@ -23437,7 +23436,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="286" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A286" t="s">
         <v>57</v>
       </c>
@@ -23510,7 +23509,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="287" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A287" t="s">
         <v>57</v>
       </c>
@@ -23583,7 +23582,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="288" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A288" t="s">
         <v>57</v>
       </c>
@@ -23656,7 +23655,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="289" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A289" t="s">
         <v>57</v>
       </c>
@@ -23729,7 +23728,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="290" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A290" t="s">
         <v>57</v>
       </c>
@@ -23802,7 +23801,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="291" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A291" t="s">
         <v>57</v>
       </c>
@@ -23875,7 +23874,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="292" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A292" t="s">
         <v>57</v>
       </c>
@@ -23948,7 +23947,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="293" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A293" t="s">
         <v>57</v>
       </c>
@@ -24021,7 +24020,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="294" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A294" t="s">
         <v>57</v>
       </c>
@@ -24094,7 +24093,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="295" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A295" t="s">
         <v>57</v>
       </c>
@@ -24167,7 +24166,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="296" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A296" t="s">
         <v>57</v>
       </c>
@@ -24240,7 +24239,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="297" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A297" t="s">
         <v>58</v>
       </c>
@@ -24313,7 +24312,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="298" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A298" t="s">
         <v>58</v>
       </c>
@@ -24386,7 +24385,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="299" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A299" t="s">
         <v>58</v>
       </c>
@@ -24459,7 +24458,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="300" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A300" t="s">
         <v>58</v>
       </c>
@@ -24532,7 +24531,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="301" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A301" t="s">
         <v>58</v>
       </c>
@@ -24605,7 +24604,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="302" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A302" t="s">
         <v>58</v>
       </c>
@@ -24678,7 +24677,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="303" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A303" t="s">
         <v>58</v>
       </c>
@@ -24751,7 +24750,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="304" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A304" t="s">
         <v>58</v>
       </c>
@@ -24824,7 +24823,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="305" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A305" t="s">
         <v>58</v>
       </c>
@@ -24897,7 +24896,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="306" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A306" t="s">
         <v>58</v>
       </c>
@@ -24970,7 +24969,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="307" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A307" t="s">
         <v>58</v>
       </c>
@@ -25043,7 +25042,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="308" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A308" t="s">
         <v>58</v>
       </c>
@@ -25116,7 +25115,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="309" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A309" t="s">
         <v>58</v>
       </c>
@@ -25189,7 +25188,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="310" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A310" t="s">
         <v>58</v>
       </c>
@@ -25262,7 +25261,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="311" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A311" t="s">
         <v>58</v>
       </c>
@@ -25335,7 +25334,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="312" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A312" t="s">
         <v>59</v>
       </c>
@@ -25407,7 +25406,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="313" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A313" t="s">
         <v>59</v>
       </c>
@@ -25480,7 +25479,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="314" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A314" t="s">
         <v>59</v>
       </c>
@@ -25553,7 +25552,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="315" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A315" t="s">
         <v>59</v>
       </c>
@@ -25626,7 +25625,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="316" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A316" t="s">
         <v>59</v>
       </c>
@@ -25699,7 +25698,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="317" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="317" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A317" t="s">
         <v>59</v>
       </c>
@@ -25772,7 +25771,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="318" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A318" t="s">
         <v>59</v>
       </c>
@@ -25845,7 +25844,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="319" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="319" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A319" t="s">
         <v>59</v>
       </c>
@@ -25918,7 +25917,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="320" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="320" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A320" t="s">
         <v>59</v>
       </c>
@@ -25991,7 +25990,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="321" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="321" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A321" t="s">
         <v>59</v>
       </c>
@@ -26064,7 +26063,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="322" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="322" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A322" t="s">
         <v>59</v>
       </c>
@@ -26137,7 +26136,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="323" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="323" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A323" t="s">
         <v>59</v>
       </c>
@@ -26210,7 +26209,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="324" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="324" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A324" t="s">
         <v>59</v>
       </c>
@@ -26283,7 +26282,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="325" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="325" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A325" t="s">
         <v>59</v>
       </c>
@@ -26356,7 +26355,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="326" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="326" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A326" t="s">
         <v>59</v>
       </c>
@@ -26429,7 +26428,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="327" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="327" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A327" t="s">
         <v>60</v>
       </c>
@@ -26501,7 +26500,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="328" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="328" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A328" t="s">
         <v>60</v>
       </c>
@@ -26574,7 +26573,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="329" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="329" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A329" t="s">
         <v>60</v>
       </c>
@@ -26647,7 +26646,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="330" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="330" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A330" t="s">
         <v>60</v>
       </c>
@@ -26720,7 +26719,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="331" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="331" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A331" t="s">
         <v>60</v>
       </c>
@@ -26793,7 +26792,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="332" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="332" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A332" t="s">
         <v>60</v>
       </c>
@@ -26866,7 +26865,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="333" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="333" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A333" t="s">
         <v>60</v>
       </c>
@@ -26939,7 +26938,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="334" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="334" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A334" t="s">
         <v>60</v>
       </c>
@@ -27012,7 +27011,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="335" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="335" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A335" t="s">
         <v>60</v>
       </c>
@@ -27085,7 +27084,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="336" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="336" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A336" t="s">
         <v>60</v>
       </c>
@@ -27158,7 +27157,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="337" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="337" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A337" t="s">
         <v>60</v>
       </c>
@@ -27231,7 +27230,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="338" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="338" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A338" t="s">
         <v>60</v>
       </c>
@@ -27304,7 +27303,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="339" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="339" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A339" t="s">
         <v>60</v>
       </c>
@@ -27377,7 +27376,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="340" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="340" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A340" t="s">
         <v>60</v>
       </c>
@@ -27450,7 +27449,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="341" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="341" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A341" t="s">
         <v>60</v>
       </c>
@@ -27523,7 +27522,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="342" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="342" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A342" t="s">
         <v>61</v>
       </c>
@@ -27598,7 +27597,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="343" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="343" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A343" t="s">
         <v>61</v>
       </c>
@@ -27671,7 +27670,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="344" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="344" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A344" t="s">
         <v>61</v>
       </c>
@@ -27745,7 +27744,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="345" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="345" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A345" t="s">
         <v>61</v>
       </c>
@@ -27819,7 +27818,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="346" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="346" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A346" t="s">
         <v>61</v>
       </c>
@@ -27893,7 +27892,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="347" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="347" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A347" t="s">
         <v>61</v>
       </c>
@@ -27967,7 +27966,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="348" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="348" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A348" t="s">
         <v>61</v>
       </c>
@@ -28041,7 +28040,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="349" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="349" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A349" t="s">
         <v>61</v>
       </c>
@@ -28115,7 +28114,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="350" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="350" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A350" t="s">
         <v>61</v>
       </c>
@@ -28189,7 +28188,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="351" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="351" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A351" t="s">
         <v>61</v>
       </c>
@@ -28263,7 +28262,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="352" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="352" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A352" t="s">
         <v>61</v>
       </c>
@@ -28337,7 +28336,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="353" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="353" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A353" t="s">
         <v>61</v>
       </c>
@@ -28411,7 +28410,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="354" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="354" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A354" t="s">
         <v>61</v>
       </c>
@@ -28485,7 +28484,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="355" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="355" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A355" t="s">
         <v>61</v>
       </c>
@@ -28559,7 +28558,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="356" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="356" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A356" t="s">
         <v>61</v>
       </c>
@@ -28633,7 +28632,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="357" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="357" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A357" t="s">
         <v>63</v>
       </c>
@@ -28705,7 +28704,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="358" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="358" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A358" t="s">
         <v>63</v>
       </c>
@@ -28779,7 +28778,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="359" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="359" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A359" t="s">
         <v>63</v>
       </c>
@@ -28853,7 +28852,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="360" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="360" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A360" t="s">
         <v>63</v>
       </c>
@@ -28927,7 +28926,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="361" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="361" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A361" t="s">
         <v>63</v>
       </c>
@@ -29001,7 +29000,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="362" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="362" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A362" t="s">
         <v>63</v>
       </c>
@@ -29075,7 +29074,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="363" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="363" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A363" t="s">
         <v>63</v>
       </c>
@@ -29149,7 +29148,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="364" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="364" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A364" t="s">
         <v>63</v>
       </c>
@@ -29223,7 +29222,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="365" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="365" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A365" t="s">
         <v>63</v>
       </c>
@@ -29297,7 +29296,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="366" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="366" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A366" t="s">
         <v>63</v>
       </c>
@@ -29371,7 +29370,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="367" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="367" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A367" t="s">
         <v>64</v>
       </c>
@@ -29443,7 +29442,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="368" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="368" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A368" t="s">
         <v>64</v>
       </c>
@@ -29516,7 +29515,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="369" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="369" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A369" t="s">
         <v>64</v>
       </c>
@@ -29589,7 +29588,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="370" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="370" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A370" t="s">
         <v>64</v>
       </c>
@@ -29662,7 +29661,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="371" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="371" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A371" t="s">
         <v>64</v>
       </c>
@@ -29735,7 +29734,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="372" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="372" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A372" t="s">
         <v>64</v>
       </c>
@@ -29808,7 +29807,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="373" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="373" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A373" t="s">
         <v>64</v>
       </c>
@@ -29881,7 +29880,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="374" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="374" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A374" t="s">
         <v>64</v>
       </c>
@@ -29954,7 +29953,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="375" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="375" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A375" t="s">
         <v>64</v>
       </c>
@@ -30027,7 +30026,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="376" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="376" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A376" t="s">
         <v>64</v>
       </c>
@@ -30100,7 +30099,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="377" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="377" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A377" t="s">
         <v>65</v>
       </c>
@@ -30172,7 +30171,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="378" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="378" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A378" t="s">
         <v>65</v>
       </c>
@@ -30248,7 +30247,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="379" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="379" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A379" t="s">
         <v>65</v>
       </c>
@@ -30321,7 +30320,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="380" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="380" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A380" t="s">
         <v>65</v>
       </c>
@@ -30394,7 +30393,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="381" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="381" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A381" t="s">
         <v>65</v>
       </c>
@@ -30467,7 +30466,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="382" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="382" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A382" t="s">
         <v>65</v>
       </c>
@@ -30540,7 +30539,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="383" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="383" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A383" t="s">
         <v>65</v>
       </c>
@@ -30613,7 +30612,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="384" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="384" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A384" t="s">
         <v>65</v>
       </c>
@@ -30686,7 +30685,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="385" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="385" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A385" t="s">
         <v>65</v>
       </c>
@@ -30759,7 +30758,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="386" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="386" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A386" t="s">
         <v>65</v>
       </c>
@@ -30832,7 +30831,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="387" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="387" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A387" t="s">
         <v>65</v>
       </c>
@@ -30905,7 +30904,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="388" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="388" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A388" t="s">
         <v>65</v>
       </c>
@@ -30978,7 +30977,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="389" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="389" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A389" t="s">
         <v>65</v>
       </c>
@@ -31051,7 +31050,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="390" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="390" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A390" t="s">
         <v>65</v>
       </c>
@@ -31124,7 +31123,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="391" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="391" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A391" t="s">
         <v>65</v>
       </c>
@@ -31196,7 +31195,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="392" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="392" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A392" t="s">
         <v>66</v>
       </c>
@@ -31272,7 +31271,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="393" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="393" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A393" t="s">
         <v>66</v>
       </c>
@@ -31345,7 +31344,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="394" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="394" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A394" t="s">
         <v>66</v>
       </c>
@@ -31418,7 +31417,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="395" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="395" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A395" t="s">
         <v>66</v>
       </c>
@@ -31491,7 +31490,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="396" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="396" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A396" t="s">
         <v>66</v>
       </c>
@@ -31564,7 +31563,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="397" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="397" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A397" t="s">
         <v>66</v>
       </c>
@@ -31637,7 +31636,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="398" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="398" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A398" t="s">
         <v>66</v>
       </c>
@@ -31710,7 +31709,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="399" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="399" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A399" t="s">
         <v>66</v>
       </c>
@@ -31783,7 +31782,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="400" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="400" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A400" t="s">
         <v>66</v>
       </c>
@@ -31856,7 +31855,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="401" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="401" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A401" t="s">
         <v>66</v>
       </c>
@@ -31929,7 +31928,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="402" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="402" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A402" t="s">
         <v>66</v>
       </c>
@@ -32002,7 +32001,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="403" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="403" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A403" t="s">
         <v>66</v>
       </c>
@@ -32075,7 +32074,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="404" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="404" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A404" t="s">
         <v>66</v>
       </c>
@@ -32148,7 +32147,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="405" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="405" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A405" t="s">
         <v>66</v>
       </c>
@@ -32221,7 +32220,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="406" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="406" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A406" t="s">
         <v>66</v>
       </c>
@@ -32294,7 +32293,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="407" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="407" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A407" t="s">
         <v>67</v>
       </c>
@@ -32366,7 +32365,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="408" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="408" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A408" t="s">
         <v>67</v>
       </c>
@@ -32439,7 +32438,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="409" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="409" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A409" t="s">
         <v>67</v>
       </c>
@@ -32512,7 +32511,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="410" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="410" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A410" t="s">
         <v>67</v>
       </c>
@@ -32585,7 +32584,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="411" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="411" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A411" t="s">
         <v>67</v>
       </c>
@@ -32658,7 +32657,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="412" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="412" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A412" t="s">
         <v>67</v>
       </c>
@@ -32731,7 +32730,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="413" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="413" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A413" t="s">
         <v>67</v>
       </c>
@@ -32804,7 +32803,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="414" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="414" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A414" t="s">
         <v>67</v>
       </c>
@@ -32877,7 +32876,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="415" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="415" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A415" t="s">
         <v>67</v>
       </c>
@@ -32950,7 +32949,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="416" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="416" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A416" t="s">
         <v>67</v>
       </c>
@@ -33023,7 +33022,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="417" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="417" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A417" t="s">
         <v>68</v>
       </c>
@@ -33096,7 +33095,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="418" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="418" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A418" t="s">
         <v>68</v>
       </c>
@@ -33169,7 +33168,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="419" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="419" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A419" t="s">
         <v>68</v>
       </c>
@@ -33242,7 +33241,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="420" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="420" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A420" t="s">
         <v>68</v>
       </c>
@@ -33315,7 +33314,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="421" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="421" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A421" t="s">
         <v>68</v>
       </c>
@@ -33388,7 +33387,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="422" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="422" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A422" t="s">
         <v>68</v>
       </c>
@@ -33461,7 +33460,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="423" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="423" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A423" t="s">
         <v>68</v>
       </c>
@@ -33534,7 +33533,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="424" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="424" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A424" t="s">
         <v>68</v>
       </c>
@@ -33607,7 +33606,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="425" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="425" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A425" t="s">
         <v>68</v>
       </c>
@@ -33680,7 +33679,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="426" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="426" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A426" t="s">
         <v>68</v>
       </c>
@@ -33753,7 +33752,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="427" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="427" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A427" t="s">
         <v>69</v>
       </c>
@@ -33826,7 +33825,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="428" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="428" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A428" t="s">
         <v>69</v>
       </c>
@@ -33899,7 +33898,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="429" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="429" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A429" t="s">
         <v>69</v>
       </c>
@@ -33972,7 +33971,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="430" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="430" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A430" t="s">
         <v>69</v>
       </c>
@@ -34045,7 +34044,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="431" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="431" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A431" t="s">
         <v>69</v>
       </c>
@@ -34118,7 +34117,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="432" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="432" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A432" t="s">
         <v>69</v>
       </c>
@@ -34191,7 +34190,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="433" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="433" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A433" t="s">
         <v>69</v>
       </c>
@@ -34264,7 +34263,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="434" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="434" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A434" t="s">
         <v>69</v>
       </c>
@@ -34337,7 +34336,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="435" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="435" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A435" t="s">
         <v>69</v>
       </c>
@@ -34410,7 +34409,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="436" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="436" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A436" t="s">
         <v>69</v>
       </c>
@@ -34483,7 +34482,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="437" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="437" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A437" t="s">
         <v>70</v>
       </c>
@@ -34555,7 +34554,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="438" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="438" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A438" t="s">
         <v>70</v>
       </c>
@@ -34629,7 +34628,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="439" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="439" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A439" t="s">
         <v>70</v>
       </c>
@@ -34703,7 +34702,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="440" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="440" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A440" t="s">
         <v>70</v>
       </c>
@@ -34776,7 +34775,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="441" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="441" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A441" t="s">
         <v>70</v>
       </c>
@@ -34850,7 +34849,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="442" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="442" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A442" t="s">
         <v>70</v>
       </c>
@@ -34924,7 +34923,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="443" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="443" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A443" t="s">
         <v>70</v>
       </c>
@@ -34998,7 +34997,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="444" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="444" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A444" t="s">
         <v>70</v>
       </c>
@@ -35072,7 +35071,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="445" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="445" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A445" t="s">
         <v>70</v>
       </c>
@@ -35146,7 +35145,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="446" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="446" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A446" t="s">
         <v>70</v>
       </c>
@@ -35220,7 +35219,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="447" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="447" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A447" t="s">
         <v>71</v>
       </c>
@@ -35293,7 +35292,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="448" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="448" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A448" t="s">
         <v>71</v>
       </c>
@@ -35367,7 +35366,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="449" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="449" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A449" t="s">
         <v>71</v>
       </c>
@@ -35441,7 +35440,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="450" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="450" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A450" t="s">
         <v>71</v>
       </c>
@@ -35515,7 +35514,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="451" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="451" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A451" t="s">
         <v>71</v>
       </c>
@@ -35589,7 +35588,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="452" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="452" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A452" t="s">
         <v>71</v>
       </c>
@@ -35663,7 +35662,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="453" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="453" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A453" t="s">
         <v>71</v>
       </c>
@@ -35737,7 +35736,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="454" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="454" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A454" t="s">
         <v>71</v>
       </c>
@@ -35810,7 +35809,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="455" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="455" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A455" t="s">
         <v>71</v>
       </c>
@@ -35884,7 +35883,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="456" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="456" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A456" t="s">
         <v>71</v>
       </c>
@@ -36697,18 +36696,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:Y466" xr:uid="{00000000-0009-0000-0000-000000000000}">
-    <filterColumn colId="0">
-      <filters>
-        <filter val="190531_2_10mg-kg AMPH_3.csv"/>
-      </filters>
-    </filterColumn>
-    <filterColumn colId="1">
-      <filters>
-        <filter val="1905312"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:Y466" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>